<commit_message>
Att Ata e Tabelas no BD
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-disel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF278E77-5E67-4DEB-9021-219862F31DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4438F15-3837-42E2-977D-8BB3444E33D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="2535" yWindow="2850" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="237">
   <si>
     <t>Requisito</t>
   </si>
@@ -877,6 +877,30 @@
   <si>
     <t>Realizado</t>
   </si>
+  <si>
+    <t>* Finalizamos o gráfico burndown com a produtividade da equipe,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> juntamente colocamos na tabela de backlog o tamanho dos requisitos e suas prioridades.</t>
+  </si>
+  <si>
+    <t>SPRINT 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vitor /Guilherme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Alteramos também o grafico de burndown com melhorias e avançamos principalmente no </t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulador financeiro. </t>
+  </si>
+  <si>
+    <t>passamos para a equipe sobre a reunião com o Marcos para validação da documentação.</t>
+  </si>
+  <si>
+    <t>*Discutimos tópicos sobre as entregas na semana, avançamos em alguns pontos de melhoria e</t>
+  </si>
 </sst>
 </file>
 
@@ -885,7 +909,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -980,6 +1004,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1219,7 +1249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1457,12 +1487,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1498,21 +1522,58 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1534,22 +1595,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1639,7 +1700,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1652,7 +1713,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
+              <a:rPr lang="pt-BR" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
               <a:t>GRÁFICO BURNDOWN - PRODUTIVIDADE</a:t>
             </a:r>
           </a:p>
@@ -1671,7 +1739,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1694,37 +1762,43 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0047300936588633E-2"/>
-          <c:y val="0.11601050046363083"/>
-          <c:w val="0.9199609836697219"/>
-          <c:h val="0.7976649038372704"/>
+          <c:x val="4.387853365929964E-2"/>
+          <c:y val="9.9791610147005771E-2"/>
+          <c:w val="0.94316908780579456"/>
+          <c:h val="0.74216838734873847"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BackLog!$N$2:$O$2</c:f>
+              <c:f>BackLog!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Realizado</c:v>
+                  <c:v>Planejado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1747,8 +1821,8 @@
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1772,13 +1846,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1786,22 +1861,48 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>BackLog!$K$3:$K$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL:</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SPRINT 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SPRINT 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SPRINT 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SPRINT 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BackLog!$O$3:$O$6</c:f>
+              <c:f>BackLog!$L$3:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>154</c:v>
+                  <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1810,48 +1911,41 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-4B3B-4DA4-964C-DD6167A36292}"/>
+              <c16:uniqueId val="{00000007-5838-4123-9429-C60DDC4229AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BackLog!$K$2</c:f>
+              <c:f>BackLog!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Planejado</c:v>
+                  <c:v>Realizado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -1871,8 +1965,8 @@
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1896,13 +1990,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1912,9 +2007,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>BackLog!$K$3:$K$6</c:f>
+              <c:f>BackLog!$K$3:$K$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>TOTAL:</c:v>
                 </c:pt>
@@ -1927,26 +2022,32 @@
                 <c:pt idx="3">
                   <c:v>SPRINT 3</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>SPRINT 4</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BackLog!$L$3:$L$6</c:f>
+              <c:f>BackLog!$O$3:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>346</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>139</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1954,104 +2055,38 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4B3B-4DA4-964C-DD6167A36292}"/>
+              <c16:uniqueId val="{0000000C-5838-4123-9429-C60DDC4229AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="587220063"/>
-        <c:axId val="309969455"/>
+        <c:axId val="1085862847"/>
+        <c:axId val="1079574015"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="587220063"/>
+        <c:axId val="1085862847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="309969455"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="309969455"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -2080,7 +2115,66 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="587220063"/>
+        <c:crossAx val="1079574015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1079574015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1085862847"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2093,7 +2187,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2125,18 +2219,11 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2208,7 +2295,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2219,7 +2306,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2232,7 +2319,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -2242,18 +2329,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -2273,11 +2360,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -2309,45 +2396,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2359,17 +2436,14 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2378,15 +2452,15 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2408,13 +2482,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2429,15 +2505,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2448,16 +2524,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2466,10 +2543,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -2485,7 +2562,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -2493,7 +2570,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2512,16 +2589,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2530,16 +2608,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2548,16 +2627,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2573,20 +2653,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2600,7 +2680,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -2617,10 +2697,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -2641,7 +2721,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2650,14 +2730,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2671,7 +2750,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -2687,8 +2766,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2704,17 +2783,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2722,7 +2790,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -2732,23 +2800,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>169208</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>582194</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>201705</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>11205</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>268940</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>79458</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E10DC1E-1512-D692-6FE4-A40009A02E0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{388BB993-1FC6-FCB2-8C03-168137EB7E46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3088,21 +3156,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" style="108" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" style="107" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="107" customWidth="1"/>
-    <col min="4" max="4" width="14" style="100" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="100" customWidth="1"/>
+    <col min="1" max="1" width="63.85546875" style="106" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.28515625" style="105" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="105" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="100" customWidth="1"/>
+    <col min="5" max="5" width="17" style="100" customWidth="1"/>
     <col min="6" max="6" width="18" style="100" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="107" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="100" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="105" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="100" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" style="100" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="100"/>
     <col min="11" max="11" width="15.42578125" style="100" customWidth="1"/>
@@ -3114,1087 +3182,1120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="127" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="101" t="s">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+    </row>
+    <row r="2" spans="1:17" s="124" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="126" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="101" t="s">
+      <c r="E2" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="101" t="s">
+      <c r="G2" s="126" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="101" t="s">
+      <c r="H2" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="101" t="s">
+      <c r="I2" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="117" t="s">
+      <c r="K2" s="128" t="s">
         <v>227</v>
       </c>
-      <c r="L2" s="117"/>
-      <c r="N2" s="117" t="s">
+      <c r="L2" s="128"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="128" t="s">
         <v>228</v>
       </c>
-      <c r="O2" s="117"/>
+      <c r="O2" s="128"/>
     </row>
     <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="104" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="101" t="s">
         <v>147</v>
       </c>
       <c r="C3" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="105">
+      <c r="E3" s="102">
         <v>21</v>
       </c>
-      <c r="F3" s="105">
+      <c r="F3" s="102">
         <v>2</v>
       </c>
-      <c r="G3" s="104" t="s">
+      <c r="G3" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="105" t="s">
+      <c r="H3" s="102" t="s">
         <v>203</v>
       </c>
-      <c r="I3" s="105" t="s">
+      <c r="I3" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="110" t="s">
+      <c r="K3" s="108" t="s">
         <v>225</v>
       </c>
-      <c r="L3" s="109">
+      <c r="L3" s="107">
         <f>SUM(E3:E37)</f>
         <v>346</v>
       </c>
-      <c r="N3" s="110" t="s">
+      <c r="N3" s="108" t="s">
         <v>225</v>
       </c>
-      <c r="O3" s="109">
+      <c r="O3" s="107">
         <f>SUM(O4:O6)</f>
         <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="101" t="s">
         <v>149</v>
       </c>
       <c r="C4" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E4" s="105">
+      <c r="E4" s="102">
         <v>8</v>
       </c>
-      <c r="F4" s="105">
+      <c r="F4" s="102">
         <v>1</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H4" s="105" t="s">
+      <c r="H4" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="I4" s="105" t="s">
+      <c r="I4" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="K4" s="111" t="s">
+      <c r="K4" s="109" t="s">
         <v>180</v>
       </c>
-      <c r="L4" s="112">
+      <c r="L4" s="110">
         <f>SUMIF(G3:G37,K4,E3:E37)</f>
         <v>88</v>
       </c>
-      <c r="N4" s="111" t="s">
+      <c r="N4" s="109" t="s">
         <v>180</v>
       </c>
-      <c r="O4" s="112">
+      <c r="O4" s="110">
         <f>SUM(E15:E26)</f>
         <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="106" t="s">
+      <c r="A5" s="104" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="101" t="s">
         <v>151</v>
       </c>
       <c r="C5" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="105" t="s">
+      <c r="D5" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E5" s="105">
+      <c r="E5" s="102">
         <v>8</v>
       </c>
-      <c r="F5" s="105">
+      <c r="F5" s="102">
         <v>1</v>
       </c>
-      <c r="G5" s="104" t="s">
+      <c r="G5" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="105" t="s">
+      <c r="H5" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="105" t="s">
+      <c r="I5" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="K5" s="111" t="s">
+      <c r="K5" s="109" t="s">
         <v>145</v>
       </c>
-      <c r="L5" s="112">
+      <c r="L5" s="110">
         <f t="shared" ref="L5:L6" si="0">SUMIF(G4:G38,K5,E4:E38)</f>
         <v>98</v>
       </c>
-      <c r="N5" s="111" t="s">
+      <c r="N5" s="109" t="s">
         <v>145</v>
       </c>
-      <c r="O5" s="112">
+      <c r="O5" s="110">
         <f>SUM(E3,E6,E8,E12,E13)</f>
         <v>66</v>
       </c>
-      <c r="Q5" s="105"/>
+      <c r="Q5" s="103"/>
     </row>
     <row r="6" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="101" t="s">
         <v>153</v>
       </c>
       <c r="C6" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E6" s="105">
+      <c r="E6" s="102">
         <v>8</v>
       </c>
-      <c r="F6" s="105">
+      <c r="F6" s="102">
         <v>1</v>
       </c>
-      <c r="G6" s="104" t="s">
+      <c r="G6" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H6" s="105" t="s">
+      <c r="H6" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="105" t="s">
+      <c r="I6" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="K6" s="111" t="s">
+      <c r="K6" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="L6" s="112">
+      <c r="L6" s="110">
         <f t="shared" si="0"/>
         <v>139</v>
       </c>
-      <c r="N6" s="111" t="s">
+      <c r="N6" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="O6" s="112">
+      <c r="O6" s="110">
         <v>0</v>
       </c>
-      <c r="Q6" s="105"/>
+      <c r="Q6" s="103"/>
     </row>
     <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="104" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="101" t="s">
         <v>144</v>
       </c>
       <c r="C7" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E7" s="105">
+      <c r="E7" s="102">
         <v>8</v>
       </c>
-      <c r="F7" s="105">
+      <c r="F7" s="102">
         <v>1</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="105" t="s">
+      <c r="H7" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="105" t="s">
+      <c r="I7" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="K7" s="113" t="s">
+      <c r="K7" s="109" t="s">
+        <v>231</v>
+      </c>
+      <c r="L7" s="110">
+        <v>0</v>
+      </c>
+      <c r="N7" s="109" t="s">
+        <v>231</v>
+      </c>
+      <c r="O7" s="110">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="103"/>
+    </row>
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="104" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="101" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="104" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="102" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="102">
+        <v>8</v>
+      </c>
+      <c r="F8" s="102">
+        <v>1</v>
+      </c>
+      <c r="G8" s="102" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="102" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" s="102" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="111" t="s">
         <v>226</v>
       </c>
-      <c r="L7" s="114">
+      <c r="L8" s="112">
         <f>AVERAGE(L4:L6)</f>
         <v>108.33333333333333</v>
       </c>
-      <c r="N7" s="113" t="s">
+      <c r="N8" s="111" t="s">
         <v>226</v>
       </c>
-      <c r="O7" s="114">
+      <c r="O8" s="112">
         <f>AVERAGE(O4:O6)</f>
         <v>51.333333333333336</v>
       </c>
-      <c r="Q7" s="105"/>
-    </row>
-    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="106" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="103" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="104" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="105" t="s">
-        <v>222</v>
-      </c>
-      <c r="E8" s="105">
-        <v>8</v>
-      </c>
-      <c r="F8" s="105">
-        <v>1</v>
-      </c>
-      <c r="G8" s="104" t="s">
-        <v>145</v>
-      </c>
-      <c r="H8" s="105" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="105" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q8" s="105"/>
+      <c r="Q8" s="103"/>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="106" t="s">
+      <c r="A9" s="104" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="101" t="s">
         <v>157</v>
       </c>
       <c r="C9" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E9" s="105">
+      <c r="E9" s="102">
         <v>5</v>
       </c>
-      <c r="F9" s="105">
+      <c r="F9" s="102">
         <v>2</v>
       </c>
-      <c r="G9" s="104" t="s">
+      <c r="G9" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H9" s="105" t="s">
+      <c r="H9" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="105" t="s">
+      <c r="I9" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="Q9" s="105"/>
+      <c r="Q9" s="103"/>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="104" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="101" t="s">
         <v>159</v>
       </c>
       <c r="C10" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="105" t="s">
+      <c r="D10" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E10" s="105">
+      <c r="E10" s="102">
         <v>8</v>
       </c>
-      <c r="F10" s="105">
+      <c r="F10" s="102">
         <v>1</v>
       </c>
-      <c r="G10" s="104" t="s">
+      <c r="G10" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H10" s="105" t="s">
+      <c r="H10" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="I10" s="105" t="s">
+      <c r="I10" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="Q10" s="105"/>
+      <c r="Q10" s="103"/>
     </row>
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="104" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="101" t="s">
         <v>160</v>
       </c>
       <c r="C11" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E11" s="105">
+      <c r="E11" s="102">
         <v>8</v>
       </c>
-      <c r="F11" s="105">
+      <c r="F11" s="102">
         <v>1</v>
       </c>
-      <c r="G11" s="104" t="s">
+      <c r="G11" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H11" s="105" t="s">
+      <c r="H11" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="I11" s="105" t="s">
+      <c r="I11" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="Q11" s="105"/>
+      <c r="Q11" s="103"/>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="104" t="s">
         <v>161</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="101" t="s">
         <v>162</v>
       </c>
       <c r="C12" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="105">
+      <c r="E12" s="102">
         <v>21</v>
       </c>
-      <c r="F12" s="105">
+      <c r="F12" s="102">
         <v>1</v>
       </c>
-      <c r="G12" s="104" t="s">
+      <c r="G12" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H12" s="105" t="s">
+      <c r="H12" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="105" t="s">
+      <c r="I12" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="K12" s="115"/>
-      <c r="Q12" s="105"/>
+      <c r="K12" s="113"/>
+      <c r="Q12" s="103"/>
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="104" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="101" t="s">
         <v>164</v>
       </c>
       <c r="C13" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="105" t="s">
+      <c r="D13" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E13" s="105">
+      <c r="E13" s="102">
         <v>8</v>
       </c>
-      <c r="F13" s="105">
+      <c r="F13" s="102">
         <v>2</v>
       </c>
-      <c r="G13" s="104" t="s">
+      <c r="G13" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H13" s="105" t="s">
+      <c r="H13" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="105" t="s">
+      <c r="I13" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="Q13" s="105"/>
+      <c r="Q13" s="103"/>
     </row>
     <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="104" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="101" t="s">
         <v>166</v>
       </c>
       <c r="C14" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="105" t="s">
+      <c r="D14" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E14" s="105">
+      <c r="E14" s="102">
         <v>8</v>
       </c>
-      <c r="F14" s="105">
+      <c r="F14" s="102">
         <v>2</v>
       </c>
-      <c r="G14" s="104" t="s">
+      <c r="G14" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H14" s="105" t="s">
+      <c r="H14" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="I14" s="105" t="s">
+      <c r="I14" s="102" t="s">
         <v>220</v>
       </c>
-      <c r="Q14" s="105"/>
+      <c r="Q14" s="103"/>
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="106" t="s">
+      <c r="A15" s="104" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="102" t="s">
         <v>143</v>
       </c>
       <c r="C15" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="105" t="s">
+      <c r="D15" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E15" s="105">
+      <c r="E15" s="102">
         <v>3</v>
       </c>
-      <c r="F15" s="105">
+      <c r="F15" s="102">
         <v>1</v>
       </c>
-      <c r="G15" s="104" t="s">
+      <c r="G15" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H15" s="105" t="s">
+      <c r="H15" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="I15" s="105" t="s">
+      <c r="I15" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="Q15" s="105"/>
+      <c r="Q15" s="103"/>
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="102" t="s">
         <v>148</v>
       </c>
       <c r="C16" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="105" t="s">
+      <c r="D16" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E16" s="105">
+      <c r="E16" s="102">
         <v>3</v>
       </c>
-      <c r="F16" s="105">
+      <c r="F16" s="102">
         <v>1</v>
       </c>
-      <c r="G16" s="104" t="s">
+      <c r="G16" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H16" s="105" t="s">
+      <c r="H16" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="I16" s="105" t="s">
+      <c r="I16" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="Q16" s="105"/>
+      <c r="Q16" s="103"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="106" t="s">
+      <c r="A17" s="104" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="101" t="s">
         <v>168</v>
       </c>
       <c r="C17" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="105" t="s">
+      <c r="D17" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E17" s="105">
+      <c r="E17" s="102">
         <v>13</v>
       </c>
-      <c r="F17" s="105">
+      <c r="F17" s="102">
         <v>1</v>
       </c>
-      <c r="G17" s="104" t="s">
+      <c r="G17" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H17" s="105" t="s">
+      <c r="H17" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="105" t="s">
+      <c r="I17" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="106" t="s">
+      <c r="A18" s="104" t="s">
         <v>170</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="102" t="s">
         <v>171</v>
       </c>
       <c r="C18" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="105" t="s">
+      <c r="D18" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="105">
+      <c r="E18" s="102">
         <v>3</v>
       </c>
-      <c r="F18" s="105">
+      <c r="F18" s="102">
         <v>1</v>
       </c>
-      <c r="G18" s="104" t="s">
+      <c r="G18" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H18" s="105" t="s">
+      <c r="H18" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="I18" s="105" t="s">
+      <c r="I18" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="106" t="s">
+      <c r="A19" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="102" t="s">
         <v>172</v>
       </c>
       <c r="C19" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E19" s="105">
+      <c r="E19" s="102">
         <v>3</v>
       </c>
-      <c r="F19" s="105">
+      <c r="F19" s="102">
         <v>1</v>
       </c>
-      <c r="G19" s="104" t="s">
+      <c r="G19" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H19" s="105" t="s">
+      <c r="H19" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="I19" s="105" t="s">
+      <c r="I19" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="106" t="s">
+      <c r="A20" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="101" t="s">
         <v>173</v>
       </c>
       <c r="C20" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="105" t="s">
+      <c r="D20" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E20" s="105">
+      <c r="E20" s="102">
         <v>21</v>
       </c>
-      <c r="F20" s="105">
+      <c r="F20" s="102">
         <v>1</v>
       </c>
-      <c r="G20" s="104" t="s">
+      <c r="G20" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H20" s="105" t="s">
+      <c r="H20" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="I20" s="105" t="s">
+      <c r="I20" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="106" t="s">
+      <c r="A21" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="101" t="s">
         <v>174</v>
       </c>
       <c r="C21" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="105" t="s">
+      <c r="D21" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="105">
+      <c r="E21" s="102">
         <v>21</v>
       </c>
-      <c r="F21" s="105">
+      <c r="F21" s="102">
         <v>1</v>
       </c>
-      <c r="G21" s="104" t="s">
+      <c r="G21" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H21" s="105" t="s">
+      <c r="H21" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="I21" s="105" t="s">
+      <c r="I21" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="106" t="s">
+      <c r="A22" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="102" t="s">
         <v>175</v>
       </c>
       <c r="C22" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="105" t="s">
+      <c r="D22" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E22" s="105">
+      <c r="E22" s="102">
         <v>5</v>
       </c>
-      <c r="F22" s="105">
+      <c r="F22" s="102">
         <v>1</v>
       </c>
-      <c r="G22" s="104" t="s">
+      <c r="G22" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H22" s="105" t="s">
+      <c r="H22" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="I22" s="105" t="s">
+      <c r="I22" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="106" t="s">
+      <c r="A23" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="102" t="s">
         <v>176</v>
       </c>
       <c r="C23" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="105" t="s">
+      <c r="D23" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E23" s="105">
+      <c r="E23" s="102">
         <v>5</v>
       </c>
-      <c r="F23" s="105">
+      <c r="F23" s="102">
         <v>1</v>
       </c>
-      <c r="G23" s="104" t="s">
+      <c r="G23" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H23" s="105" t="s">
+      <c r="H23" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="I23" s="105" t="s">
+      <c r="I23" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="106" t="s">
+      <c r="A24" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="102" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="105" t="s">
+      <c r="D24" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E24" s="105">
+      <c r="E24" s="102">
         <v>5</v>
       </c>
-      <c r="F24" s="105">
+      <c r="F24" s="102">
         <v>1</v>
       </c>
-      <c r="G24" s="104" t="s">
+      <c r="G24" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H24" s="105" t="s">
+      <c r="H24" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="I24" s="105" t="s">
+      <c r="I24" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="106" t="s">
+      <c r="A25" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="104" t="s">
+      <c r="B25" s="102" t="s">
         <v>177</v>
       </c>
       <c r="C25" s="104" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="105" t="s">
+      <c r="D25" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E25" s="105">
+      <c r="E25" s="102">
         <v>3</v>
       </c>
-      <c r="F25" s="105">
+      <c r="F25" s="102">
         <v>3</v>
       </c>
-      <c r="G25" s="104" t="s">
+      <c r="G25" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H25" s="105" t="s">
+      <c r="H25" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="I25" s="105" t="s">
+      <c r="I25" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="106" t="s">
+      <c r="A26" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="104" t="s">
+      <c r="B26" s="102" t="s">
         <v>178</v>
       </c>
       <c r="C26" s="104" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="105" t="s">
+      <c r="D26" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E26" s="105">
+      <c r="E26" s="102">
         <v>3</v>
       </c>
-      <c r="F26" s="105">
+      <c r="F26" s="102">
         <v>3</v>
       </c>
-      <c r="G26" s="104" t="s">
+      <c r="G26" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="H26" s="105" t="s">
+      <c r="H26" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="I26" s="105" t="s">
+      <c r="I26" s="102" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="106" t="s">
+      <c r="A27" s="104" t="s">
         <v>181</v>
       </c>
-      <c r="B27" s="103" t="s">
+      <c r="B27" s="101" t="s">
         <v>184</v>
       </c>
       <c r="C27" s="104" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="105" t="s">
+      <c r="D27" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E27" s="105">
+      <c r="E27" s="102">
         <v>8</v>
       </c>
-      <c r="F27" s="105">
+      <c r="F27" s="102">
         <v>3</v>
       </c>
-      <c r="G27" s="107" t="s">
+      <c r="G27" s="105" t="s">
         <v>187</v>
       </c>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="106" t="s">
+      <c r="A28" s="104" t="s">
         <v>182</v>
       </c>
-      <c r="B28" s="104" t="s">
+      <c r="B28" s="102" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="107" t="s">
+      <c r="C28" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="105" t="s">
+      <c r="D28" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E28" s="105">
+      <c r="E28" s="102">
         <v>13</v>
       </c>
-      <c r="F28" s="105">
+      <c r="F28" s="102">
         <v>3</v>
       </c>
-      <c r="G28" s="107" t="s">
+      <c r="G28" s="105" t="s">
         <v>187</v>
       </c>
+      <c r="H28" s="105"/>
+      <c r="I28" s="105"/>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="104" t="s">
         <v>183</v>
       </c>
-      <c r="B29" s="103" t="s">
+      <c r="B29" s="101" t="s">
         <v>186</v>
       </c>
-      <c r="C29" s="107" t="s">
+      <c r="C29" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="105" t="s">
+      <c r="D29" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="E29" s="105">
+      <c r="E29" s="102">
         <v>5</v>
       </c>
-      <c r="F29" s="105">
+      <c r="F29" s="102">
         <v>3</v>
       </c>
-      <c r="G29" s="107" t="s">
+      <c r="G29" s="105" t="s">
         <v>187</v>
       </c>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="106" t="s">
+      <c r="A30" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="105" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="107" t="s">
+      <c r="C30" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="105" t="s">
+      <c r="D30" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E30" s="105">
+      <c r="E30" s="102">
         <v>8</v>
       </c>
-      <c r="F30" s="105">
+      <c r="F30" s="102">
         <v>3</v>
       </c>
-      <c r="G30" s="107" t="s">
+      <c r="G30" s="105" t="s">
         <v>187</v>
       </c>
+      <c r="H30" s="105"/>
+      <c r="I30" s="105"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="106" t="s">
+      <c r="A31" s="104" t="s">
         <v>206</v>
       </c>
-      <c r="B31" s="107" t="s">
+      <c r="B31" s="105" t="s">
         <v>213</v>
       </c>
-      <c r="C31" s="107" t="s">
+      <c r="C31" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="105" t="s">
+      <c r="D31" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E31" s="105">
+      <c r="E31" s="102">
         <v>8</v>
       </c>
-      <c r="F31" s="105">
+      <c r="F31" s="102">
         <v>3</v>
       </c>
-      <c r="G31" s="107" t="s">
+      <c r="G31" s="105" t="s">
         <v>187</v>
       </c>
+      <c r="H31" s="105"/>
+      <c r="I31" s="105"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="106" t="s">
+      <c r="A32" s="104" t="s">
         <v>207</v>
       </c>
-      <c r="B32" s="107" t="s">
+      <c r="B32" s="105" t="s">
         <v>214</v>
       </c>
-      <c r="C32" s="107" t="s">
+      <c r="C32" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="105" t="s">
+      <c r="D32" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E32" s="105">
+      <c r="E32" s="102">
         <v>13</v>
       </c>
-      <c r="F32" s="105">
+      <c r="F32" s="102">
         <v>3</v>
       </c>
-      <c r="G32" s="107" t="s">
+      <c r="G32" s="105" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="106" t="s">
+      <c r="H32" s="105"/>
+      <c r="I32" s="105"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="104" t="s">
         <v>208</v>
       </c>
-      <c r="B33" s="107" t="s">
+      <c r="B33" s="105" t="s">
         <v>215</v>
       </c>
-      <c r="C33" s="107" t="s">
+      <c r="C33" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="105" t="s">
+      <c r="D33" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="E33" s="105">
+      <c r="E33" s="102">
         <v>8</v>
       </c>
-      <c r="F33" s="105">
+      <c r="F33" s="102">
         <v>3</v>
       </c>
-      <c r="G33" s="107" t="s">
+      <c r="G33" s="105" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="106" t="s">
+      <c r="H33" s="105"/>
+      <c r="I33" s="105"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="104" t="s">
         <v>209</v>
       </c>
-      <c r="B34" s="107" t="s">
+      <c r="B34" s="105" t="s">
         <v>216</v>
       </c>
-      <c r="C34" s="107" t="s">
+      <c r="C34" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="105" t="s">
+      <c r="D34" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E34" s="105">
+      <c r="E34" s="102">
         <v>13</v>
       </c>
-      <c r="F34" s="105">
+      <c r="F34" s="102">
         <v>3</v>
       </c>
-      <c r="G34" s="107" t="s">
+      <c r="G34" s="105" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="106" t="s">
+      <c r="H34" s="105"/>
+      <c r="I34" s="105"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="104" t="s">
         <v>223</v>
       </c>
-      <c r="B35" s="107" t="s">
+      <c r="B35" s="105" t="s">
         <v>217</v>
       </c>
-      <c r="C35" s="107" t="s">
+      <c r="C35" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="105" t="s">
+      <c r="D35" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E35" s="105">
+      <c r="E35" s="102">
         <v>21</v>
       </c>
-      <c r="F35" s="105">
+      <c r="F35" s="102">
         <v>3</v>
       </c>
-      <c r="G35" s="107" t="s">
+      <c r="G35" s="105" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="106" t="s">
+      <c r="H35" s="105"/>
+      <c r="I35" s="105"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="104" t="s">
         <v>210</v>
       </c>
-      <c r="B36" s="107" t="s">
+      <c r="B36" s="105" t="s">
         <v>218</v>
       </c>
-      <c r="C36" s="107" t="s">
+      <c r="C36" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="105" t="s">
+      <c r="D36" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="E36" s="105">
+      <c r="E36" s="102">
         <v>21</v>
       </c>
-      <c r="F36" s="105">
+      <c r="F36" s="102">
         <v>3</v>
       </c>
-      <c r="G36" s="107" t="s">
+      <c r="G36" s="105" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="106" t="s">
+      <c r="H36" s="105"/>
+      <c r="I36" s="105"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="104" t="s">
         <v>211</v>
       </c>
-      <c r="B37" s="107" t="s">
+      <c r="B37" s="105" t="s">
         <v>224</v>
       </c>
-      <c r="C37" s="107" t="s">
+      <c r="C37" s="105" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="105" t="s">
+      <c r="D37" s="125" t="s">
         <v>221</v>
       </c>
-      <c r="E37" s="105">
+      <c r="E37" s="125">
         <v>21</v>
       </c>
-      <c r="F37" s="105">
+      <c r="F37" s="125">
         <v>3</v>
       </c>
-      <c r="G37" s="107" t="s">
+      <c r="G37" s="105" t="s">
         <v>187</v>
       </c>
+      <c r="H37" s="124"/>
+      <c r="I37" s="124"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:I37" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}"/>
@@ -4203,6 +4304,7 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="N2:O2"/>
   </mergeCells>
+  <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="D2:I2 C2:C1048576">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"ESSENCIAL"</formula>
@@ -4214,7 +4316,7 @@
       <formula>"DESEJÁVEL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C26" xr:uid="{C6A8AFFE-3DC7-45BF-9737-E7A938D030B3}">
       <formula1>"Desejável, Essencial, Importante"</formula1>
     </dataValidation>
@@ -4260,7 +4362,7 @@
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="129" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4283,7 +4385,7 @@
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="118"/>
+      <c r="G2" s="129"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4636,8 +4738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="B1:R69"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R60" sqref="R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4645,13 +4747,13 @@
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="3.5703125" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" customWidth="1"/>
     <col min="13" max="13" width="3.28515625" customWidth="1"/>
@@ -4664,88 +4766,88 @@
   <sheetData>
     <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="123"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="134"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="121" t="s">
+      <c r="H2" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="123"/>
-      <c r="N2" s="121" t="s">
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="134"/>
+      <c r="N2" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="122"/>
-      <c r="R2" s="123"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="133"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="124">
+      <c r="C3" s="135">
         <v>45554</v>
       </c>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="125"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="136"/>
       <c r="G3" s="7"/>
       <c r="H3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="124">
+      <c r="I3" s="135">
         <v>45555</v>
       </c>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="125"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="136"/>
       <c r="N3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="124">
+      <c r="O3" s="135">
         <v>45557</v>
       </c>
-      <c r="P3" s="124"/>
-      <c r="Q3" s="124"/>
-      <c r="R3" s="125"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="136"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="132" t="s">
+      <c r="C4" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="133"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="142"/>
       <c r="G4" s="8"/>
       <c r="H4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="132" t="s">
+      <c r="I4" s="141" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="132"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="133"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="141"/>
+      <c r="L4" s="142"/>
       <c r="N4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="132" t="s">
+      <c r="O4" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="132"/>
-      <c r="Q4" s="132"/>
-      <c r="R4" s="133"/>
+      <c r="P4" s="141"/>
+      <c r="Q4" s="141"/>
+      <c r="R4" s="142"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
@@ -4876,22 +4978,22 @@
       <c r="R10" s="24"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131" t="s">
+      <c r="C11" s="140"/>
+      <c r="D11" s="140" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="131"/>
+      <c r="E11" s="140"/>
       <c r="F11" s="26" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="130" t="s">
+      <c r="H11" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="131"/>
+      <c r="I11" s="140"/>
       <c r="J11" s="28" t="s">
         <v>88</v>
       </c>
@@ -4899,10 +5001,10 @@
       <c r="L11" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="N11" s="130" t="s">
+      <c r="N11" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="O11" s="131"/>
+      <c r="O11" s="140"/>
       <c r="P11" s="44" t="s">
         <v>88</v>
       </c>
@@ -4914,22 +5016,22 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120" t="s">
+      <c r="C12" s="130"/>
+      <c r="D12" s="130" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="120"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="18">
         <v>45560</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="130"/>
       <c r="L12" s="18"/>
       <c r="N12" s="51" t="s">
         <v>90</v>
@@ -4946,22 +5048,22 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="119" t="s">
+      <c r="B13" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120" t="s">
+      <c r="C13" s="130"/>
+      <c r="D13" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="120"/>
+      <c r="E13" s="130"/>
       <c r="F13" s="18">
         <v>45560</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="119"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
+      <c r="H13" s="131"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="130"/>
       <c r="L13" s="18"/>
       <c r="N13" s="47" t="s">
         <v>91</v>
@@ -4978,22 +5080,22 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120" t="s">
+      <c r="C14" s="130"/>
+      <c r="D14" s="130" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="120"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="18">
         <v>45560</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="120"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="130"/>
       <c r="L14" s="18"/>
       <c r="N14" s="47" t="s">
         <v>92</v>
@@ -5010,21 +5112,21 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="127" t="s">
+      <c r="B15" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="126"/>
-      <c r="D15" s="126" t="s">
+      <c r="C15" s="137"/>
+      <c r="D15" s="137" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="126"/>
+      <c r="E15" s="137"/>
       <c r="F15" s="21">
         <v>45560</v>
       </c>
-      <c r="H15" s="127"/>
-      <c r="I15" s="126"/>
-      <c r="J15" s="126"/>
-      <c r="K15" s="126"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="137"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="137"/>
       <c r="L15" s="21"/>
       <c r="N15" s="86" t="s">
         <v>95</v>
@@ -5053,85 +5155,85 @@
       <c r="R16" s="69"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="121" t="s">
+      <c r="B17" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
-      <c r="E17" s="122"/>
-      <c r="F17" s="123"/>
-      <c r="H17" s="121" t="s">
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="134"/>
+      <c r="H17" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="122"/>
-      <c r="J17" s="122"/>
-      <c r="K17" s="122"/>
-      <c r="L17" s="123"/>
-      <c r="N17" s="121" t="s">
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
+      <c r="K17" s="133"/>
+      <c r="L17" s="134"/>
+      <c r="N17" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="O17" s="122"/>
-      <c r="P17" s="122"/>
-      <c r="Q17" s="122"/>
-      <c r="R17" s="123"/>
+      <c r="O17" s="133"/>
+      <c r="P17" s="133"/>
+      <c r="Q17" s="133"/>
+      <c r="R17" s="134"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="124">
+      <c r="C18" s="135">
         <v>45558</v>
       </c>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="125"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="136"/>
       <c r="H18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="124">
+      <c r="I18" s="135">
         <v>45559</v>
       </c>
-      <c r="J18" s="124"/>
-      <c r="K18" s="124"/>
-      <c r="L18" s="125"/>
+      <c r="J18" s="135"/>
+      <c r="K18" s="135"/>
+      <c r="L18" s="136"/>
       <c r="N18" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="O18" s="124">
+      <c r="O18" s="135">
         <v>45560</v>
       </c>
-      <c r="P18" s="124"/>
-      <c r="Q18" s="124"/>
-      <c r="R18" s="125"/>
+      <c r="P18" s="135"/>
+      <c r="Q18" s="135"/>
+      <c r="R18" s="136"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="128" t="s">
+      <c r="C19" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="129"/>
+      <c r="D19" s="143"/>
+      <c r="E19" s="143"/>
+      <c r="F19" s="144"/>
       <c r="H19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="128" t="s">
+      <c r="I19" s="143" t="s">
         <v>122</v>
       </c>
-      <c r="J19" s="128"/>
-      <c r="K19" s="128"/>
-      <c r="L19" s="129"/>
+      <c r="J19" s="143"/>
+      <c r="K19" s="143"/>
+      <c r="L19" s="144"/>
       <c r="N19" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="128" t="s">
+      <c r="O19" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="P19" s="128"/>
-      <c r="Q19" s="128"/>
-      <c r="R19" s="129"/>
+      <c r="P19" s="143"/>
+      <c r="Q19" s="143"/>
+      <c r="R19" s="144"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
@@ -5281,10 +5383,10 @@
       <c r="R26" s="24"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="130" t="s">
+      <c r="B27" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="131"/>
+      <c r="C27" s="140"/>
       <c r="D27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5294,10 +5396,10 @@
       <c r="F27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="130" t="s">
+      <c r="H27" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I27" s="131"/>
+      <c r="I27" s="140"/>
       <c r="J27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5307,10 +5409,10 @@
       <c r="L27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N27" s="130" t="s">
+      <c r="N27" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="O27" s="131"/>
+      <c r="O27" s="140"/>
       <c r="P27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5511,27 +5613,27 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="122"/>
-      <c r="D35" s="122"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="123"/>
-      <c r="H35" s="121" t="s">
+      <c r="C35" s="133"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="134"/>
+      <c r="H35" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I35" s="122"/>
-      <c r="J35" s="122"/>
-      <c r="K35" s="122"/>
-      <c r="L35" s="123"/>
-      <c r="N35" s="121" t="s">
+      <c r="I35" s="133"/>
+      <c r="J35" s="133"/>
+      <c r="K35" s="133"/>
+      <c r="L35" s="134"/>
+      <c r="N35" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="122"/>
-      <c r="P35" s="122"/>
-      <c r="Q35" s="122"/>
-      <c r="R35" s="123"/>
+      <c r="O35" s="133"/>
+      <c r="P35" s="133"/>
+      <c r="Q35" s="133"/>
+      <c r="R35" s="134"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
@@ -5546,12 +5648,12 @@
       <c r="H36" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="124">
+      <c r="I36" s="135">
         <v>45562</v>
       </c>
-      <c r="J36" s="124"/>
-      <c r="K36" s="124"/>
-      <c r="L36" s="125"/>
+      <c r="J36" s="135"/>
+      <c r="K36" s="135"/>
+      <c r="L36" s="136"/>
       <c r="N36" s="77" t="s">
         <v>79</v>
       </c>
@@ -5575,12 +5677,12 @@
       <c r="H37" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I37" s="128" t="s">
+      <c r="I37" s="143" t="s">
         <v>192</v>
       </c>
-      <c r="J37" s="128"/>
-      <c r="K37" s="128"/>
-      <c r="L37" s="129"/>
+      <c r="J37" s="143"/>
+      <c r="K37" s="143"/>
+      <c r="L37" s="144"/>
       <c r="N37" s="80" t="s">
         <v>80</v>
       </c>
@@ -5735,10 +5837,10 @@
       <c r="R44" s="24"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="130" t="s">
+      <c r="B45" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="131"/>
+      <c r="C45" s="140"/>
       <c r="D45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5748,10 +5850,10 @@
       <c r="F45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H45" s="130" t="s">
+      <c r="H45" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I45" s="131"/>
+      <c r="I45" s="140"/>
       <c r="J45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5761,10 +5863,10 @@
       <c r="L45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N45" s="130" t="s">
+      <c r="N45" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="O45" s="131"/>
+      <c r="O45" s="140"/>
       <c r="P45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5810,7 +5912,7 @@
         <v>120</v>
       </c>
       <c r="Q46" s="97" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="R46" s="98">
         <v>45571</v>
@@ -5981,20 +6083,27 @@
       </c>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="121" t="s">
+      <c r="B53" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="122"/>
-      <c r="D53" s="122"/>
-      <c r="E53" s="122"/>
-      <c r="F53" s="123"/>
-      <c r="H53" s="121" t="s">
+      <c r="C53" s="133"/>
+      <c r="D53" s="133"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="134"/>
+      <c r="H53" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I53" s="122"/>
-      <c r="J53" s="122"/>
-      <c r="K53" s="122"/>
-      <c r="L53" s="123"/>
+      <c r="I53" s="133"/>
+      <c r="J53" s="133"/>
+      <c r="K53" s="133"/>
+      <c r="L53" s="134"/>
+      <c r="N53" s="132" t="s">
+        <v>78</v>
+      </c>
+      <c r="O53" s="133"/>
+      <c r="P53" s="133"/>
+      <c r="Q53" s="133"/>
+      <c r="R53" s="134"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
@@ -6015,6 +6124,15 @@
       <c r="J54" s="70"/>
       <c r="K54" s="70"/>
       <c r="L54" s="71"/>
+      <c r="N54" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="O54" s="11">
+        <v>45572</v>
+      </c>
+      <c r="P54" s="70"/>
+      <c r="Q54" s="70"/>
+      <c r="R54" s="71"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="s">
@@ -6035,6 +6153,15 @@
       <c r="J55" s="16"/>
       <c r="K55" s="16"/>
       <c r="L55" s="17"/>
+      <c r="N55" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="O55" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="17"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
@@ -6047,6 +6174,11 @@
       <c r="J56" s="20"/>
       <c r="K56" s="20"/>
       <c r="L56" s="72"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="20"/>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="72"/>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" s="22" t="s">
@@ -6063,6 +6195,13 @@
       <c r="J57" s="23"/>
       <c r="K57" s="23"/>
       <c r="L57" s="24"/>
+      <c r="N57" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="O57" s="23"/>
+      <c r="P57" s="23"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="24"/>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
@@ -6072,11 +6211,20 @@
       <c r="D58" s="29"/>
       <c r="E58" s="29"/>
       <c r="F58" s="30"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="30"/>
+      <c r="H58" s="118" t="s">
+        <v>229</v>
+      </c>
+      <c r="I58" s="119"/>
+      <c r="J58" s="119"/>
+      <c r="K58" s="119"/>
+      <c r="L58" s="120"/>
+      <c r="N58" s="118" t="s">
+        <v>236</v>
+      </c>
+      <c r="O58" s="119"/>
+      <c r="P58" s="119"/>
+      <c r="Q58" s="119"/>
+      <c r="R58" s="120"/>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
@@ -6086,11 +6234,20 @@
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
       <c r="F59" s="17"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="17"/>
+      <c r="H59" s="117" t="s">
+        <v>230</v>
+      </c>
+      <c r="I59" s="121"/>
+      <c r="J59" s="121"/>
+      <c r="K59" s="121"/>
+      <c r="L59" s="122"/>
+      <c r="N59" s="117" t="s">
+        <v>235</v>
+      </c>
+      <c r="O59" s="121"/>
+      <c r="P59" s="121"/>
+      <c r="Q59" s="121"/>
+      <c r="R59" s="122"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="15" t="s">
@@ -6100,11 +6257,18 @@
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
       <c r="F60" s="17"/>
-      <c r="H60" s="15"/>
+      <c r="H60" s="123"/>
       <c r="I60" s="16"/>
       <c r="J60" s="16"/>
       <c r="K60" s="16"/>
       <c r="L60" s="17"/>
+      <c r="N60" s="123" t="s">
+        <v>233</v>
+      </c>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+      <c r="Q60" s="16"/>
+      <c r="R60" s="17"/>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" s="12" t="s">
@@ -6119,6 +6283,13 @@
       <c r="J61" s="31"/>
       <c r="K61" s="31"/>
       <c r="L61" s="32"/>
+      <c r="N61" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="O61" s="31"/>
+      <c r="P61" s="31"/>
+      <c r="Q61" s="31"/>
+      <c r="R61" s="32"/>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B62" s="22" t="s">
@@ -6135,12 +6306,19 @@
       <c r="J62" s="23"/>
       <c r="K62" s="23"/>
       <c r="L62" s="24"/>
+      <c r="N62" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="O62" s="23"/>
+      <c r="P62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="24"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="130" t="s">
+      <c r="B63" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="131"/>
+      <c r="C63" s="140"/>
       <c r="D63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6150,10 +6328,10 @@
       <c r="F63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="130" t="s">
+      <c r="H63" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I63" s="131"/>
+      <c r="I63" s="140"/>
       <c r="J63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6161,6 +6339,19 @@
         <v>117</v>
       </c>
       <c r="L63" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="N63" s="139" t="s">
+        <v>87</v>
+      </c>
+      <c r="O63" s="140"/>
+      <c r="P63" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q63" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="R63" s="26" t="s">
         <v>89</v>
       </c>
     </row>
@@ -6191,8 +6382,21 @@
       <c r="L64" s="98">
         <v>45571</v>
       </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N64" s="95" t="s">
+        <v>126</v>
+      </c>
+      <c r="O64" s="96"/>
+      <c r="P64" s="96" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q64" s="97" t="s">
+        <v>134</v>
+      </c>
+      <c r="R64" s="98">
+        <v>45571</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="89" t="s">
         <v>127</v>
       </c>
@@ -6217,10 +6421,23 @@
         <v>118</v>
       </c>
       <c r="L65" s="50">
-        <v>45571</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45573</v>
+      </c>
+      <c r="N65" s="89" t="s">
+        <v>127</v>
+      </c>
+      <c r="O65" s="49"/>
+      <c r="P65" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q65" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="R65" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66" s="89" t="s">
         <v>128</v>
       </c>
@@ -6245,10 +6462,23 @@
         <v>118</v>
       </c>
       <c r="L66" s="50">
-        <v>45571</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45573</v>
+      </c>
+      <c r="N66" s="89" t="s">
+        <v>128</v>
+      </c>
+      <c r="O66" s="49"/>
+      <c r="P66" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q66" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="R66" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" s="89" t="s">
         <v>202</v>
       </c>
@@ -6273,10 +6503,23 @@
         <v>118</v>
       </c>
       <c r="L67" s="50">
-        <v>45571</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45573</v>
+      </c>
+      <c r="N67" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="O67" s="49"/>
+      <c r="P67" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q67" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="R67" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" s="89" t="s">
         <v>201</v>
       </c>
@@ -6301,16 +6544,29 @@
         <v>118</v>
       </c>
       <c r="L68" s="50">
-        <v>45571</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45573</v>
+      </c>
+      <c r="N68" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="O68" s="49"/>
+      <c r="P68" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q68" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="R68" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="99" t="s">
         <v>204</v>
       </c>
       <c r="C69" s="75"/>
       <c r="D69" s="75" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="E69" s="75" t="s">
         <v>133</v>
@@ -6318,22 +6574,37 @@
       <c r="F69" s="76">
         <v>45571</v>
       </c>
-      <c r="H69" s="99" t="s">
+      <c r="H69" s="114" t="s">
         <v>204</v>
       </c>
-      <c r="I69" s="75"/>
-      <c r="J69" s="75" t="s">
-        <v>203</v>
-      </c>
-      <c r="K69" s="75" t="s">
-        <v>133</v>
-      </c>
-      <c r="L69" s="76">
-        <v>45571</v>
+      <c r="I69" s="115"/>
+      <c r="J69" s="115" t="s">
+        <v>132</v>
+      </c>
+      <c r="K69" s="115" t="s">
+        <v>134</v>
+      </c>
+      <c r="L69" s="116">
+        <v>45572</v>
+      </c>
+      <c r="N69" s="114" t="s">
+        <v>204</v>
+      </c>
+      <c r="O69" s="115"/>
+      <c r="P69" s="115" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q69" s="115" t="s">
+        <v>134</v>
+      </c>
+      <c r="R69" s="116">
+        <v>45572</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="55">
+    <mergeCell ref="N53:R53"/>
+    <mergeCell ref="N63:O63"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="B63:C63"/>
@@ -6347,6 +6618,7 @@
     <mergeCell ref="H35:L35"/>
     <mergeCell ref="I36:L36"/>
     <mergeCell ref="I37:L37"/>
+    <mergeCell ref="O19:R19"/>
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="O3:R3"/>
     <mergeCell ref="O4:R4"/>
@@ -6355,7 +6627,6 @@
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="O19:R19"/>
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:F2"/>
@@ -6377,16 +6648,16 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C18:F18"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mudanças do simulador e gráfico de burndown
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-disel-2\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Gotardo\Desktop\Projeto\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4438F15-3837-42E2-977D-8BB3444E33D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE0D009-1228-4EB2-992D-571026666A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="2850" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -1568,50 +1568,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1894,13 +1894,13 @@
                   <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>139</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2035,16 +2035,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>154</c:v>
+                  <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3156,32 +3156,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" style="106" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" style="105" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="105" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="100" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" style="106" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" style="105" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="105" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="100" customWidth="1"/>
     <col min="5" max="5" width="17" style="100" customWidth="1"/>
     <col min="6" max="6" width="18" style="100" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="105" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="100" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="100" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="100"/>
-    <col min="11" max="11" width="15.42578125" style="100" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" style="105" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="100" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="100" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="100"/>
+    <col min="11" max="11" width="15.44140625" style="100" customWidth="1"/>
     <col min="12" max="12" width="13" style="100" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="100"/>
-    <col min="14" max="14" width="15.5703125" style="100" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="100" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="100"/>
+    <col min="13" max="13" width="9.109375" style="100"/>
+    <col min="14" max="14" width="15.5546875" style="100" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="100" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="100"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="127" t="s">
         <v>93</v>
       </c>
@@ -3194,7 +3194,7 @@
       <c r="H1" s="127"/>
       <c r="I1" s="127"/>
     </row>
-    <row r="2" spans="1:17" s="124" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="124" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="126" t="s">
         <v>0</v>
       </c>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="O2" s="128"/>
     </row>
-    <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="104" t="s">
         <v>146</v>
       </c>
@@ -3272,10 +3272,10 @@
       </c>
       <c r="O3" s="107">
         <f>SUM(O4:O6)</f>
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="104" t="s">
         <v>99</v>
       </c>
@@ -3307,18 +3307,16 @@
         <v>180</v>
       </c>
       <c r="L4" s="110">
-        <f>SUMIF(G3:G37,K4,E3:E37)</f>
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="N4" s="109" t="s">
         <v>180</v>
       </c>
       <c r="O4" s="110">
-        <f>SUM(E15:E26)</f>
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104" t="s">
         <v>150</v>
       </c>
@@ -3350,19 +3348,17 @@
         <v>145</v>
       </c>
       <c r="L5" s="110">
-        <f t="shared" ref="L5:L6" si="0">SUMIF(G4:G38,K5,E4:E38)</f>
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="N5" s="109" t="s">
         <v>145</v>
       </c>
       <c r="O5" s="110">
-        <f>SUM(E3,E6,E8,E12,E13)</f>
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="Q5" s="103"/>
     </row>
-    <row r="6" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="104" t="s">
         <v>100</v>
       </c>
@@ -3394,18 +3390,17 @@
         <v>187</v>
       </c>
       <c r="L6" s="110">
-        <f t="shared" si="0"/>
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="N6" s="109" t="s">
         <v>187</v>
       </c>
       <c r="O6" s="110">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="Q6" s="103"/>
     </row>
-    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104" t="s">
         <v>152</v>
       </c>
@@ -3447,7 +3442,7 @@
       </c>
       <c r="Q7" s="103"/>
     </row>
-    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="104" t="s">
         <v>154</v>
       </c>
@@ -3480,18 +3475,18 @@
       </c>
       <c r="L8" s="112">
         <f>AVERAGE(L4:L6)</f>
-        <v>108.33333333333333</v>
+        <v>115</v>
       </c>
       <c r="N8" s="111" t="s">
         <v>226</v>
       </c>
       <c r="O8" s="112">
         <f>AVERAGE(O4:O6)</f>
-        <v>51.333333333333336</v>
+        <v>115.33333333333333</v>
       </c>
       <c r="Q8" s="103"/>
     </row>
-    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="104" t="s">
         <v>156</v>
       </c>
@@ -3521,7 +3516,7 @@
       </c>
       <c r="Q9" s="103"/>
     </row>
-    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="104" t="s">
         <v>158</v>
       </c>
@@ -3551,7 +3546,7 @@
       </c>
       <c r="Q10" s="103"/>
     </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="104" t="s">
         <v>169</v>
       </c>
@@ -3581,7 +3576,7 @@
       </c>
       <c r="Q11" s="103"/>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="104" t="s">
         <v>161</v>
       </c>
@@ -3612,7 +3607,7 @@
       <c r="K12" s="113"/>
       <c r="Q12" s="103"/>
     </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="104" t="s">
         <v>163</v>
       </c>
@@ -3642,7 +3637,7 @@
       </c>
       <c r="Q13" s="103"/>
     </row>
-    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="104" t="s">
         <v>165</v>
       </c>
@@ -3672,7 +3667,7 @@
       </c>
       <c r="Q14" s="103"/>
     </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="104" t="s">
         <v>142</v>
       </c>
@@ -3702,7 +3697,7 @@
       </c>
       <c r="Q15" s="103"/>
     </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="104" t="s">
         <v>5</v>
       </c>
@@ -3732,7 +3727,7 @@
       </c>
       <c r="Q16" s="103"/>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
         <v>167</v>
       </c>
@@ -3761,7 +3756,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="104" t="s">
         <v>170</v>
       </c>
@@ -3790,7 +3785,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="104" t="s">
         <v>10</v>
       </c>
@@ -3819,7 +3814,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="104" t="s">
         <v>11</v>
       </c>
@@ -3848,7 +3843,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="104" t="s">
         <v>3</v>
       </c>
@@ -3877,7 +3872,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="104" t="s">
         <v>7</v>
       </c>
@@ -3906,7 +3901,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="104" t="s">
         <v>12</v>
       </c>
@@ -3935,7 +3930,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="104" t="s">
         <v>6</v>
       </c>
@@ -3964,7 +3959,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="104" t="s">
         <v>8</v>
       </c>
@@ -3993,7 +3988,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="104" t="s">
         <v>9</v>
       </c>
@@ -4022,7 +4017,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="104" t="s">
         <v>181</v>
       </c>
@@ -4047,7 +4042,7 @@
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="104" t="s">
         <v>182</v>
       </c>
@@ -4072,7 +4067,7 @@
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="104" t="s">
         <v>183</v>
       </c>
@@ -4097,7 +4092,7 @@
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="104" t="s">
         <v>205</v>
       </c>
@@ -4122,7 +4117,7 @@
       <c r="H30" s="105"/>
       <c r="I30" s="105"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="104" t="s">
         <v>206</v>
       </c>
@@ -4147,7 +4142,7 @@
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="104" t="s">
         <v>207</v>
       </c>
@@ -4172,7 +4167,7 @@
       <c r="H32" s="105"/>
       <c r="I32" s="105"/>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="104" t="s">
         <v>208</v>
       </c>
@@ -4197,7 +4192,7 @@
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="104" t="s">
         <v>209</v>
       </c>
@@ -4222,7 +4217,7 @@
       <c r="H34" s="105"/>
       <c r="I34" s="105"/>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="104" t="s">
         <v>223</v>
       </c>
@@ -4247,7 +4242,7 @@
       <c r="H35" s="105"/>
       <c r="I35" s="105"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="104" t="s">
         <v>210</v>
       </c>
@@ -4272,7 +4267,7 @@
       <c r="H36" s="105"/>
       <c r="I36" s="105"/>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="104" t="s">
         <v>211</v>
       </c>
@@ -4323,9 +4318,6 @@
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="O4" formulaRange="1"/>
-  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4338,12 +4330,12 @@
       <selection activeCell="A7" sqref="A7:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4366,7 +4358,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -4387,7 +4379,7 @@
       </c>
       <c r="G2" s="129"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -4410,7 +4402,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -4433,7 +4425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -4456,7 +4448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -4479,7 +4471,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -4500,7 +4492,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -4521,7 +4513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
@@ -4542,7 +4534,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -4563,7 +4555,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
@@ -4584,7 +4576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>56</v>
       </c>
@@ -4605,7 +4597,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>59</v>
       </c>
@@ -4626,7 +4618,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -4647,7 +4639,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -4668,7 +4660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -4689,7 +4681,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>74</v>
       </c>
@@ -4738,118 +4730,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="B1:R69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="F53" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R60" sqref="R60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="132" t="s">
+    <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="132"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="132" t="s">
+      <c r="H2" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="134"/>
-      <c r="N2" s="132" t="s">
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="132"/>
+      <c r="N2" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="133"/>
-      <c r="P2" s="133"/>
-      <c r="Q2" s="133"/>
-      <c r="R2" s="134"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="132"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="135">
+      <c r="C3" s="136">
         <v>45554</v>
       </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="137"/>
       <c r="G3" s="7"/>
       <c r="H3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="135">
+      <c r="I3" s="136">
         <v>45555</v>
       </c>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
+      <c r="L3" s="137"/>
       <c r="N3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="135">
+      <c r="O3" s="136">
         <v>45557</v>
       </c>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="136"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P3" s="136"/>
+      <c r="Q3" s="136"/>
+      <c r="R3" s="137"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="142"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="141"/>
       <c r="G4" s="8"/>
       <c r="H4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="141" t="s">
+      <c r="I4" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="142"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="141"/>
       <c r="N4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="141" t="s">
+      <c r="O4" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="142"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P4" s="140"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="141"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>81</v>
       </c>
@@ -4872,7 +4864,7 @@
       <c r="Q5" s="23"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>84</v>
       </c>
@@ -4895,7 +4887,7 @@
       <c r="Q6" s="29"/>
       <c r="R6" s="30"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>83</v>
       </c>
@@ -4916,7 +4908,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="17"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>85</v>
       </c>
@@ -4935,7 +4927,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="17"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>86</v>
       </c>
@@ -4954,7 +4946,7 @@
       <c r="Q9" s="31"/>
       <c r="R9" s="32"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
         <v>189</v>
       </c>
@@ -4977,23 +4969,23 @@
       <c r="Q10" s="23"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="139" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140" t="s">
+      <c r="C11" s="134"/>
+      <c r="D11" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="140"/>
+      <c r="E11" s="134"/>
       <c r="F11" s="26" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="139" t="s">
+      <c r="H11" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="140"/>
+      <c r="I11" s="134"/>
       <c r="J11" s="28" t="s">
         <v>88</v>
       </c>
@@ -5001,10 +4993,10 @@
       <c r="L11" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="N11" s="139" t="s">
+      <c r="N11" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="O11" s="140"/>
+      <c r="O11" s="134"/>
       <c r="P11" s="44" t="s">
         <v>88</v>
       </c>
@@ -5015,23 +5007,23 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="131" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="130"/>
-      <c r="D12" s="130" t="s">
+      <c r="C12" s="143"/>
+      <c r="D12" s="143" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="130"/>
+      <c r="E12" s="143"/>
       <c r="F12" s="18">
         <v>45560</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="131"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="130"/>
-      <c r="K12" s="130"/>
+      <c r="H12" s="142"/>
+      <c r="I12" s="143"/>
+      <c r="J12" s="143"/>
+      <c r="K12" s="143"/>
       <c r="L12" s="18"/>
       <c r="N12" s="51" t="s">
         <v>90</v>
@@ -5047,23 +5039,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="131" t="s">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="130"/>
-      <c r="D13" s="130" t="s">
+      <c r="C13" s="143"/>
+      <c r="D13" s="143" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="130"/>
+      <c r="E13" s="143"/>
       <c r="F13" s="18">
         <v>45560</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="131"/>
-      <c r="I13" s="130"/>
-      <c r="J13" s="130"/>
-      <c r="K13" s="130"/>
+      <c r="H13" s="142"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="143"/>
+      <c r="K13" s="143"/>
       <c r="L13" s="18"/>
       <c r="N13" s="47" t="s">
         <v>91</v>
@@ -5079,23 +5071,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="131" t="s">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="142" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="130"/>
-      <c r="D14" s="130" t="s">
+      <c r="C14" s="143"/>
+      <c r="D14" s="143" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="130"/>
+      <c r="E14" s="143"/>
       <c r="F14" s="18">
         <v>45560</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="131"/>
-      <c r="I14" s="130"/>
-      <c r="J14" s="130"/>
-      <c r="K14" s="130"/>
+      <c r="H14" s="142"/>
+      <c r="I14" s="143"/>
+      <c r="J14" s="143"/>
+      <c r="K14" s="143"/>
       <c r="L14" s="18"/>
       <c r="N14" s="47" t="s">
         <v>92</v>
@@ -5111,22 +5103,22 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="138" t="s">
+    <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="144" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="137"/>
-      <c r="D15" s="137" t="s">
+      <c r="C15" s="135"/>
+      <c r="D15" s="135" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="137"/>
+      <c r="E15" s="135"/>
       <c r="F15" s="21">
         <v>45560</v>
       </c>
-      <c r="H15" s="138"/>
-      <c r="I15" s="137"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="137"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="135"/>
+      <c r="J15" s="135"/>
+      <c r="K15" s="135"/>
       <c r="L15" s="21"/>
       <c r="N15" s="86" t="s">
         <v>95</v>
@@ -5142,7 +5134,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -5154,88 +5146,88 @@
       <c r="Q16" s="68"/>
       <c r="R16" s="69"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="132" t="s">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="133"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="134"/>
-      <c r="H17" s="132" t="s">
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
+      <c r="H17" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="133"/>
-      <c r="J17" s="133"/>
-      <c r="K17" s="133"/>
-      <c r="L17" s="134"/>
-      <c r="N17" s="132" t="s">
+      <c r="I17" s="131"/>
+      <c r="J17" s="131"/>
+      <c r="K17" s="131"/>
+      <c r="L17" s="132"/>
+      <c r="N17" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="O17" s="133"/>
-      <c r="P17" s="133"/>
-      <c r="Q17" s="133"/>
-      <c r="R17" s="134"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O17" s="131"/>
+      <c r="P17" s="131"/>
+      <c r="Q17" s="131"/>
+      <c r="R17" s="132"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="135">
+      <c r="C18" s="136">
         <v>45558</v>
       </c>
-      <c r="D18" s="135"/>
-      <c r="E18" s="135"/>
-      <c r="F18" s="136"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="137"/>
       <c r="H18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="135">
+      <c r="I18" s="136">
         <v>45559</v>
       </c>
-      <c r="J18" s="135"/>
-      <c r="K18" s="135"/>
-      <c r="L18" s="136"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="136"/>
+      <c r="L18" s="137"/>
       <c r="N18" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="O18" s="135">
+      <c r="O18" s="136">
         <v>45560</v>
       </c>
-      <c r="P18" s="135"/>
-      <c r="Q18" s="135"/>
-      <c r="R18" s="136"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P18" s="136"/>
+      <c r="Q18" s="136"/>
+      <c r="R18" s="137"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="143" t="s">
+      <c r="C19" s="138" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="143"/>
-      <c r="E19" s="143"/>
-      <c r="F19" s="144"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="138"/>
+      <c r="F19" s="139"/>
       <c r="H19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="143" t="s">
+      <c r="I19" s="138" t="s">
         <v>122</v>
       </c>
-      <c r="J19" s="143"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="144"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="139"/>
       <c r="N19" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="143" t="s">
+      <c r="O19" s="138" t="s">
         <v>82</v>
       </c>
-      <c r="P19" s="143"/>
-      <c r="Q19" s="143"/>
-      <c r="R19" s="144"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P19" s="138"/>
+      <c r="Q19" s="138"/>
+      <c r="R19" s="139"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -5252,7 +5244,7 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="14"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="22" t="s">
         <v>81</v>
       </c>
@@ -5275,7 +5267,7 @@
       <c r="Q21" s="23"/>
       <c r="R21" s="24"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="35" t="s">
         <v>111</v>
       </c>
@@ -5298,7 +5290,7 @@
       <c r="Q22" s="36"/>
       <c r="R22" s="37"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="38" t="s">
         <v>110</v>
       </c>
@@ -5321,7 +5313,7 @@
       <c r="Q23" s="39"/>
       <c r="R23" s="40"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="38" t="s">
         <v>112</v>
       </c>
@@ -5342,7 +5334,7 @@
       <c r="Q24" s="39"/>
       <c r="R24" s="40"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
@@ -5359,7 +5351,7 @@
       <c r="Q25" s="42"/>
       <c r="R25" s="43"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
         <v>189</v>
       </c>
@@ -5382,11 +5374,11 @@
       <c r="Q26" s="23"/>
       <c r="R26" s="24"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="139" t="s">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="140"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5396,10 +5388,10 @@
       <c r="F27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="139" t="s">
+      <c r="H27" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="I27" s="140"/>
+      <c r="I27" s="134"/>
       <c r="J27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5409,10 +5401,10 @@
       <c r="L27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N27" s="139" t="s">
+      <c r="N27" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="O27" s="140"/>
+      <c r="O27" s="134"/>
       <c r="P27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5423,7 +5415,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="90" t="s">
         <v>113</v>
       </c>
@@ -5464,7 +5456,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="47" t="s">
         <v>91</v>
       </c>
@@ -5505,7 +5497,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="51" t="s">
         <v>115</v>
       </c>
@@ -5546,7 +5538,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="51" t="s">
         <v>119</v>
       </c>
@@ -5587,7 +5579,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="55"/>
       <c r="C32" s="56"/>
       <c r="D32" s="56"/>
@@ -5612,30 +5604,30 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="132" t="s">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B35" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="133"/>
-      <c r="D35" s="133"/>
-      <c r="E35" s="133"/>
-      <c r="F35" s="134"/>
-      <c r="H35" s="132" t="s">
+      <c r="C35" s="131"/>
+      <c r="D35" s="131"/>
+      <c r="E35" s="131"/>
+      <c r="F35" s="132"/>
+      <c r="H35" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="I35" s="133"/>
-      <c r="J35" s="133"/>
-      <c r="K35" s="133"/>
-      <c r="L35" s="134"/>
-      <c r="N35" s="132" t="s">
+      <c r="I35" s="131"/>
+      <c r="J35" s="131"/>
+      <c r="K35" s="131"/>
+      <c r="L35" s="132"/>
+      <c r="N35" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="133"/>
-      <c r="P35" s="133"/>
-      <c r="Q35" s="133"/>
-      <c r="R35" s="134"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O35" s="131"/>
+      <c r="P35" s="131"/>
+      <c r="Q35" s="131"/>
+      <c r="R35" s="132"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>79</v>
       </c>
@@ -5648,12 +5640,12 @@
       <c r="H36" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="135">
+      <c r="I36" s="136">
         <v>45562</v>
       </c>
-      <c r="J36" s="135"/>
-      <c r="K36" s="135"/>
-      <c r="L36" s="136"/>
+      <c r="J36" s="136"/>
+      <c r="K36" s="136"/>
+      <c r="L36" s="137"/>
       <c r="N36" s="77" t="s">
         <v>79</v>
       </c>
@@ -5664,7 +5656,7 @@
       <c r="Q36" s="78"/>
       <c r="R36" s="79"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="s">
         <v>80</v>
       </c>
@@ -5677,12 +5669,12 @@
       <c r="H37" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I37" s="143" t="s">
+      <c r="I37" s="138" t="s">
         <v>192</v>
       </c>
-      <c r="J37" s="143"/>
-      <c r="K37" s="143"/>
-      <c r="L37" s="144"/>
+      <c r="J37" s="138"/>
+      <c r="K37" s="138"/>
+      <c r="L37" s="139"/>
       <c r="N37" s="80" t="s">
         <v>80</v>
       </c>
@@ -5693,7 +5685,7 @@
       <c r="Q37" s="33"/>
       <c r="R37" s="34"/>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
@@ -5710,7 +5702,7 @@
       <c r="Q38" s="31"/>
       <c r="R38" s="32"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B39" s="22" t="s">
         <v>81</v>
       </c>
@@ -5733,7 +5725,7 @@
       <c r="Q39" s="23"/>
       <c r="R39" s="24"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>190</v>
       </c>
@@ -5756,7 +5748,7 @@
       <c r="Q40" s="29"/>
       <c r="R40" s="30"/>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="s">
         <v>191</v>
       </c>
@@ -5779,7 +5771,7 @@
       <c r="Q41" s="16"/>
       <c r="R41" s="17"/>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B42" s="15"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -5796,7 +5788,7 @@
       <c r="Q42" s="16"/>
       <c r="R42" s="17"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
       <c r="C43" s="31"/>
       <c r="D43" s="31"/>
@@ -5813,7 +5805,7 @@
       <c r="Q43" s="31"/>
       <c r="R43" s="32"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B44" s="22" t="s">
         <v>189</v>
       </c>
@@ -5836,11 +5828,11 @@
       <c r="Q44" s="23"/>
       <c r="R44" s="24"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="139" t="s">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B45" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="140"/>
+      <c r="C45" s="134"/>
       <c r="D45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5850,10 +5842,10 @@
       <c r="F45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H45" s="139" t="s">
+      <c r="H45" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="I45" s="140"/>
+      <c r="I45" s="134"/>
       <c r="J45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5863,10 +5855,10 @@
       <c r="L45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N45" s="139" t="s">
+      <c r="N45" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="O45" s="140"/>
+      <c r="O45" s="134"/>
       <c r="P45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5877,7 +5869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B46" s="81" t="s">
         <v>126</v>
       </c>
@@ -5918,7 +5910,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B47" s="89" t="s">
         <v>127</v>
       </c>
@@ -5959,7 +5951,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B48" s="82" t="s">
         <v>128</v>
       </c>
@@ -6000,7 +5992,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B49" s="82" t="s">
         <v>129</v>
       </c>
@@ -6041,7 +6033,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B50" s="92" t="s">
         <v>196</v>
       </c>
@@ -6082,30 +6074,30 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="132" t="s">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B53" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="133"/>
-      <c r="D53" s="133"/>
-      <c r="E53" s="133"/>
-      <c r="F53" s="134"/>
-      <c r="H53" s="132" t="s">
+      <c r="C53" s="131"/>
+      <c r="D53" s="131"/>
+      <c r="E53" s="131"/>
+      <c r="F53" s="132"/>
+      <c r="H53" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="I53" s="133"/>
-      <c r="J53" s="133"/>
-      <c r="K53" s="133"/>
-      <c r="L53" s="134"/>
-      <c r="N53" s="132" t="s">
+      <c r="I53" s="131"/>
+      <c r="J53" s="131"/>
+      <c r="K53" s="131"/>
+      <c r="L53" s="132"/>
+      <c r="N53" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="O53" s="133"/>
-      <c r="P53" s="133"/>
-      <c r="Q53" s="133"/>
-      <c r="R53" s="134"/>
-    </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O53" s="131"/>
+      <c r="P53" s="131"/>
+      <c r="Q53" s="131"/>
+      <c r="R53" s="132"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
         <v>79</v>
       </c>
@@ -6134,7 +6126,7 @@
       <c r="Q54" s="70"/>
       <c r="R54" s="71"/>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B55" s="15" t="s">
         <v>80</v>
       </c>
@@ -6163,7 +6155,7 @@
       <c r="Q55" s="16"/>
       <c r="R55" s="17"/>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B56" s="12"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -6180,7 +6172,7 @@
       <c r="Q56" s="20"/>
       <c r="R56" s="72"/>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B57" s="22" t="s">
         <v>81</v>
       </c>
@@ -6203,7 +6195,7 @@
       <c r="Q57" s="23"/>
       <c r="R57" s="24"/>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>199</v>
       </c>
@@ -6226,7 +6218,7 @@
       <c r="Q58" s="119"/>
       <c r="R58" s="120"/>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B59" s="15" t="s">
         <v>197</v>
       </c>
@@ -6249,7 +6241,7 @@
       <c r="Q59" s="121"/>
       <c r="R59" s="122"/>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B60" s="15" t="s">
         <v>198</v>
       </c>
@@ -6270,7 +6262,7 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="17"/>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B61" s="12" t="s">
         <v>200</v>
       </c>
@@ -6291,7 +6283,7 @@
       <c r="Q61" s="31"/>
       <c r="R61" s="32"/>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B62" s="22" t="s">
         <v>189</v>
       </c>
@@ -6314,11 +6306,11 @@
       <c r="Q62" s="23"/>
       <c r="R62" s="24"/>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="139" t="s">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B63" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="140"/>
+      <c r="C63" s="134"/>
       <c r="D63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6328,10 +6320,10 @@
       <c r="F63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="139" t="s">
+      <c r="H63" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="I63" s="140"/>
+      <c r="I63" s="134"/>
       <c r="J63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6341,10 +6333,10 @@
       <c r="L63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N63" s="139" t="s">
+      <c r="N63" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="O63" s="140"/>
+      <c r="O63" s="134"/>
       <c r="P63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6355,7 +6347,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B64" s="95" t="s">
         <v>126</v>
       </c>
@@ -6396,7 +6388,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B65" s="89" t="s">
         <v>127</v>
       </c>
@@ -6437,7 +6429,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B66" s="89" t="s">
         <v>128</v>
       </c>
@@ -6478,7 +6470,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B67" s="89" t="s">
         <v>202</v>
       </c>
@@ -6519,7 +6511,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B68" s="89" t="s">
         <v>201</v>
       </c>
@@ -6560,7 +6552,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B69" s="99" t="s">
         <v>204</v>
       </c>
@@ -6603,6 +6595,45 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="N53:R53"/>
     <mergeCell ref="N63:O63"/>
     <mergeCell ref="J15:K15"/>
@@ -6619,45 +6650,6 @@
     <mergeCell ref="I36:L36"/>
     <mergeCell ref="I37:L37"/>
     <mergeCell ref="O19:R19"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizações nos gráficos do simulador
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Gotardo\Desktop\Projeto\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE0D009-1228-4EB2-992D-571026666A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDAEDC3-AF9A-4CAD-8EA5-B0226FE845F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
@@ -1249,7 +1249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1568,6 +1568,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1577,6 +1583,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1584,12 +1602,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1598,20 +1613,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1803,64 +1806,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>BackLog!$K$3:$K$7</c:f>
@@ -3158,13 +3103,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.88671875" style="106" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.33203125" style="105" customWidth="1"/>
+    <col min="2" max="2" width="73.5546875" style="105" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.109375" style="105" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" style="100" customWidth="1"/>
     <col min="5" max="5" width="17" style="100" customWidth="1"/>
@@ -3201,7 +3146,7 @@
       <c r="B2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="126" t="s">
+      <c r="C2" s="145" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="126" t="s">
@@ -3232,14 +3177,14 @@
       </c>
       <c r="O2" s="128"/>
     </row>
-    <row r="3" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="104" t="s">
         <v>146</v>
       </c>
       <c r="B3" s="101" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="102" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="102" t="s">
@@ -3275,14 +3220,14 @@
         <v>346</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="104" t="s">
         <v>99</v>
       </c>
       <c r="B4" s="101" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="102" t="s">
@@ -3316,14 +3261,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104" t="s">
         <v>150</v>
       </c>
       <c r="B5" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="104" t="s">
+      <c r="C5" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="102" t="s">
@@ -3358,14 +3303,14 @@
       </c>
       <c r="Q5" s="103"/>
     </row>
-    <row r="6" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="104" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="101" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="102" t="s">
@@ -3400,14 +3345,14 @@
       </c>
       <c r="Q6" s="103"/>
     </row>
-    <row r="7" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104" t="s">
         <v>152</v>
       </c>
       <c r="B7" s="101" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="102" t="s">
@@ -3442,14 +3387,14 @@
       </c>
       <c r="Q7" s="103"/>
     </row>
-    <row r="8" spans="1:17" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="104" t="s">
         <v>154</v>
       </c>
       <c r="B8" s="101" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="102" t="s">
@@ -3486,14 +3431,14 @@
       </c>
       <c r="Q8" s="103"/>
     </row>
-    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="104" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="104" t="s">
+      <c r="C9" s="102" t="s">
         <v>104</v>
       </c>
       <c r="D9" s="102" t="s">
@@ -3516,14 +3461,14 @@
       </c>
       <c r="Q9" s="103"/>
     </row>
-    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="104" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="101" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D10" s="102" t="s">
@@ -3546,14 +3491,14 @@
       </c>
       <c r="Q10" s="103"/>
     </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104" t="s">
         <v>169</v>
       </c>
       <c r="B11" s="101" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D11" s="102" t="s">
@@ -3576,14 +3521,14 @@
       </c>
       <c r="Q11" s="103"/>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104" t="s">
         <v>161</v>
       </c>
       <c r="B12" s="101" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="104" t="s">
+      <c r="C12" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="102" t="s">
@@ -3607,14 +3552,14 @@
       <c r="K12" s="113"/>
       <c r="Q12" s="103"/>
     </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="104" t="s">
         <v>163</v>
       </c>
       <c r="B13" s="101" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="102" t="s">
         <v>104</v>
       </c>
       <c r="D13" s="102" t="s">
@@ -3637,14 +3582,14 @@
       </c>
       <c r="Q13" s="103"/>
     </row>
-    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="104" t="s">
         <v>165</v>
       </c>
       <c r="B14" s="101" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="102" t="s">
         <v>104</v>
       </c>
       <c r="D14" s="102" t="s">
@@ -3667,14 +3612,14 @@
       </c>
       <c r="Q14" s="103"/>
     </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="104" t="s">
         <v>142</v>
       </c>
       <c r="B15" s="102" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="102" t="s">
@@ -3697,14 +3642,14 @@
       </c>
       <c r="Q15" s="103"/>
     </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="102" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D16" s="102" t="s">
@@ -3727,14 +3672,14 @@
       </c>
       <c r="Q16" s="103"/>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
         <v>167</v>
       </c>
       <c r="B17" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D17" s="102" t="s">
@@ -3756,14 +3701,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="104" t="s">
         <v>170</v>
       </c>
       <c r="B18" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D18" s="102" t="s">
@@ -3785,14 +3730,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="104" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="C19" s="104" t="s">
+      <c r="C19" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D19" s="102" t="s">
@@ -3814,14 +3759,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="104" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="101" t="s">
         <v>173</v>
       </c>
-      <c r="C20" s="104" t="s">
+      <c r="C20" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D20" s="102" t="s">
@@ -3843,14 +3788,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="104" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="101" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="104" t="s">
+      <c r="C21" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D21" s="102" t="s">
@@ -3872,14 +3817,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="104" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="102" t="s">
         <v>175</v>
       </c>
-      <c r="C22" s="104" t="s">
+      <c r="C22" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D22" s="102" t="s">
@@ -3901,14 +3846,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="104" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D23" s="102" t="s">
@@ -3930,14 +3875,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="104" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="104" t="s">
+      <c r="C24" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D24" s="102" t="s">
@@ -3959,14 +3904,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="104" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="102" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="104" t="s">
+      <c r="C25" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D25" s="102" t="s">
@@ -3988,14 +3933,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="104" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="102" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="104" t="s">
+      <c r="C26" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D26" s="102" t="s">
@@ -4017,14 +3962,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="104" t="s">
         <v>181</v>
       </c>
       <c r="B27" s="101" t="s">
         <v>184</v>
       </c>
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D27" s="102" t="s">
@@ -4042,14 +3987,14 @@
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="104" t="s">
         <v>182</v>
       </c>
       <c r="B28" s="102" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D28" s="102" t="s">
@@ -4067,14 +4012,14 @@
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="104" t="s">
         <v>183</v>
       </c>
       <c r="B29" s="101" t="s">
         <v>186</v>
       </c>
-      <c r="C29" s="106" t="s">
+      <c r="C29" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D29" s="102" t="s">
@@ -4092,14 +4037,14 @@
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="104" t="s">
         <v>205</v>
       </c>
       <c r="B30" s="105" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="106" t="s">
+      <c r="C30" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D30" s="102" t="s">
@@ -4117,14 +4062,14 @@
       <c r="H30" s="105"/>
       <c r="I30" s="105"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="104" t="s">
         <v>206</v>
       </c>
       <c r="B31" s="105" t="s">
         <v>213</v>
       </c>
-      <c r="C31" s="106" t="s">
+      <c r="C31" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D31" s="102" t="s">
@@ -4142,14 +4087,14 @@
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="104" t="s">
         <v>207</v>
       </c>
       <c r="B32" s="105" t="s">
         <v>214</v>
       </c>
-      <c r="C32" s="106" t="s">
+      <c r="C32" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D32" s="102" t="s">
@@ -4167,14 +4112,14 @@
       <c r="H32" s="105"/>
       <c r="I32" s="105"/>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="104" t="s">
         <v>208</v>
       </c>
       <c r="B33" s="105" t="s">
         <v>215</v>
       </c>
-      <c r="C33" s="106" t="s">
+      <c r="C33" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D33" s="102" t="s">
@@ -4192,14 +4137,14 @@
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="104" t="s">
         <v>209</v>
       </c>
       <c r="B34" s="105" t="s">
         <v>216</v>
       </c>
-      <c r="C34" s="106" t="s">
+      <c r="C34" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D34" s="102" t="s">
@@ -4217,14 +4162,14 @@
       <c r="H34" s="105"/>
       <c r="I34" s="105"/>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="104" t="s">
         <v>223</v>
       </c>
       <c r="B35" s="105" t="s">
         <v>217</v>
       </c>
-      <c r="C35" s="106" t="s">
+      <c r="C35" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D35" s="102" t="s">
@@ -4242,14 +4187,14 @@
       <c r="H35" s="105"/>
       <c r="I35" s="105"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="104" t="s">
         <v>210</v>
       </c>
       <c r="B36" s="105" t="s">
         <v>218</v>
       </c>
-      <c r="C36" s="106" t="s">
+      <c r="C36" s="105" t="s">
         <v>102</v>
       </c>
       <c r="D36" s="102" t="s">
@@ -4267,7 +4212,7 @@
       <c r="H36" s="105"/>
       <c r="I36" s="105"/>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="104" t="s">
         <v>211</v>
       </c>
@@ -4758,88 +4703,88 @@
   <sheetData>
     <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="132"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="134"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="130" t="s">
+      <c r="H2" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="132"/>
-      <c r="N2" s="130" t="s">
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="134"/>
+      <c r="N2" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="131"/>
-      <c r="P2" s="131"/>
-      <c r="Q2" s="131"/>
-      <c r="R2" s="132"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="133"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="136">
+      <c r="C3" s="135">
         <v>45554</v>
       </c>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="137"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="136"/>
       <c r="G3" s="7"/>
       <c r="H3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="136">
+      <c r="I3" s="135">
         <v>45555</v>
       </c>
-      <c r="J3" s="136"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="137"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="136"/>
       <c r="N3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="136">
+      <c r="O3" s="135">
         <v>45557</v>
       </c>
-      <c r="P3" s="136"/>
-      <c r="Q3" s="136"/>
-      <c r="R3" s="137"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="136"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="140"/>
-      <c r="E4" s="140"/>
-      <c r="F4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="142"/>
       <c r="G4" s="8"/>
       <c r="H4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="140" t="s">
+      <c r="I4" s="141" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="141"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="141"/>
+      <c r="L4" s="142"/>
       <c r="N4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="140" t="s">
+      <c r="O4" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="140"/>
-      <c r="Q4" s="140"/>
-      <c r="R4" s="141"/>
+      <c r="P4" s="141"/>
+      <c r="Q4" s="141"/>
+      <c r="R4" s="142"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
@@ -4970,22 +4915,22 @@
       <c r="R10" s="24"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="133" t="s">
+      <c r="B11" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134" t="s">
+      <c r="C11" s="140"/>
+      <c r="D11" s="140" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="134"/>
+      <c r="E11" s="140"/>
       <c r="F11" s="26" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="133" t="s">
+      <c r="H11" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="134"/>
+      <c r="I11" s="140"/>
       <c r="J11" s="28" t="s">
         <v>88</v>
       </c>
@@ -4993,10 +4938,10 @@
       <c r="L11" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="N11" s="133" t="s">
+      <c r="N11" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="O11" s="134"/>
+      <c r="O11" s="140"/>
       <c r="P11" s="44" t="s">
         <v>88</v>
       </c>
@@ -5008,22 +4953,22 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="143"/>
-      <c r="D12" s="143" t="s">
+      <c r="C12" s="130"/>
+      <c r="D12" s="130" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="143"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="18">
         <v>45560</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="142"/>
-      <c r="I12" s="143"/>
-      <c r="J12" s="143"/>
-      <c r="K12" s="143"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="130"/>
       <c r="L12" s="18"/>
       <c r="N12" s="51" t="s">
         <v>90</v>
@@ -5040,22 +4985,22 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="142" t="s">
+      <c r="B13" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="143"/>
-      <c r="D13" s="143" t="s">
+      <c r="C13" s="130"/>
+      <c r="D13" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="143"/>
+      <c r="E13" s="130"/>
       <c r="F13" s="18">
         <v>45560</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="142"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
+      <c r="H13" s="131"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="130"/>
       <c r="L13" s="18"/>
       <c r="N13" s="47" t="s">
         <v>91</v>
@@ -5072,22 +5017,22 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="143"/>
-      <c r="D14" s="143" t="s">
+      <c r="C14" s="130"/>
+      <c r="D14" s="130" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="143"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="18">
         <v>45560</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="142"/>
-      <c r="I14" s="143"/>
-      <c r="J14" s="143"/>
-      <c r="K14" s="143"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="130"/>
       <c r="L14" s="18"/>
       <c r="N14" s="47" t="s">
         <v>92</v>
@@ -5104,21 +5049,21 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135" t="s">
+      <c r="C15" s="137"/>
+      <c r="D15" s="137" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="135"/>
+      <c r="E15" s="137"/>
       <c r="F15" s="21">
         <v>45560</v>
       </c>
-      <c r="H15" s="144"/>
-      <c r="I15" s="135"/>
-      <c r="J15" s="135"/>
-      <c r="K15" s="135"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="137"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="137"/>
       <c r="L15" s="21"/>
       <c r="N15" s="86" t="s">
         <v>95</v>
@@ -5147,85 +5092,85 @@
       <c r="R16" s="69"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="130" t="s">
+      <c r="B17" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
-      <c r="H17" s="130" t="s">
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="134"/>
+      <c r="H17" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="131"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="132"/>
-      <c r="N17" s="130" t="s">
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
+      <c r="K17" s="133"/>
+      <c r="L17" s="134"/>
+      <c r="N17" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="O17" s="131"/>
-      <c r="P17" s="131"/>
-      <c r="Q17" s="131"/>
-      <c r="R17" s="132"/>
+      <c r="O17" s="133"/>
+      <c r="P17" s="133"/>
+      <c r="Q17" s="133"/>
+      <c r="R17" s="134"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="136">
+      <c r="C18" s="135">
         <v>45558</v>
       </c>
-      <c r="D18" s="136"/>
-      <c r="E18" s="136"/>
-      <c r="F18" s="137"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="136"/>
       <c r="H18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="136">
+      <c r="I18" s="135">
         <v>45559</v>
       </c>
-      <c r="J18" s="136"/>
-      <c r="K18" s="136"/>
-      <c r="L18" s="137"/>
+      <c r="J18" s="135"/>
+      <c r="K18" s="135"/>
+      <c r="L18" s="136"/>
       <c r="N18" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="O18" s="136">
+      <c r="O18" s="135">
         <v>45560</v>
       </c>
-      <c r="P18" s="136"/>
-      <c r="Q18" s="136"/>
-      <c r="R18" s="137"/>
+      <c r="P18" s="135"/>
+      <c r="Q18" s="135"/>
+      <c r="R18" s="136"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="138" t="s">
+      <c r="C19" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="139"/>
+      <c r="D19" s="143"/>
+      <c r="E19" s="143"/>
+      <c r="F19" s="144"/>
       <c r="H19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="138" t="s">
+      <c r="I19" s="143" t="s">
         <v>122</v>
       </c>
-      <c r="J19" s="138"/>
-      <c r="K19" s="138"/>
-      <c r="L19" s="139"/>
+      <c r="J19" s="143"/>
+      <c r="K19" s="143"/>
+      <c r="L19" s="144"/>
       <c r="N19" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="138" t="s">
+      <c r="O19" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="P19" s="138"/>
-      <c r="Q19" s="138"/>
-      <c r="R19" s="139"/>
+      <c r="P19" s="143"/>
+      <c r="Q19" s="143"/>
+      <c r="R19" s="144"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
@@ -5375,10 +5320,10 @@
       <c r="R26" s="24"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="133" t="s">
+      <c r="B27" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="134"/>
+      <c r="C27" s="140"/>
       <c r="D27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5388,10 +5333,10 @@
       <c r="F27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="133" t="s">
+      <c r="H27" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I27" s="134"/>
+      <c r="I27" s="140"/>
       <c r="J27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5401,10 +5346,10 @@
       <c r="L27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N27" s="133" t="s">
+      <c r="N27" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="O27" s="134"/>
+      <c r="O27" s="140"/>
       <c r="P27" s="44" t="s">
         <v>88</v>
       </c>
@@ -5605,27 +5550,27 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="130" t="s">
+      <c r="B35" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="131"/>
-      <c r="D35" s="131"/>
-      <c r="E35" s="131"/>
-      <c r="F35" s="132"/>
-      <c r="H35" s="130" t="s">
+      <c r="C35" s="133"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="134"/>
+      <c r="H35" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I35" s="131"/>
-      <c r="J35" s="131"/>
-      <c r="K35" s="131"/>
-      <c r="L35" s="132"/>
-      <c r="N35" s="130" t="s">
+      <c r="I35" s="133"/>
+      <c r="J35" s="133"/>
+      <c r="K35" s="133"/>
+      <c r="L35" s="134"/>
+      <c r="N35" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="131"/>
-      <c r="P35" s="131"/>
-      <c r="Q35" s="131"/>
-      <c r="R35" s="132"/>
+      <c r="O35" s="133"/>
+      <c r="P35" s="133"/>
+      <c r="Q35" s="133"/>
+      <c r="R35" s="134"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
@@ -5640,12 +5585,12 @@
       <c r="H36" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="136">
+      <c r="I36" s="135">
         <v>45562</v>
       </c>
-      <c r="J36" s="136"/>
-      <c r="K36" s="136"/>
-      <c r="L36" s="137"/>
+      <c r="J36" s="135"/>
+      <c r="K36" s="135"/>
+      <c r="L36" s="136"/>
       <c r="N36" s="77" t="s">
         <v>79</v>
       </c>
@@ -5669,12 +5614,12 @@
       <c r="H37" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I37" s="138" t="s">
+      <c r="I37" s="143" t="s">
         <v>192</v>
       </c>
-      <c r="J37" s="138"/>
-      <c r="K37" s="138"/>
-      <c r="L37" s="139"/>
+      <c r="J37" s="143"/>
+      <c r="K37" s="143"/>
+      <c r="L37" s="144"/>
       <c r="N37" s="80" t="s">
         <v>80</v>
       </c>
@@ -5829,10 +5774,10 @@
       <c r="R44" s="24"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="133" t="s">
+      <c r="B45" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="134"/>
+      <c r="C45" s="140"/>
       <c r="D45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5842,10 +5787,10 @@
       <c r="F45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H45" s="133" t="s">
+      <c r="H45" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I45" s="134"/>
+      <c r="I45" s="140"/>
       <c r="J45" s="44" t="s">
         <v>88</v>
       </c>
@@ -5855,10 +5800,10 @@
       <c r="L45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N45" s="133" t="s">
+      <c r="N45" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="O45" s="134"/>
+      <c r="O45" s="140"/>
       <c r="P45" s="44" t="s">
         <v>88</v>
       </c>
@@ -6075,27 +6020,27 @@
       </c>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B53" s="130" t="s">
+      <c r="B53" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="131"/>
-      <c r="D53" s="131"/>
-      <c r="E53" s="131"/>
-      <c r="F53" s="132"/>
-      <c r="H53" s="130" t="s">
+      <c r="C53" s="133"/>
+      <c r="D53" s="133"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="134"/>
+      <c r="H53" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I53" s="131"/>
-      <c r="J53" s="131"/>
-      <c r="K53" s="131"/>
-      <c r="L53" s="132"/>
-      <c r="N53" s="130" t="s">
+      <c r="I53" s="133"/>
+      <c r="J53" s="133"/>
+      <c r="K53" s="133"/>
+      <c r="L53" s="134"/>
+      <c r="N53" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="O53" s="131"/>
-      <c r="P53" s="131"/>
-      <c r="Q53" s="131"/>
-      <c r="R53" s="132"/>
+      <c r="O53" s="133"/>
+      <c r="P53" s="133"/>
+      <c r="Q53" s="133"/>
+      <c r="R53" s="134"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
@@ -6307,10 +6252,10 @@
       <c r="R62" s="24"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="133" t="s">
+      <c r="B63" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="134"/>
+      <c r="C63" s="140"/>
       <c r="D63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6320,10 +6265,10 @@
       <c r="F63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="133" t="s">
+      <c r="H63" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="I63" s="134"/>
+      <c r="I63" s="140"/>
       <c r="J63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6333,10 +6278,10 @@
       <c r="L63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N63" s="133" t="s">
+      <c r="N63" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="O63" s="134"/>
+      <c r="O63" s="140"/>
       <c r="P63" s="44" t="s">
         <v>88</v>
       </c>
@@ -6595,21 +6540,30 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="N53:R53"/>
+    <mergeCell ref="N63:O63"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="H53:L53"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="N35:R35"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:F2"/>
@@ -6626,30 +6580,21 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="N53:R53"/>
-    <mergeCell ref="N63:O63"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="H53:L53"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="N35:R35"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="I37:L37"/>
-    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Att Ata, backlog, doc
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-disel-2\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8B8B80-9B6F-4044-91E0-DD96978B9EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF6CDC7-2E92-48BC-98EF-34A1CE0B8F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="250">
   <si>
     <t>Requisito</t>
   </si>
@@ -512,12 +512,6 @@
     <t>* Foco na documentação com a atualização no uso de somente um sensor</t>
   </si>
   <si>
-    <t>Não finalizado</t>
-  </si>
-  <si>
-    <t>Parcialmente Finalizado</t>
-  </si>
-  <si>
     <t>* Discussão a respeito do marketing do simulador financeiro</t>
   </si>
   <si>
@@ -542,9 +536,6 @@
     <t>Progresso</t>
   </si>
   <si>
-    <t>Parcialmente Feito</t>
-  </si>
-  <si>
     <t>Script do Arduíno</t>
   </si>
   <si>
@@ -557,9 +548,6 @@
     <t>Rafael Ausente</t>
   </si>
   <si>
-    <t>Finalizado</t>
-  </si>
-  <si>
     <t>* Finalização do código do arduíno, focando somente no sensor ultrassônico</t>
   </si>
   <si>
@@ -587,9 +575,6 @@
     <t>Vitor / Guilherme</t>
   </si>
   <si>
-    <t>Iniciar</t>
-  </si>
-  <si>
     <t>Feito</t>
   </si>
   <si>
@@ -797,9 +782,6 @@
     <t>Site (Área do Simulador)/Remodelagem</t>
   </si>
   <si>
-    <t>Todos</t>
-  </si>
-  <si>
     <t>Gráfico Burndown/Tabela de Risco</t>
   </si>
   <si>
@@ -848,9 +830,6 @@
     <t>Pequeno</t>
   </si>
   <si>
-    <t>A fazer</t>
-  </si>
-  <si>
     <t>Grande</t>
   </si>
   <si>
@@ -930,6 +909,36 @@
   </si>
   <si>
     <t>Vitor Suave</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>EM ANDAMENTO</t>
+  </si>
+  <si>
+    <t>PENDENTE</t>
+  </si>
+  <si>
+    <t>Rafael não estava presente (Ficou doente)</t>
+  </si>
+  <si>
+    <t>* Reunião com o Marcos OK! Foi passado para a equipe os detalhes a mudar no projeto e algumas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dicas para o fechamento dos entregavéis. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Finalizaremos até o final da semana as atividades propostas com as devidas mudanças. </t>
+  </si>
+  <si>
+    <t>Modificação na Documentação</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1058,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1095,6 +1104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1308,7 +1323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1615,6 +1630,27 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1663,33 +1699,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1808,8 +1819,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23882354564831096"/>
-          <c:y val="9.0027485126991172E-2"/>
+          <c:x val="0.29795955542368685"/>
+          <c:y val="9.0027507315284347E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1983,7 +1994,7 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>139</c:v>
@@ -3288,103 +3299,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+    <sheetView zoomScale="39" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.140625" style="106" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" style="105" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="105" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="100" customWidth="1"/>
+    <col min="1" max="1" width="75.6640625" style="106" customWidth="1"/>
+    <col min="2" max="2" width="79.5546875" style="105" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="105" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="100" customWidth="1"/>
     <col min="5" max="5" width="17" style="100" customWidth="1"/>
     <col min="6" max="6" width="18" style="100" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="105" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="100" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="100" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="100"/>
-    <col min="11" max="11" width="15.42578125" style="100" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" style="105" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="100" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="100" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="100"/>
+    <col min="11" max="11" width="15.44140625" style="100" customWidth="1"/>
     <col min="12" max="12" width="13" style="100" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="100"/>
-    <col min="14" max="14" width="15.5703125" style="100" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="100" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="100"/>
-    <col min="18" max="18" width="15.7109375" style="100" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="100"/>
+    <col min="13" max="13" width="9.109375" style="100"/>
+    <col min="14" max="14" width="15.5546875" style="100" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="100" customWidth="1"/>
+    <col min="16" max="17" width="9.109375" style="100"/>
+    <col min="18" max="18" width="15.6640625" style="100" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="100"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="148" t="s">
-        <v>240</v>
-      </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="150"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="145"/>
-      <c r="N1" s="145"/>
-      <c r="O1" s="145"/>
-      <c r="P1" s="145"/>
-      <c r="Q1" s="145"/>
-      <c r="R1" s="145"/>
-    </row>
-    <row r="2" spans="1:18" s="124" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="151" t="s">
+    <row r="1" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="129" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="131"/>
+    </row>
+    <row r="2" spans="1:18" s="124" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="151" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="151" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="151" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="151" t="s">
+      <c r="D2" s="126" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="126" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="126" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="126" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="126" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="126" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="102"/>
+    </row>
+    <row r="3" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="104" t="s">
         <v>140</v>
       </c>
-      <c r="H2" s="151" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="151" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="146"/>
-      <c r="O2" s="146"/>
-      <c r="P2" s="146"/>
-      <c r="Q2" s="146"/>
-      <c r="R2" s="146"/>
-    </row>
-    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="104" t="s">
-        <v>145</v>
-      </c>
       <c r="B3" s="101" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C3" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E3" s="102">
         <v>21</v>
@@ -3393,39 +3389,39 @@
         <v>2</v>
       </c>
       <c r="G3" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H3" s="102" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
       <c r="I3" s="102" t="s">
-        <v>133</v>
-      </c>
-      <c r="K3" s="144" t="s">
-        <v>226</v>
-      </c>
-      <c r="L3" s="144"/>
-      <c r="N3" s="144" t="s">
-        <v>227</v>
-      </c>
-      <c r="O3" s="144"/>
-      <c r="Q3" s="144" t="s">
-        <v>241</v>
-      </c>
-      <c r="R3" s="144"/>
-    </row>
-    <row r="4" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="K3" s="132" t="s">
+        <v>219</v>
+      </c>
+      <c r="L3" s="132"/>
+      <c r="N3" s="132" t="s">
+        <v>220</v>
+      </c>
+      <c r="O3" s="132"/>
+      <c r="Q3" s="132" t="s">
+        <v>234</v>
+      </c>
+      <c r="R3" s="132"/>
+    </row>
+    <row r="4" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="104" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="101" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C4" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D4" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E4" s="102">
         <v>8</v>
@@ -3434,45 +3430,45 @@
         <v>1</v>
       </c>
       <c r="G4" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H4" s="102" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="I4" s="102" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="K4" s="108" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="L4" s="107">
         <f>SUM(E3:E37)</f>
         <v>346</v>
       </c>
       <c r="N4" s="108" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="O4" s="107">
         <f>SUM(O5:O7)</f>
         <v>154</v>
       </c>
-      <c r="Q4" s="142" t="s">
-        <v>242</v>
-      </c>
-      <c r="R4" s="143"/>
-    </row>
-    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q4" s="127" t="s">
+        <v>235</v>
+      </c>
+      <c r="R4" s="128"/>
+    </row>
+    <row r="5" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B5" s="101" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C5" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D5" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E5" s="102">
         <v>8</v>
@@ -3481,45 +3477,45 @@
         <v>1</v>
       </c>
       <c r="G5" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H5" s="102" t="s">
         <v>95</v>
       </c>
       <c r="I5" s="102" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="K5" s="109" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="L5" s="110">
-        <f>SUMIF(G3:G37,K5,E3:E37)</f>
+        <f>SUMIF($G$3:$G$37,K5,$E$3:$E$37)</f>
         <v>88</v>
       </c>
       <c r="N5" s="109" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="O5" s="110">
         <f>SUM(E15:E26)</f>
         <v>88</v>
       </c>
-      <c r="Q5" s="142" t="s">
-        <v>243</v>
-      </c>
-      <c r="R5" s="143"/>
-    </row>
-    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="127" t="s">
+        <v>236</v>
+      </c>
+      <c r="R5" s="128"/>
+    </row>
+    <row r="6" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="104" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="101" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C6" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D6" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E6" s="102">
         <v>8</v>
@@ -3528,45 +3524,45 @@
         <v>1</v>
       </c>
       <c r="G6" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H6" s="102" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="102" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="L6" s="110">
+        <f t="shared" ref="L6:L7" si="0">SUMIF($G$3:$G$37,K6,$E$3:$E$37)</f>
         <v>119</v>
       </c>
-      <c r="I6" s="102" t="s">
-        <v>133</v>
-      </c>
-      <c r="K6" s="109" t="s">
-        <v>144</v>
-      </c>
-      <c r="L6" s="110">
-        <f>SUMIF(G4:G38,K6,E4:E38)</f>
-        <v>98</v>
-      </c>
       <c r="N6" s="109" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="O6" s="110">
         <f>SUM(E3,E6,E8,E12,E13)</f>
         <v>66</v>
       </c>
-      <c r="Q6" s="142" t="s">
-        <v>244</v>
-      </c>
-      <c r="R6" s="143"/>
-    </row>
-    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="127" t="s">
+        <v>237</v>
+      </c>
+      <c r="R6" s="128"/>
+    </row>
+    <row r="7" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B7" s="101" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C7" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D7" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E7" s="102">
         <v>8</v>
@@ -3575,44 +3571,44 @@
         <v>1</v>
       </c>
       <c r="G7" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H7" s="102" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I7" s="102" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="K7" s="109" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="L7" s="110">
-        <f>SUMIF(G5:G39,K7,E5:E39)</f>
+        <f t="shared" si="0"/>
         <v>139</v>
       </c>
       <c r="N7" s="109" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="O7" s="110">
         <v>0</v>
       </c>
-      <c r="Q7" s="142" t="s">
-        <v>245</v>
-      </c>
-      <c r="R7" s="143"/>
-    </row>
-    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="127" t="s">
+        <v>238</v>
+      </c>
+      <c r="R7" s="128"/>
+    </row>
+    <row r="8" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="104" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B8" s="101" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C8" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D8" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E8" s="102">
         <v>8</v>
@@ -3621,43 +3617,43 @@
         <v>1</v>
       </c>
       <c r="G8" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H8" s="102" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I8" s="102" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="K8" s="109" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="L8" s="110">
         <v>0</v>
       </c>
       <c r="N8" s="109" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="O8" s="110">
         <v>0</v>
       </c>
-      <c r="Q8" s="142" t="s">
-        <v>246</v>
-      </c>
-      <c r="R8" s="143"/>
-    </row>
-    <row r="9" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="127" t="s">
+        <v>239</v>
+      </c>
+      <c r="R8" s="128"/>
+    </row>
+    <row r="9" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="104" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B9" s="101" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C9" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E9" s="102">
         <v>5</v>
@@ -3666,23 +3662,23 @@
         <v>2</v>
       </c>
       <c r="G9" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H9" s="102" t="s">
         <v>96</v>
       </c>
       <c r="I9" s="102" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="K9" s="111" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="L9" s="112">
         <f>AVERAGE(L5:L7)</f>
-        <v>108.33333333333333</v>
+        <v>115.33333333333333</v>
       </c>
       <c r="N9" s="111" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="O9" s="112">
         <f>AVERAGE(O5:O7)</f>
@@ -3690,18 +3686,18 @@
       </c>
       <c r="Q9" s="103"/>
     </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="104" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B10" s="101" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C10" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D10" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E10" s="102">
         <v>8</v>
@@ -3710,28 +3706,28 @@
         <v>1</v>
       </c>
       <c r="G10" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H10" s="102" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I10" s="102" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="Q10" s="103"/>
     </row>
-    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="104" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B11" s="101" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C11" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D11" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E11" s="102">
         <v>8</v>
@@ -3740,28 +3736,28 @@
         <v>1</v>
       </c>
       <c r="G11" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H11" s="102" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I11" s="102" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="Q11" s="103"/>
     </row>
-    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="104" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B12" s="101" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C12" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D12" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E12" s="102">
         <v>21</v>
@@ -3770,29 +3766,29 @@
         <v>1</v>
       </c>
       <c r="G12" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H12" s="102" t="s">
         <v>96</v>
       </c>
       <c r="I12" s="102" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="K12" s="113"/>
       <c r="Q12" s="103"/>
     </row>
-    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="104" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B13" s="101" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C13" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D13" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E13" s="102">
         <v>8</v>
@@ -3801,28 +3797,28 @@
         <v>2</v>
       </c>
       <c r="G13" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H13" s="102" t="s">
         <v>96</v>
       </c>
       <c r="I13" s="102" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="Q13" s="103"/>
     </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="104" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B14" s="101" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C14" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D14" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E14" s="102">
         <v>8</v>
@@ -3831,28 +3827,28 @@
         <v>2</v>
       </c>
       <c r="G14" s="102" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H14" s="102" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I14" s="102" t="s">
-        <v>219</v>
+        <v>48</v>
       </c>
       <c r="Q14" s="103"/>
     </row>
-    <row r="15" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="104" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B15" s="102" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C15" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D15" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E15" s="102">
         <v>3</v>
@@ -3861,28 +3857,28 @@
         <v>1</v>
       </c>
       <c r="G15" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H15" s="102" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I15" s="102" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="Q15" s="103"/>
     </row>
-    <row r="16" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="102" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C16" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D16" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E16" s="102">
         <v>3</v>
@@ -3891,28 +3887,28 @@
         <v>1</v>
       </c>
       <c r="G16" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H16" s="102" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I16" s="102" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="Q16" s="103"/>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B17" s="101" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C17" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E17" s="102">
         <v>13</v>
@@ -3921,27 +3917,27 @@
         <v>1</v>
       </c>
       <c r="G17" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H17" s="102" t="s">
         <v>96</v>
       </c>
       <c r="I17" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="104" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B18" s="102" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C18" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D18" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E18" s="102">
         <v>3</v>
@@ -3950,27 +3946,27 @@
         <v>1</v>
       </c>
       <c r="G18" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H18" s="102" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I18" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="104" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="102" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C19" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D19" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E19" s="102">
         <v>3</v>
@@ -3979,27 +3975,27 @@
         <v>1</v>
       </c>
       <c r="G19" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H19" s="102" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I19" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="104" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="101" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C20" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D20" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E20" s="102">
         <v>21</v>
@@ -4008,27 +4004,27 @@
         <v>1</v>
       </c>
       <c r="G20" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H20" s="102" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I20" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="104" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="101" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C21" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D21" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E21" s="102">
         <v>21</v>
@@ -4037,27 +4033,27 @@
         <v>1</v>
       </c>
       <c r="G21" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H21" s="102" t="s">
         <v>95</v>
       </c>
       <c r="I21" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="104" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="102" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C22" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D22" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E22" s="102">
         <v>5</v>
@@ -4066,27 +4062,27 @@
         <v>1</v>
       </c>
       <c r="G22" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H22" s="102" t="s">
         <v>96</v>
       </c>
       <c r="I22" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="104" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="102" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C23" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D23" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E23" s="102">
         <v>5</v>
@@ -4095,27 +4091,27 @@
         <v>1</v>
       </c>
       <c r="G23" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H23" s="102" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I23" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="104" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="102" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C24" s="102" t="s">
         <v>102</v>
       </c>
       <c r="D24" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E24" s="102">
         <v>5</v>
@@ -4124,27 +4120,27 @@
         <v>1</v>
       </c>
       <c r="G24" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H24" s="102" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I24" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="104" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="102" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C25" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D25" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E25" s="102">
         <v>3</v>
@@ -4153,27 +4149,27 @@
         <v>3</v>
       </c>
       <c r="G25" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H25" s="102" t="s">
         <v>95</v>
       </c>
       <c r="I25" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="104" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="102" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C26" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D26" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E26" s="102">
         <v>3</v>
@@ -4182,27 +4178,27 @@
         <v>3</v>
       </c>
       <c r="G26" s="102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H26" s="102" t="s">
         <v>95</v>
       </c>
       <c r="I26" s="102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="104" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B27" s="101" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C27" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D27" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E27" s="102">
         <v>8</v>
@@ -4211,23 +4207,27 @@
         <v>3</v>
       </c>
       <c r="G27" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H27" s="102"/>
-      <c r="I27" s="102"/>
-    </row>
-    <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H27" s="102" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="104" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B28" s="102" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C28" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D28" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E28" s="102">
         <v>13</v>
@@ -4236,23 +4236,27 @@
         <v>3</v>
       </c>
       <c r="G28" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H28" s="105"/>
-      <c r="I28" s="105"/>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H28" s="102" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="104" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B29" s="101" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C29" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D29" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E29" s="102">
         <v>5</v>
@@ -4261,23 +4265,27 @@
         <v>3</v>
       </c>
       <c r="G29" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-    </row>
-    <row r="30" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H29" s="102" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="104" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B30" s="102" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C30" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D30" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E30" s="102">
         <v>8</v>
@@ -4286,23 +4294,27 @@
         <v>3</v>
       </c>
       <c r="G30" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H30" s="105"/>
-      <c r="I30" s="105"/>
-    </row>
-    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H30" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="104" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B31" s="102" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C31" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D31" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E31" s="102">
         <v>8</v>
@@ -4311,23 +4323,27 @@
         <v>3</v>
       </c>
       <c r="G31" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H31" s="105"/>
-      <c r="I31" s="105"/>
-    </row>
-    <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H31" s="102" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="104" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B32" s="102" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C32" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D32" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E32" s="102">
         <v>13</v>
@@ -4336,23 +4352,27 @@
         <v>3</v>
       </c>
       <c r="G32" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H32" s="105"/>
-      <c r="I32" s="105"/>
-    </row>
-    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H32" s="102" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="104" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B33" s="102" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C33" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D33" s="102" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E33" s="102">
         <v>8</v>
@@ -4361,23 +4381,27 @@
         <v>3</v>
       </c>
       <c r="G33" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H33" s="105"/>
-      <c r="I33" s="105"/>
-    </row>
-    <row r="34" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H33" s="102" t="s">
+        <v>116</v>
+      </c>
+      <c r="I33" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="104" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B34" s="102" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C34" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D34" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E34" s="102">
         <v>13</v>
@@ -4386,23 +4410,27 @@
         <v>3</v>
       </c>
       <c r="G34" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
-    </row>
-    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H34" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="I34" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="104" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B35" s="102" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C35" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D35" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E35" s="102">
         <v>21</v>
@@ -4411,23 +4439,27 @@
         <v>3</v>
       </c>
       <c r="G35" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H35" s="105"/>
-      <c r="I35" s="105"/>
-    </row>
-    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H35" s="102" t="s">
+        <v>116</v>
+      </c>
+      <c r="I35" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="104" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B36" s="102" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C36" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D36" s="102" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E36" s="102">
         <v>21</v>
@@ -4436,23 +4468,27 @@
         <v>3</v>
       </c>
       <c r="G36" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H36" s="105"/>
-      <c r="I36" s="105"/>
-    </row>
-    <row r="37" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="H36" s="102" t="s">
+        <v>126</v>
+      </c>
+      <c r="I36" s="102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="104" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B37" s="102" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C37" s="102" t="s">
         <v>101</v>
       </c>
       <c r="D37" s="125" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E37" s="125">
         <v>21</v>
@@ -4461,10 +4497,14 @@
         <v>3</v>
       </c>
       <c r="G37" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="H37" s="124"/>
-      <c r="I37" s="124"/>
+        <v>181</v>
+      </c>
+      <c r="H37" s="125" t="s">
+        <v>96</v>
+      </c>
+      <c r="I37" s="102" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:I37" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}"/>
@@ -4491,13 +4531,16 @@
       <formula>"DESEJÁVEL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C26" xr:uid="{C6A8AFFE-3DC7-45BF-9737-E7A938D030B3}">
       <formula1>"Desejável, Essencial, Importante"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="O5" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4510,12 +4553,12 @@
       <selection activeCell="A7" sqref="A7:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4534,11 +4577,11 @@
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="126" t="s">
+      <c r="G1" s="133" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -4557,9 +4600,9 @@
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="126"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="133"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -4582,7 +4625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -4605,7 +4648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -4628,7 +4671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -4651,7 +4694,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -4672,7 +4715,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -4693,7 +4736,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
@@ -4714,7 +4757,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -4735,7 +4778,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
@@ -4756,7 +4799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>56</v>
       </c>
@@ -4777,7 +4820,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>59</v>
       </c>
@@ -4798,7 +4841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -4819,7 +4862,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -4840,7 +4883,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -4861,7 +4904,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>74</v>
       </c>
@@ -4908,120 +4951,120 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
-  <dimension ref="B1:R85"/>
+  <dimension ref="B1:R86"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q88" sqref="Q88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="127" t="s">
+    <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="129"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="136"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="127" t="s">
+      <c r="H2" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="129"/>
-      <c r="N2" s="127" t="s">
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
+      <c r="L2" s="136"/>
+      <c r="N2" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="129"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="135"/>
+      <c r="R2" s="136"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="134">
+      <c r="C3" s="141">
         <v>45554</v>
       </c>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="135"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="142"/>
       <c r="G3" s="7"/>
       <c r="H3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="134">
+      <c r="I3" s="141">
         <v>45555</v>
       </c>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="135"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="142"/>
       <c r="N3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="134">
+      <c r="O3" s="141">
         <v>45557</v>
       </c>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="134"/>
-      <c r="R3" s="135"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P3" s="141"/>
+      <c r="Q3" s="141"/>
+      <c r="R3" s="142"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="138" t="s">
+      <c r="C4" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="139"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="146"/>
       <c r="G4" s="8"/>
       <c r="H4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="138" t="s">
+      <c r="I4" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="138"/>
-      <c r="K4" s="138"/>
-      <c r="L4" s="139"/>
+      <c r="J4" s="145"/>
+      <c r="K4" s="145"/>
+      <c r="L4" s="146"/>
       <c r="N4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="138" t="s">
+      <c r="O4" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="138"/>
-      <c r="Q4" s="138"/>
-      <c r="R4" s="139"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P4" s="145"/>
+      <c r="Q4" s="145"/>
+      <c r="R4" s="146"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>81</v>
       </c>
@@ -5044,7 +5087,7 @@
       <c r="Q5" s="23"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>84</v>
       </c>
@@ -5067,7 +5110,7 @@
       <c r="Q6" s="29"/>
       <c r="R6" s="30"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>83</v>
       </c>
@@ -5088,7 +5131,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="17"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>85</v>
       </c>
@@ -5107,7 +5150,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="17"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>86</v>
       </c>
@@ -5126,46 +5169,46 @@
       <c r="Q9" s="31"/>
       <c r="R9" s="32"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="24"/>
       <c r="H10" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
       <c r="K10" s="23"/>
       <c r="L10" s="24"/>
       <c r="N10" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
       <c r="Q10" s="23"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="130" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131" t="s">
+      <c r="C11" s="138"/>
+      <c r="D11" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="131"/>
+      <c r="E11" s="138"/>
       <c r="F11" s="26" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="130" t="s">
+      <c r="H11" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="131"/>
+      <c r="I11" s="138"/>
       <c r="J11" s="28" t="s">
         <v>88</v>
       </c>
@@ -5173,37 +5216,37 @@
       <c r="L11" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="N11" s="130" t="s">
+      <c r="N11" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="O11" s="131"/>
+      <c r="O11" s="138"/>
       <c r="P11" s="44" t="s">
         <v>88</v>
       </c>
       <c r="Q11" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R11" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="133" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="140" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132" t="s">
+      <c r="C12" s="139"/>
+      <c r="D12" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="132"/>
+      <c r="E12" s="139"/>
       <c r="F12" s="18">
         <v>45560</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="132"/>
-      <c r="J12" s="132"/>
-      <c r="K12" s="132"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="139"/>
       <c r="L12" s="18"/>
       <c r="N12" s="51" t="s">
         <v>90</v>
@@ -5213,29 +5256,29 @@
         <v>96</v>
       </c>
       <c r="Q12" s="53" t="s">
-        <v>107</v>
+        <v>241</v>
       </c>
       <c r="R12" s="54">
         <v>45560</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="133" t="s">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="140" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132" t="s">
+      <c r="C13" s="139"/>
+      <c r="D13" s="139" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="132"/>
+      <c r="E13" s="139"/>
       <c r="F13" s="18">
         <v>45560</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="133"/>
-      <c r="I13" s="132"/>
-      <c r="J13" s="132"/>
-      <c r="K13" s="132"/>
+      <c r="H13" s="140"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="139"/>
       <c r="L13" s="18"/>
       <c r="N13" s="47" t="s">
         <v>91</v>
@@ -5244,30 +5287,30 @@
       <c r="P13" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="Q13" s="49" t="s">
-        <v>108</v>
+      <c r="Q13" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R13" s="50">
         <v>45560</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="133" t="s">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="140" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="132" t="s">
+      <c r="C14" s="139"/>
+      <c r="D14" s="139" t="s">
         <v>93</v>
       </c>
-      <c r="E14" s="132"/>
+      <c r="E14" s="139"/>
       <c r="F14" s="18">
         <v>45560</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="133"/>
-      <c r="I14" s="132"/>
-      <c r="J14" s="132"/>
-      <c r="K14" s="132"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="139"/>
       <c r="L14" s="18"/>
       <c r="N14" s="47" t="s">
         <v>92</v>
@@ -5276,29 +5319,29 @@
       <c r="P14" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="Q14" s="49" t="s">
-        <v>108</v>
+      <c r="Q14" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R14" s="50">
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="137" t="s">
+    <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="144" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="136"/>
-      <c r="D15" s="136" t="s">
+      <c r="C15" s="143"/>
+      <c r="D15" s="143" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="136"/>
+      <c r="E15" s="143"/>
       <c r="F15" s="21">
         <v>45560</v>
       </c>
-      <c r="H15" s="137"/>
-      <c r="I15" s="136"/>
-      <c r="J15" s="136"/>
-      <c r="K15" s="136"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="143"/>
+      <c r="J15" s="143"/>
+      <c r="K15" s="143"/>
       <c r="L15" s="21"/>
       <c r="N15" s="86" t="s">
         <v>94</v>
@@ -5308,13 +5351,13 @@
         <v>95</v>
       </c>
       <c r="Q15" s="75" t="s">
-        <v>107</v>
+        <v>241</v>
       </c>
       <c r="R15" s="76">
         <v>45560</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -5326,88 +5369,88 @@
       <c r="Q16" s="68"/>
       <c r="R16" s="69"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="127" t="s">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="128"/>
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="129"/>
-      <c r="H17" s="127" t="s">
+      <c r="C17" s="135"/>
+      <c r="D17" s="135"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="136"/>
+      <c r="H17" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="128"/>
-      <c r="J17" s="128"/>
-      <c r="K17" s="128"/>
-      <c r="L17" s="129"/>
-      <c r="N17" s="127" t="s">
+      <c r="I17" s="135"/>
+      <c r="J17" s="135"/>
+      <c r="K17" s="135"/>
+      <c r="L17" s="136"/>
+      <c r="N17" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="O17" s="128"/>
-      <c r="P17" s="128"/>
-      <c r="Q17" s="128"/>
-      <c r="R17" s="129"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O17" s="135"/>
+      <c r="P17" s="135"/>
+      <c r="Q17" s="135"/>
+      <c r="R17" s="136"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="134">
+      <c r="C18" s="141">
         <v>45558</v>
       </c>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="135"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="142"/>
       <c r="H18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="134">
+      <c r="I18" s="141">
         <v>45559</v>
       </c>
-      <c r="J18" s="134"/>
-      <c r="K18" s="134"/>
-      <c r="L18" s="135"/>
+      <c r="J18" s="141"/>
+      <c r="K18" s="141"/>
+      <c r="L18" s="142"/>
       <c r="N18" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="O18" s="134">
+      <c r="O18" s="141">
         <v>45560</v>
       </c>
-      <c r="P18" s="134"/>
-      <c r="Q18" s="134"/>
-      <c r="R18" s="135"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P18" s="141"/>
+      <c r="Q18" s="141"/>
+      <c r="R18" s="142"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="140" t="s">
+      <c r="C19" s="147" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="141"/>
+      <c r="D19" s="147"/>
+      <c r="E19" s="147"/>
+      <c r="F19" s="148"/>
       <c r="H19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="140" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" s="140"/>
-      <c r="K19" s="140"/>
-      <c r="L19" s="141"/>
+      <c r="I19" s="147" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" s="147"/>
+      <c r="K19" s="147"/>
+      <c r="L19" s="148"/>
       <c r="N19" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="140" t="s">
+      <c r="O19" s="147" t="s">
         <v>82</v>
       </c>
-      <c r="P19" s="140"/>
-      <c r="Q19" s="140"/>
-      <c r="R19" s="141"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P19" s="147"/>
+      <c r="Q19" s="147"/>
+      <c r="R19" s="148"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -5424,7 +5467,7 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="14"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="22" t="s">
         <v>81</v>
       </c>
@@ -5447,62 +5490,62 @@
       <c r="Q21" s="23"/>
       <c r="R21" s="24"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
       <c r="F22" s="37"/>
       <c r="H22" s="35" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I22" s="36"/>
       <c r="J22" s="36"/>
       <c r="K22" s="36"/>
       <c r="L22" s="37"/>
       <c r="N22" s="35" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="O22" s="36"/>
       <c r="P22" s="36"/>
       <c r="Q22" s="36"/>
       <c r="R22" s="37"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
       <c r="E23" s="39"/>
       <c r="F23" s="40"/>
       <c r="H23" s="38" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I23" s="39"/>
       <c r="J23" s="39"/>
       <c r="K23" s="39"/>
       <c r="L23" s="40"/>
       <c r="N23" s="38" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O23" s="39"/>
       <c r="P23" s="39"/>
       <c r="Q23" s="39"/>
       <c r="R23" s="40"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C24" s="39"/>
       <c r="D24" s="39"/>
       <c r="E24" s="39"/>
       <c r="F24" s="40"/>
       <c r="H24" s="38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
@@ -5514,7 +5557,7 @@
       <c r="Q24" s="39"/>
       <c r="R24" s="40"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
@@ -5531,121 +5574,121 @@
       <c r="Q25" s="42"/>
       <c r="R25" s="43"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
       <c r="F26" s="24"/>
       <c r="H26" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
       <c r="L26" s="24"/>
       <c r="N26" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
       <c r="Q26" s="23"/>
       <c r="R26" s="24"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="130" t="s">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="131"/>
+      <c r="C27" s="138"/>
       <c r="D27" s="44" t="s">
         <v>88</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="130" t="s">
+      <c r="H27" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="I27" s="131"/>
+      <c r="I27" s="138"/>
       <c r="J27" s="44" t="s">
         <v>88</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L27" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N27" s="130" t="s">
+      <c r="N27" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="O27" s="131"/>
+      <c r="O27" s="138"/>
       <c r="P27" s="44" t="s">
         <v>88</v>
       </c>
       <c r="Q27" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R27" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="90" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C28" s="91"/>
       <c r="D28" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="45" t="s">
-        <v>117</v>
+        <v>111</v>
+      </c>
+      <c r="E28" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F28" s="46">
         <v>45560</v>
       </c>
       <c r="H28" s="59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I28" s="60"/>
       <c r="J28" s="61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K28" s="61" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="L28" s="62">
         <v>45560</v>
       </c>
       <c r="N28" s="81" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O28" s="73"/>
       <c r="P28" s="73" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Q28" s="73" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="R28" s="74">
         <v>45537</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C29" s="48"/>
       <c r="D29" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="49" t="s">
         <v>117</v>
+      </c>
+      <c r="E29" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F29" s="50">
         <v>45560</v>
@@ -5655,111 +5698,111 @@
       </c>
       <c r="I29" s="64"/>
       <c r="J29" s="65" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K29" s="65" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="L29" s="66">
         <v>45560</v>
       </c>
       <c r="N29" s="82" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O29" s="53"/>
       <c r="P29" s="53" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="Q29" s="53" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="R29" s="54">
         <v>45537</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C30" s="52"/>
       <c r="D30" s="53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E30" s="53" t="s">
-        <v>31</v>
+        <v>241</v>
       </c>
       <c r="F30" s="54">
         <v>45560</v>
       </c>
       <c r="H30" s="63" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I30" s="64"/>
       <c r="J30" s="65" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K30" s="65" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="L30" s="66">
         <v>45560</v>
       </c>
       <c r="N30" s="82" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O30" s="53"/>
       <c r="P30" s="53" t="s">
         <v>95</v>
       </c>
       <c r="Q30" s="53" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="R30" s="54">
         <v>45537</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="51" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C31" s="52"/>
       <c r="D31" s="53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E31" s="53" t="s">
-        <v>31</v>
+        <v>241</v>
       </c>
       <c r="F31" s="54">
         <v>45565</v>
       </c>
       <c r="H31" s="63" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I31" s="64"/>
       <c r="J31" s="65" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K31" s="65" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="L31" s="66">
         <v>45565</v>
       </c>
       <c r="N31" s="82" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O31" s="53"/>
       <c r="P31" s="53" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q31" s="53" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="R31" s="54">
         <v>45537</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="55"/>
       <c r="C32" s="56"/>
       <c r="D32" s="56"/>
@@ -5775,39 +5818,39 @@
       </c>
       <c r="O32" s="84"/>
       <c r="P32" s="84" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q32" s="84" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="R32" s="85">
         <v>45561</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="127" t="s">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B35" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="128"/>
-      <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="129"/>
-      <c r="H35" s="127" t="s">
+      <c r="C35" s="135"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="135"/>
+      <c r="F35" s="136"/>
+      <c r="H35" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="I35" s="128"/>
-      <c r="J35" s="128"/>
-      <c r="K35" s="128"/>
-      <c r="L35" s="129"/>
-      <c r="N35" s="127" t="s">
+      <c r="I35" s="135"/>
+      <c r="J35" s="135"/>
+      <c r="K35" s="135"/>
+      <c r="L35" s="136"/>
+      <c r="N35" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="128"/>
-      <c r="P35" s="128"/>
-      <c r="Q35" s="128"/>
-      <c r="R35" s="129"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O35" s="135"/>
+      <c r="P35" s="135"/>
+      <c r="Q35" s="135"/>
+      <c r="R35" s="136"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>79</v>
       </c>
@@ -5820,12 +5863,12 @@
       <c r="H36" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="134">
+      <c r="I36" s="141">
         <v>45562</v>
       </c>
-      <c r="J36" s="134"/>
-      <c r="K36" s="134"/>
-      <c r="L36" s="135"/>
+      <c r="J36" s="141"/>
+      <c r="K36" s="141"/>
+      <c r="L36" s="142"/>
       <c r="N36" s="77" t="s">
         <v>79</v>
       </c>
@@ -5836,7 +5879,7 @@
       <c r="Q36" s="78"/>
       <c r="R36" s="79"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="s">
         <v>80</v>
       </c>
@@ -5849,12 +5892,12 @@
       <c r="H37" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I37" s="140" t="s">
-        <v>191</v>
-      </c>
-      <c r="J37" s="140"/>
-      <c r="K37" s="140"/>
-      <c r="L37" s="141"/>
+      <c r="I37" s="147" t="s">
+        <v>186</v>
+      </c>
+      <c r="J37" s="147"/>
+      <c r="K37" s="147"/>
+      <c r="L37" s="148"/>
       <c r="N37" s="80" t="s">
         <v>80</v>
       </c>
@@ -5865,7 +5908,7 @@
       <c r="Q37" s="33"/>
       <c r="R37" s="34"/>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
@@ -5882,7 +5925,7 @@
       <c r="Q38" s="31"/>
       <c r="R38" s="32"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B39" s="22" t="s">
         <v>81</v>
       </c>
@@ -5905,53 +5948,53 @@
       <c r="Q39" s="23"/>
       <c r="R39" s="24"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
       <c r="F40" s="30"/>
       <c r="H40" s="10" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I40" s="29"/>
       <c r="J40" s="29"/>
       <c r="K40" s="29"/>
       <c r="L40" s="30"/>
       <c r="N40" s="10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="O40" s="29"/>
       <c r="P40" s="29"/>
       <c r="Q40" s="29"/>
       <c r="R40" s="30"/>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="17"/>
       <c r="H41" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
       <c r="L41" s="17"/>
       <c r="N41" s="15" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="O41" s="16"/>
       <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
       <c r="R41" s="17"/>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B42" s="15"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -5968,7 +6011,7 @@
       <c r="Q42" s="16"/>
       <c r="R42" s="17"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
       <c r="C43" s="31"/>
       <c r="D43" s="31"/>
@@ -5985,299 +6028,299 @@
       <c r="Q43" s="31"/>
       <c r="R43" s="32"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B44" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="23"/>
       <c r="E44" s="23"/>
       <c r="F44" s="24"/>
       <c r="H44" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="24"/>
       <c r="N44" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="O44" s="23"/>
       <c r="P44" s="23"/>
       <c r="Q44" s="23"/>
       <c r="R44" s="24"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="130" t="s">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B45" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="131"/>
+      <c r="C45" s="138"/>
       <c r="D45" s="44" t="s">
         <v>88</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H45" s="130" t="s">
+      <c r="H45" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="I45" s="131"/>
+      <c r="I45" s="138"/>
       <c r="J45" s="44" t="s">
         <v>88</v>
       </c>
       <c r="K45" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L45" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N45" s="130" t="s">
+      <c r="N45" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="O45" s="131"/>
+      <c r="O45" s="138"/>
       <c r="P45" s="44" t="s">
         <v>88</v>
       </c>
       <c r="Q45" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R45" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B46" s="81" t="s">
-        <v>125</v>
-      </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73" t="s">
-        <v>119</v>
-      </c>
-      <c r="E46" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="F46" s="54">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B46" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="F46" s="50">
         <v>45571</v>
       </c>
       <c r="H46" s="88" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I46" s="45"/>
       <c r="J46" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="K46" s="49" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="K46" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L46" s="50">
         <v>45571</v>
       </c>
       <c r="N46" s="95" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O46" s="96"/>
       <c r="P46" s="96" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q46" s="97" t="s">
-        <v>133</v>
+        <v>240</v>
       </c>
       <c r="R46" s="98">
         <v>45571</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B47" s="89" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C47" s="49"/>
       <c r="D47" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="E47" s="49" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="E47" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F47" s="50">
         <v>45571</v>
       </c>
       <c r="H47" s="89" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I47" s="49"/>
       <c r="J47" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="K47" s="49" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="K47" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L47" s="50">
         <v>45571</v>
       </c>
       <c r="N47" s="89" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O47" s="49"/>
       <c r="P47" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q47" s="49" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="Q47" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R47" s="50">
         <v>45571</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B48" s="82" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C48" s="53"/>
       <c r="D48" s="53" t="s">
         <v>95</v>
       </c>
       <c r="E48" s="53" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="F48" s="54">
         <v>45571</v>
       </c>
       <c r="H48" s="89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I48" s="49"/>
       <c r="J48" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="K48" s="49" t="s">
-        <v>117</v>
+      <c r="K48" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L48" s="50">
         <v>45571</v>
       </c>
       <c r="N48" s="89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O48" s="49"/>
       <c r="P48" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="Q48" s="49" t="s">
-        <v>117</v>
+      <c r="Q48" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R48" s="50">
         <v>45571</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B49" s="82" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C49" s="53"/>
       <c r="D49" s="53" t="s">
         <v>96</v>
       </c>
       <c r="E49" s="53" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="F49" s="54">
         <v>45571</v>
       </c>
       <c r="H49" s="89" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I49" s="49"/>
       <c r="J49" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="K49" s="49" t="s">
-        <v>117</v>
+      <c r="K49" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L49" s="50">
         <v>45571</v>
       </c>
       <c r="N49" s="89" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O49" s="49"/>
       <c r="P49" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="Q49" s="49" t="s">
-        <v>117</v>
+      <c r="Q49" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R49" s="50">
         <v>45571</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B50" s="92" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C50" s="93"/>
       <c r="D50" s="93" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E50" s="93" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
       <c r="F50" s="94">
         <v>45571</v>
       </c>
       <c r="H50" s="92" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I50" s="93"/>
       <c r="J50" s="93" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K50" s="93" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
       <c r="L50" s="94">
         <v>45571</v>
       </c>
       <c r="N50" s="92" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O50" s="93"/>
       <c r="P50" s="93" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q50" s="93" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
       <c r="R50" s="94">
         <v>45571</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="127" t="s">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B53" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="128"/>
-      <c r="D53" s="128"/>
-      <c r="E53" s="128"/>
-      <c r="F53" s="129"/>
-      <c r="H53" s="127" t="s">
+      <c r="C53" s="135"/>
+      <c r="D53" s="135"/>
+      <c r="E53" s="135"/>
+      <c r="F53" s="136"/>
+      <c r="H53" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="I53" s="128"/>
-      <c r="J53" s="128"/>
-      <c r="K53" s="128"/>
-      <c r="L53" s="129"/>
-      <c r="N53" s="127" t="s">
+      <c r="I53" s="135"/>
+      <c r="J53" s="135"/>
+      <c r="K53" s="135"/>
+      <c r="L53" s="136"/>
+      <c r="N53" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="O53" s="128"/>
-      <c r="P53" s="128"/>
-      <c r="Q53" s="128"/>
-      <c r="R53" s="129"/>
-    </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O53" s="135"/>
+      <c r="P53" s="135"/>
+      <c r="Q53" s="135"/>
+      <c r="R53" s="136"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
         <v>79</v>
       </c>
@@ -6306,7 +6349,7 @@
       <c r="Q54" s="70"/>
       <c r="R54" s="71"/>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B55" s="15" t="s">
         <v>80</v>
       </c>
@@ -6335,7 +6378,7 @@
       <c r="Q55" s="16"/>
       <c r="R55" s="17"/>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B56" s="12"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -6352,7 +6395,7 @@
       <c r="Q56" s="20"/>
       <c r="R56" s="72"/>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B57" s="22" t="s">
         <v>81</v>
       </c>
@@ -6375,55 +6418,55 @@
       <c r="Q57" s="23"/>
       <c r="R57" s="24"/>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C58" s="29"/>
       <c r="D58" s="29"/>
       <c r="E58" s="29"/>
       <c r="F58" s="30"/>
       <c r="H58" s="118" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="I58" s="119"/>
       <c r="J58" s="119"/>
       <c r="K58" s="119"/>
       <c r="L58" s="120"/>
       <c r="N58" s="118" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O58" s="119"/>
       <c r="P58" s="119"/>
       <c r="Q58" s="119"/>
       <c r="R58" s="120"/>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B59" s="15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
       <c r="F59" s="17"/>
       <c r="H59" s="117" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="I59" s="121"/>
       <c r="J59" s="121"/>
       <c r="K59" s="121"/>
       <c r="L59" s="122"/>
       <c r="N59" s="117" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="O59" s="121"/>
       <c r="P59" s="121"/>
       <c r="Q59" s="121"/>
       <c r="R59" s="122"/>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B60" s="15" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
@@ -6435,16 +6478,16 @@
       <c r="K60" s="16"/>
       <c r="L60" s="17"/>
       <c r="N60" s="123" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="O60" s="16"/>
       <c r="P60" s="16"/>
       <c r="Q60" s="16"/>
       <c r="R60" s="17"/>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B61" s="12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="31"/>
@@ -6456,333 +6499,327 @@
       <c r="K61" s="31"/>
       <c r="L61" s="32"/>
       <c r="N61" s="12" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="O61" s="31"/>
       <c r="P61" s="31"/>
       <c r="Q61" s="31"/>
       <c r="R61" s="32"/>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B62" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="23"/>
       <c r="E62" s="23"/>
       <c r="F62" s="24"/>
       <c r="H62" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I62" s="23"/>
       <c r="J62" s="23"/>
       <c r="K62" s="23"/>
       <c r="L62" s="24"/>
       <c r="N62" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="O62" s="23"/>
       <c r="P62" s="23"/>
       <c r="Q62" s="23"/>
       <c r="R62" s="24"/>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="130" t="s">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B63" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="131"/>
+      <c r="C63" s="138"/>
       <c r="D63" s="44" t="s">
         <v>88</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="130" t="s">
+      <c r="H63" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="I63" s="131"/>
+      <c r="I63" s="138"/>
       <c r="J63" s="44" t="s">
         <v>88</v>
       </c>
       <c r="K63" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N63" s="130" t="s">
+      <c r="N63" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="O63" s="131"/>
+      <c r="O63" s="138"/>
       <c r="P63" s="44" t="s">
         <v>88</v>
       </c>
       <c r="Q63" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R63" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B64" s="95" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C64" s="96"/>
       <c r="D64" s="96" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E64" s="97" t="s">
-        <v>133</v>
+        <v>240</v>
       </c>
       <c r="F64" s="98">
         <v>45571</v>
       </c>
       <c r="H64" s="95" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I64" s="96"/>
       <c r="J64" s="96" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K64" s="97" t="s">
-        <v>133</v>
+        <v>240</v>
       </c>
       <c r="L64" s="98">
         <v>45571</v>
       </c>
       <c r="N64" s="95" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O64" s="96"/>
       <c r="P64" s="96" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q64" s="97" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="R64" s="98">
         <v>45571</v>
       </c>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B65" s="89" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C65" s="49"/>
       <c r="D65" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="E65" s="49" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="E65" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F65" s="50">
         <v>45571</v>
       </c>
       <c r="H65" s="89" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I65" s="49"/>
       <c r="J65" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="K65" s="49" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="K65" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L65" s="50">
         <v>45573</v>
       </c>
       <c r="N65" s="89" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O65" s="49"/>
       <c r="P65" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q65" s="49" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="Q65" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R65" s="50">
         <v>45576</v>
       </c>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B66" s="89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C66" s="49"/>
       <c r="D66" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="E66" s="49" t="s">
-        <v>117</v>
+      <c r="E66" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F66" s="50">
         <v>45571</v>
       </c>
       <c r="H66" s="89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I66" s="49"/>
       <c r="J66" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="K66" s="49" t="s">
-        <v>117</v>
+      <c r="K66" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L66" s="50">
         <v>45573</v>
       </c>
       <c r="N66" s="89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O66" s="49"/>
       <c r="P66" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="Q66" s="49" t="s">
-        <v>117</v>
+      <c r="Q66" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R66" s="50">
         <v>45576</v>
       </c>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B67" s="89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C67" s="49"/>
       <c r="D67" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E67" s="49" t="s">
-        <v>117</v>
+      <c r="E67" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F67" s="50">
         <v>45571</v>
       </c>
       <c r="H67" s="89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I67" s="49"/>
       <c r="J67" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="K67" s="49" t="s">
-        <v>117</v>
+      <c r="K67" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L67" s="50">
         <v>45573</v>
       </c>
       <c r="N67" s="89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="O67" s="49"/>
       <c r="P67" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="Q67" s="49" t="s">
-        <v>117</v>
+      <c r="Q67" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="R67" s="50">
         <v>45576</v>
       </c>
     </row>
-    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B68" s="89" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C68" s="49"/>
       <c r="D68" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="E68" s="49" t="s">
         <v>117</v>
+      </c>
+      <c r="E68" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F68" s="50">
         <v>45571</v>
       </c>
       <c r="H68" s="89" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I68" s="49"/>
       <c r="J68" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="K68" s="49" t="s">
         <v>117</v>
+      </c>
+      <c r="K68" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="L68" s="50">
         <v>45573</v>
       </c>
-      <c r="N68" s="89" t="s">
-        <v>200</v>
-      </c>
-      <c r="O68" s="49"/>
-      <c r="P68" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q68" s="49" t="s">
+      <c r="N68" s="92" t="s">
+        <v>195</v>
+      </c>
+      <c r="O68" s="93"/>
+      <c r="P68" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="R68" s="50">
+      <c r="Q68" s="93" t="s">
+        <v>249</v>
+      </c>
+      <c r="R68" s="94">
         <v>45576</v>
       </c>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B69" s="99" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C69" s="75"/>
       <c r="D69" s="75" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E69" s="75" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="F69" s="76">
         <v>45571</v>
       </c>
       <c r="H69" s="114" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I69" s="115"/>
       <c r="J69" s="115" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K69" s="115" t="s">
-        <v>133</v>
+        <v>240</v>
       </c>
       <c r="L69" s="116">
         <v>45572</v>
       </c>
-      <c r="N69" s="114" t="s">
-        <v>203</v>
-      </c>
-      <c r="O69" s="115"/>
-      <c r="P69" s="115" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q69" s="115" t="s">
-        <v>133</v>
-      </c>
-      <c r="R69" s="116">
-        <v>45572</v>
-      </c>
-    </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B71" s="127" t="s">
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B71" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="C71" s="128"/>
-      <c r="D71" s="128"/>
-      <c r="E71" s="128"/>
-      <c r="F71" s="129"/>
-    </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C71" s="135"/>
+      <c r="D71" s="135"/>
+      <c r="E71" s="135"/>
+      <c r="F71" s="136"/>
+      <c r="H71" s="134" t="s">
+        <v>78</v>
+      </c>
+      <c r="I71" s="135"/>
+      <c r="J71" s="135"/>
+      <c r="K71" s="135"/>
+      <c r="L71" s="136"/>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B72" s="10" t="s">
         <v>79</v>
       </c>
@@ -6792,26 +6829,49 @@
       <c r="D72" s="70"/>
       <c r="E72" s="70"/>
       <c r="F72" s="71"/>
-    </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H72" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I72" s="11">
+        <v>45574</v>
+      </c>
+      <c r="J72" s="70"/>
+      <c r="K72" s="70"/>
+      <c r="L72" s="71"/>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B73" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
       <c r="F73" s="17"/>
-    </row>
-    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H73" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I73" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="17"/>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B74" s="12"/>
       <c r="C74" s="20"/>
       <c r="D74" s="20"/>
       <c r="E74" s="20"/>
       <c r="F74" s="72"/>
-    </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H74" s="12"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="20"/>
+      <c r="L74" s="72"/>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B75" s="22" t="s">
         <v>81</v>
       </c>
@@ -6819,127 +6879,247 @@
       <c r="D75" s="23"/>
       <c r="E75" s="23"/>
       <c r="F75" s="24"/>
-    </row>
-    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H75" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="I75" s="23"/>
+      <c r="J75" s="23"/>
+      <c r="K75" s="23"/>
+      <c r="L75" s="24"/>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B76" s="118" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C76" s="119"/>
       <c r="D76" s="119"/>
       <c r="E76" s="119"/>
       <c r="F76" s="120"/>
-    </row>
-    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H76" s="118" t="s">
+        <v>245</v>
+      </c>
+      <c r="I76" s="119"/>
+      <c r="J76" s="119"/>
+      <c r="K76" s="119"/>
+      <c r="L76" s="120"/>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B77" s="117" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C77" s="121"/>
       <c r="D77" s="121"/>
       <c r="E77" s="121"/>
       <c r="F77" s="122"/>
-    </row>
-    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H77" s="117" t="s">
+        <v>246</v>
+      </c>
+      <c r="I77" s="121"/>
+      <c r="J77" s="121"/>
+      <c r="K77" s="121"/>
+      <c r="L77" s="122"/>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B78" s="123" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C78" s="16"/>
       <c r="D78" s="16"/>
       <c r="E78" s="16"/>
       <c r="F78" s="17"/>
-    </row>
-    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H78" s="123" t="s">
+        <v>247</v>
+      </c>
+      <c r="I78" s="16"/>
+      <c r="J78" s="16"/>
+      <c r="K78" s="16"/>
+      <c r="L78" s="17"/>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B79" s="12"/>
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
       <c r="F79" s="32"/>
-    </row>
-    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H79" s="12"/>
+      <c r="I79" s="31"/>
+      <c r="J79" s="31"/>
+      <c r="K79" s="31"/>
+      <c r="L79" s="32"/>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B80" s="22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C80" s="23"/>
       <c r="D80" s="23"/>
       <c r="E80" s="23"/>
       <c r="F80" s="24"/>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="130" t="s">
+      <c r="H80" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="I80" s="23"/>
+      <c r="J80" s="23"/>
+      <c r="K80" s="23"/>
+      <c r="L80" s="24"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B81" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C81" s="131"/>
+      <c r="C81" s="138"/>
       <c r="D81" s="44" t="s">
         <v>88</v>
       </c>
       <c r="E81" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F81" s="26" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H81" s="137" t="s">
+        <v>87</v>
+      </c>
+      <c r="I81" s="138"/>
+      <c r="J81" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="K81" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="L81" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B82" s="89" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C82" s="49"/>
       <c r="D82" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="E82" s="49" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="E82" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F82" s="50">
         <v>45576</v>
       </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H82" s="89" t="s">
+        <v>122</v>
+      </c>
+      <c r="I82" s="49"/>
+      <c r="J82" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="K82" s="149" t="s">
+        <v>249</v>
+      </c>
+      <c r="L82" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B83" s="89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C83" s="49"/>
       <c r="D83" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="E83" s="49" t="s">
-        <v>117</v>
+      <c r="E83" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F83" s="50">
         <v>45576</v>
       </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H83" s="89" t="s">
+        <v>123</v>
+      </c>
+      <c r="I83" s="49"/>
+      <c r="J83" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="K83" s="149" t="s">
+        <v>249</v>
+      </c>
+      <c r="L83" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B84" s="89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C84" s="49"/>
       <c r="D84" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E84" s="49" t="s">
-        <v>117</v>
+      <c r="E84" s="149" t="s">
+        <v>249</v>
       </c>
       <c r="F84" s="50">
         <v>45576</v>
       </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H84" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="I84" s="49"/>
+      <c r="J84" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="K84" s="149" t="s">
+        <v>249</v>
+      </c>
+      <c r="L84" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B85" s="92" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C85" s="93"/>
       <c r="D85" s="93" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E85" s="93" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
       <c r="F85" s="94">
         <v>45576</v>
       </c>
+      <c r="H85" s="89" t="s">
+        <v>195</v>
+      </c>
+      <c r="I85" s="149"/>
+      <c r="J85" s="149" t="s">
+        <v>117</v>
+      </c>
+      <c r="K85" s="149" t="s">
+        <v>249</v>
+      </c>
+      <c r="L85" s="50">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H86" s="92" t="s">
+        <v>248</v>
+      </c>
+      <c r="I86" s="93"/>
+      <c r="J86" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="K86" s="93" t="s">
+        <v>249</v>
+      </c>
+      <c r="L86" s="94">
+        <v>45577</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="59">
     <mergeCell ref="N53:R53"/>
     <mergeCell ref="N63:O63"/>
     <mergeCell ref="J15:K15"/>
@@ -6997,6 +7177,8 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="H81:I81"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Arrumando pasta de documentação e gráfico de burndown
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-diesel-2\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Gotardo\Desktop\Projeto\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3539E-7497-49D0-8751-3239EC06FC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2226429B-0E18-44E0-9F87-13BCC55D24BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -1324,16 +1324,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14999847407452621"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14999847407452621"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14999847407452621"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14999847407452621"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1341,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1607,7 +1607,6 @@
     <xf numFmtId="164" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1639,92 +1638,355 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1746,27 +2008,6 @@
         <i val="0"/>
         <color rgb="FFFFC000"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2009,13 +2250,13 @@
                   <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>119</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>139</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2969,8 +3210,8 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>287111</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>266699</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3316,11 +3557,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:AF161"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3334,127 +3575,162 @@
     <col min="7" max="7" width="17.5546875" style="103" customWidth="1"/>
     <col min="8" max="8" width="19.5546875" style="98" customWidth="1"/>
     <col min="9" max="9" width="22.44140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="98"/>
+    <col min="10" max="10" width="9.109375" style="146"/>
     <col min="11" max="11" width="15.44140625" style="98" customWidth="1"/>
     <col min="12" max="12" width="13" style="98" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="98"/>
+    <col min="13" max="13" width="9.109375" style="146"/>
     <col min="14" max="14" width="15.5546875" style="98" customWidth="1"/>
     <col min="15" max="15" width="10.6640625" style="98" customWidth="1"/>
-    <col min="16" max="17" width="9.109375" style="98"/>
+    <col min="16" max="16" width="9.109375" style="146"/>
+    <col min="17" max="17" width="9.109375" style="98"/>
     <col min="18" max="18" width="15.6640625" style="98" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="98"/>
+    <col min="19" max="19" width="9.109375" style="146"/>
+    <col min="20" max="20" width="9.109375" style="153"/>
+    <col min="21" max="32" width="9.109375" style="146"/>
+    <col min="33" max="16384" width="9.109375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+    <row r="1" spans="1:32" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="147" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="132"/>
-    </row>
-    <row r="2" spans="1:18" s="122" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="N1" s="146"/>
+      <c r="O1" s="146"/>
+      <c r="Q1" s="146"/>
+      <c r="R1" s="146"/>
+    </row>
+    <row r="2" spans="1:32" s="121" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="124" t="s">
+      <c r="C2" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="124" t="s">
+      <c r="D2" s="148" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="124" t="s">
+      <c r="E2" s="148" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="124" t="s">
+      <c r="F2" s="148" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="124" t="s">
+      <c r="G2" s="148" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="124" t="s">
+      <c r="H2" s="148" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="124" t="s">
+      <c r="I2" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="100"/>
-    </row>
-    <row r="3" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="102" t="s">
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="153"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+      <c r="S2" s="153"/>
+      <c r="T2" s="153"/>
+      <c r="U2" s="153"/>
+      <c r="V2" s="153"/>
+      <c r="W2" s="153"/>
+      <c r="X2" s="153"/>
+      <c r="Y2" s="153"/>
+      <c r="Z2" s="153"/>
+      <c r="AA2" s="153"/>
+      <c r="AB2" s="153"/>
+      <c r="AC2" s="153"/>
+      <c r="AD2" s="153"/>
+      <c r="AE2" s="153"/>
+      <c r="AF2" s="153"/>
+    </row>
+    <row r="3" spans="1:32" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="151" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="151" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="151" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="151" t="s">
         <v>211</v>
       </c>
-      <c r="E3" s="100">
+      <c r="E3" s="151">
         <v>21</v>
       </c>
-      <c r="F3" s="100">
+      <c r="F3" s="151">
         <v>2</v>
       </c>
-      <c r="G3" s="100" t="s">
+      <c r="G3" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="100" t="s">
+      <c r="H3" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="I3" s="100" t="s">
+      <c r="I3" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="133" t="s">
+      <c r="K3" s="127" t="s">
         <v>217</v>
       </c>
-      <c r="L3" s="133"/>
-      <c r="N3" s="133" t="s">
+      <c r="L3" s="127"/>
+      <c r="N3" s="127" t="s">
         <v>218</v>
       </c>
-      <c r="O3" s="133"/>
-      <c r="Q3" s="133" t="s">
+      <c r="O3" s="127"/>
+      <c r="Q3" s="127" t="s">
         <v>232</v>
       </c>
-      <c r="R3" s="133"/>
-    </row>
-    <row r="4" spans="1:18" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="102" t="s">
+      <c r="R3" s="127"/>
+      <c r="T3" s="153">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="149" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="150" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E4" s="100">
+      <c r="E4" s="151">
         <v>8</v>
       </c>
-      <c r="F4" s="100">
+      <c r="F4" s="151">
         <v>1</v>
       </c>
-      <c r="G4" s="100" t="s">
+      <c r="G4" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H4" s="100" t="s">
+      <c r="H4" s="151" t="s">
         <v>95</v>
       </c>
-      <c r="I4" s="100" t="s">
+      <c r="I4" s="151" t="s">
         <v>47</v>
       </c>
       <c r="K4" s="106" t="s">
@@ -3471,45 +3747,47 @@
         <f>SUM(O5:O7)</f>
         <v>154</v>
       </c>
-      <c r="Q4" s="128" t="s">
+      <c r="Q4" s="125" t="s">
         <v>233</v>
       </c>
-      <c r="R4" s="129"/>
-    </row>
-    <row r="5" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="102" t="s">
+      <c r="R4" s="126"/>
+      <c r="T4" s="153">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="149" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="100" t="s">
+      <c r="D5" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E5" s="100">
+      <c r="E5" s="151">
         <v>8</v>
       </c>
-      <c r="F5" s="100">
+      <c r="F5" s="151">
         <v>1</v>
       </c>
-      <c r="G5" s="100" t="s">
+      <c r="G5" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H5" s="100" t="s">
+      <c r="H5" s="151" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="100" t="s">
+      <c r="I5" s="151" t="s">
         <v>240</v>
       </c>
       <c r="K5" s="107" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="108">
-        <f>SUMIF($G$3:$G$37,K5,$E$3:$E$37)</f>
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="N5" s="107" t="s">
         <v>172</v>
@@ -3518,45 +3796,47 @@
         <f>SUM(E15:E26)</f>
         <v>88</v>
       </c>
-      <c r="Q5" s="128" t="s">
+      <c r="Q5" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="R5" s="129"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="102" t="s">
+      <c r="R5" s="126"/>
+      <c r="T5" s="153">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="149" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="150" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="100">
+      <c r="E6" s="151">
         <v>8</v>
       </c>
-      <c r="F6" s="100">
+      <c r="F6" s="151">
         <v>1</v>
       </c>
-      <c r="G6" s="100" t="s">
+      <c r="G6" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="100" t="s">
+      <c r="H6" s="151" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="100" t="s">
+      <c r="I6" s="151" t="s">
         <v>47</v>
       </c>
       <c r="K6" s="107" t="s">
         <v>137</v>
       </c>
       <c r="L6" s="108">
-        <f t="shared" ref="L6:L7" si="0">SUMIF($G$3:$G$37,K6,$E$3:$E$37)</f>
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="N6" s="107" t="s">
         <v>137</v>
@@ -3565,45 +3845,47 @@
         <f>SUM(E3,E6,E8,E12,E13)</f>
         <v>66</v>
       </c>
-      <c r="Q6" s="128" t="s">
+      <c r="Q6" s="125" t="s">
         <v>235</v>
       </c>
-      <c r="R6" s="129"/>
-    </row>
-    <row r="7" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="102" t="s">
+      <c r="R6" s="126"/>
+      <c r="T6" s="153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="149" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="150" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E7" s="100">
+      <c r="E7" s="151">
         <v>8</v>
       </c>
-      <c r="F7" s="100">
+      <c r="F7" s="151">
         <v>1</v>
       </c>
-      <c r="G7" s="100" t="s">
+      <c r="G7" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="100" t="s">
+      <c r="H7" s="151" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="100" t="s">
+      <c r="I7" s="151" t="s">
         <v>240</v>
       </c>
       <c r="K7" s="107" t="s">
         <v>179</v>
       </c>
       <c r="L7" s="108">
-        <f t="shared" si="0"/>
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="N7" s="107" t="s">
         <v>179</v>
@@ -3611,37 +3893,37 @@
       <c r="O7" s="108">
         <v>0</v>
       </c>
-      <c r="Q7" s="128" t="s">
+      <c r="Q7" s="125" t="s">
         <v>236</v>
       </c>
-      <c r="R7" s="129"/>
-    </row>
-    <row r="8" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="102" t="s">
+      <c r="R7" s="126"/>
+    </row>
+    <row r="8" spans="1:32" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="149" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="150" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="100" t="s">
+      <c r="D8" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E8" s="100">
+      <c r="E8" s="151">
         <v>8</v>
       </c>
-      <c r="F8" s="100">
+      <c r="F8" s="151">
         <v>1</v>
       </c>
-      <c r="G8" s="100" t="s">
+      <c r="G8" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H8" s="100" t="s">
+      <c r="H8" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="151" t="s">
         <v>47</v>
       </c>
       <c r="K8" s="107" t="s">
@@ -3656,37 +3938,37 @@
       <c r="O8" s="108">
         <v>0</v>
       </c>
-      <c r="Q8" s="128" t="s">
+      <c r="Q8" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="R8" s="129"/>
-    </row>
-    <row r="9" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="102" t="s">
+      <c r="R8" s="126"/>
+    </row>
+    <row r="9" spans="1:32" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="149" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="150" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="151" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="151" t="s">
         <v>210</v>
       </c>
-      <c r="E9" s="100">
+      <c r="E9" s="151">
         <v>5</v>
       </c>
-      <c r="F9" s="100">
+      <c r="F9" s="151">
         <v>2</v>
       </c>
-      <c r="G9" s="100" t="s">
+      <c r="G9" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H9" s="100" t="s">
+      <c r="H9" s="151" t="s">
         <v>95</v>
       </c>
-      <c r="I9" s="100" t="s">
+      <c r="I9" s="151" t="s">
         <v>47</v>
       </c>
       <c r="K9" s="109" t="s">
@@ -3694,7 +3976,7 @@
       </c>
       <c r="L9" s="110">
         <f>AVERAGE(L5:L7)</f>
-        <v>115.33333333333333</v>
+        <v>115</v>
       </c>
       <c r="N9" s="109" t="s">
         <v>216</v>
@@ -3703,160 +3985,185 @@
         <f>AVERAGE(O5:O7)</f>
         <v>51.333333333333336</v>
       </c>
-      <c r="Q9" s="101"/>
-    </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="102" t="s">
+      <c r="Q9" s="154"/>
+      <c r="R9" s="146"/>
+    </row>
+    <row r="10" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="149" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="150" t="s">
         <v>151</v>
       </c>
-      <c r="C10" s="100" t="s">
+      <c r="C10" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="100" t="s">
+      <c r="D10" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E10" s="100">
+      <c r="E10" s="151">
         <v>8</v>
       </c>
-      <c r="F10" s="100">
+      <c r="F10" s="151">
         <v>1</v>
       </c>
-      <c r="G10" s="100" t="s">
+      <c r="G10" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H10" s="100" t="s">
+      <c r="H10" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="I10" s="100" t="s">
+      <c r="I10" s="151" t="s">
         <v>240</v>
       </c>
-      <c r="Q10" s="101"/>
-    </row>
-    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="102" t="s">
+      <c r="K10" s="146"/>
+      <c r="L10" s="146"/>
+      <c r="N10" s="146"/>
+      <c r="O10" s="146"/>
+      <c r="Q10" s="154"/>
+      <c r="R10" s="146"/>
+    </row>
+    <row r="11" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="149" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="150" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E11" s="100">
+      <c r="E11" s="151">
         <v>8</v>
       </c>
-      <c r="F11" s="100">
+      <c r="F11" s="151">
         <v>1</v>
       </c>
-      <c r="G11" s="100" t="s">
+      <c r="G11" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H11" s="100" t="s">
+      <c r="H11" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="I11" s="100" t="s">
+      <c r="I11" s="151" t="s">
         <v>240</v>
       </c>
-      <c r="Q11" s="101"/>
-    </row>
-    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="102" t="s">
+      <c r="K11" s="146"/>
+      <c r="L11" s="146"/>
+      <c r="N11" s="146"/>
+      <c r="O11" s="146"/>
+      <c r="Q11" s="154"/>
+      <c r="R11" s="146"/>
+    </row>
+    <row r="12" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="149" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="150" t="s">
         <v>154</v>
       </c>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="151" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="100">
+      <c r="E12" s="151">
         <v>21</v>
       </c>
-      <c r="F12" s="100">
+      <c r="F12" s="151">
         <v>1</v>
       </c>
-      <c r="G12" s="100" t="s">
+      <c r="G12" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H12" s="100" t="s">
+      <c r="H12" s="151" t="s">
         <v>95</v>
       </c>
-      <c r="I12" s="100" t="s">
+      <c r="I12" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="K12" s="111"/>
-      <c r="Q12" s="101"/>
-    </row>
-    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="102" t="s">
+      <c r="K12" s="155"/>
+      <c r="L12" s="146"/>
+      <c r="N12" s="146"/>
+      <c r="O12" s="146"/>
+      <c r="Q12" s="154"/>
+      <c r="R12" s="146"/>
+    </row>
+    <row r="13" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="149" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="150" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="100" t="s">
+      <c r="C13" s="151" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E13" s="100">
+      <c r="E13" s="151">
         <v>8</v>
       </c>
-      <c r="F13" s="100">
+      <c r="F13" s="151">
         <v>2</v>
       </c>
-      <c r="G13" s="100" t="s">
+      <c r="G13" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H13" s="100" t="s">
+      <c r="H13" s="151" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="100" t="s">
+      <c r="I13" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="101"/>
-    </row>
-    <row r="14" spans="1:18" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="102" t="s">
+      <c r="K13" s="146"/>
+      <c r="L13" s="146"/>
+      <c r="N13" s="146"/>
+      <c r="O13" s="146"/>
+      <c r="Q13" s="154"/>
+      <c r="R13" s="146"/>
+    </row>
+    <row r="14" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="149" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="C14" s="100" t="s">
+      <c r="C14" s="151" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D14" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E14" s="100">
+      <c r="E14" s="151">
         <v>8</v>
       </c>
-      <c r="F14" s="100">
+      <c r="F14" s="151">
         <v>2</v>
       </c>
-      <c r="G14" s="100" t="s">
+      <c r="G14" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="H14" s="100" t="s">
+      <c r="H14" s="151" t="s">
         <v>125</v>
       </c>
-      <c r="I14" s="100" t="s">
+      <c r="I14" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="Q14" s="101"/>
-    </row>
-    <row r="15" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="146"/>
+      <c r="L14" s="146"/>
+      <c r="N14" s="146"/>
+      <c r="O14" s="146"/>
+      <c r="Q14" s="154"/>
+      <c r="R14" s="146"/>
+    </row>
+    <row r="15" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="102" t="s">
         <v>134</v>
       </c>
@@ -3884,9 +4191,26 @@
       <c r="I15" s="100" t="s">
         <v>47</v>
       </c>
+      <c r="J15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="P15" s="98"/>
       <c r="Q15" s="101"/>
-    </row>
-    <row r="16" spans="1:18" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S15" s="98"/>
+      <c r="T15" s="98"/>
+      <c r="U15" s="98"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="98"/>
+      <c r="X15" s="98"/>
+      <c r="Y15" s="98"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="98"/>
+      <c r="AB15" s="98"/>
+      <c r="AC15" s="98"/>
+      <c r="AD15" s="98"/>
+      <c r="AE15" s="98"/>
+      <c r="AF15" s="98"/>
+    </row>
+    <row r="16" spans="1:32" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="102" t="s">
         <v>5</v>
       </c>
@@ -3914,9 +4238,26 @@
       <c r="I16" s="100" t="s">
         <v>47</v>
       </c>
+      <c r="J16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="P16" s="98"/>
       <c r="Q16" s="101"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S16" s="98"/>
+      <c r="T16" s="98"/>
+      <c r="U16" s="98"/>
+      <c r="V16" s="98"/>
+      <c r="W16" s="98"/>
+      <c r="X16" s="98"/>
+      <c r="Y16" s="98"/>
+      <c r="Z16" s="98"/>
+      <c r="AA16" s="98"/>
+      <c r="AB16" s="98"/>
+      <c r="AC16" s="98"/>
+      <c r="AD16" s="98"/>
+      <c r="AE16" s="98"/>
+      <c r="AF16" s="98"/>
+    </row>
+    <row r="17" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="102" t="s">
         <v>159</v>
       </c>
@@ -3944,8 +4285,25 @@
       <c r="I17" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="P17" s="98"/>
+      <c r="S17" s="98"/>
+      <c r="T17" s="98"/>
+      <c r="U17" s="98"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="98"/>
+      <c r="X17" s="98"/>
+      <c r="Y17" s="98"/>
+      <c r="Z17" s="98"/>
+      <c r="AA17" s="98"/>
+      <c r="AB17" s="98"/>
+      <c r="AC17" s="98"/>
+      <c r="AD17" s="98"/>
+      <c r="AE17" s="98"/>
+      <c r="AF17" s="98"/>
+    </row>
+    <row r="18" spans="1:32" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="102" t="s">
         <v>162</v>
       </c>
@@ -3973,8 +4331,25 @@
       <c r="I18" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="P18" s="98"/>
+      <c r="S18" s="98"/>
+      <c r="T18" s="98"/>
+      <c r="U18" s="98"/>
+      <c r="V18" s="98"/>
+      <c r="W18" s="98"/>
+      <c r="X18" s="98"/>
+      <c r="Y18" s="98"/>
+      <c r="Z18" s="98"/>
+      <c r="AA18" s="98"/>
+      <c r="AB18" s="98"/>
+      <c r="AC18" s="98"/>
+      <c r="AD18" s="98"/>
+      <c r="AE18" s="98"/>
+      <c r="AF18" s="98"/>
+    </row>
+    <row r="19" spans="1:32" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="102" t="s">
         <v>10</v>
       </c>
@@ -4002,8 +4377,25 @@
       <c r="I19" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="P19" s="98"/>
+      <c r="S19" s="98"/>
+      <c r="T19" s="98"/>
+      <c r="U19" s="98"/>
+      <c r="V19" s="98"/>
+      <c r="W19" s="98"/>
+      <c r="X19" s="98"/>
+      <c r="Y19" s="98"/>
+      <c r="Z19" s="98"/>
+      <c r="AA19" s="98"/>
+      <c r="AB19" s="98"/>
+      <c r="AC19" s="98"/>
+      <c r="AD19" s="98"/>
+      <c r="AE19" s="98"/>
+      <c r="AF19" s="98"/>
+    </row>
+    <row r="20" spans="1:32" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="102" t="s">
         <v>11</v>
       </c>
@@ -4031,8 +4423,25 @@
       <c r="I20" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="P20" s="98"/>
+      <c r="S20" s="98"/>
+      <c r="T20" s="98"/>
+      <c r="U20" s="98"/>
+      <c r="V20" s="98"/>
+      <c r="W20" s="98"/>
+      <c r="X20" s="98"/>
+      <c r="Y20" s="98"/>
+      <c r="Z20" s="98"/>
+      <c r="AA20" s="98"/>
+      <c r="AB20" s="98"/>
+      <c r="AC20" s="98"/>
+      <c r="AD20" s="98"/>
+      <c r="AE20" s="98"/>
+      <c r="AF20" s="98"/>
+    </row>
+    <row r="21" spans="1:32" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="102" t="s">
         <v>3</v>
       </c>
@@ -4060,8 +4469,25 @@
       <c r="I21" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="P21" s="98"/>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="98"/>
+      <c r="W21" s="98"/>
+      <c r="X21" s="98"/>
+      <c r="Y21" s="98"/>
+      <c r="Z21" s="98"/>
+      <c r="AA21" s="98"/>
+      <c r="AB21" s="98"/>
+      <c r="AC21" s="98"/>
+      <c r="AD21" s="98"/>
+      <c r="AE21" s="98"/>
+      <c r="AF21" s="98"/>
+    </row>
+    <row r="22" spans="1:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="102" t="s">
         <v>7</v>
       </c>
@@ -4089,8 +4515,25 @@
       <c r="I22" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="98"/>
+      <c r="M22" s="98"/>
+      <c r="P22" s="98"/>
+      <c r="S22" s="98"/>
+      <c r="T22" s="98"/>
+      <c r="U22" s="98"/>
+      <c r="V22" s="98"/>
+      <c r="W22" s="98"/>
+      <c r="X22" s="98"/>
+      <c r="Y22" s="98"/>
+      <c r="Z22" s="98"/>
+      <c r="AA22" s="98"/>
+      <c r="AB22" s="98"/>
+      <c r="AC22" s="98"/>
+      <c r="AD22" s="98"/>
+      <c r="AE22" s="98"/>
+      <c r="AF22" s="98"/>
+    </row>
+    <row r="23" spans="1:32" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="102" t="s">
         <v>12</v>
       </c>
@@ -4118,8 +4561,25 @@
       <c r="I23" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="98"/>
+      <c r="M23" s="98"/>
+      <c r="P23" s="98"/>
+      <c r="S23" s="98"/>
+      <c r="T23" s="98"/>
+      <c r="U23" s="98"/>
+      <c r="V23" s="98"/>
+      <c r="W23" s="98"/>
+      <c r="X23" s="98"/>
+      <c r="Y23" s="98"/>
+      <c r="Z23" s="98"/>
+      <c r="AA23" s="98"/>
+      <c r="AB23" s="98"/>
+      <c r="AC23" s="98"/>
+      <c r="AD23" s="98"/>
+      <c r="AE23" s="98"/>
+      <c r="AF23" s="98"/>
+    </row>
+    <row r="24" spans="1:32" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="102" t="s">
         <v>6</v>
       </c>
@@ -4147,8 +4607,25 @@
       <c r="I24" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="98"/>
+      <c r="M24" s="98"/>
+      <c r="P24" s="98"/>
+      <c r="S24" s="98"/>
+      <c r="T24" s="98"/>
+      <c r="U24" s="98"/>
+      <c r="V24" s="98"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="98"/>
+      <c r="Y24" s="98"/>
+      <c r="Z24" s="98"/>
+      <c r="AA24" s="98"/>
+      <c r="AB24" s="98"/>
+      <c r="AC24" s="98"/>
+      <c r="AD24" s="98"/>
+      <c r="AE24" s="98"/>
+      <c r="AF24" s="98"/>
+    </row>
+    <row r="25" spans="1:32" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="102" t="s">
         <v>8</v>
       </c>
@@ -4176,354 +4653,1311 @@
       <c r="I25" s="100" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="102" t="s">
+      <c r="J25" s="98"/>
+      <c r="M25" s="98"/>
+      <c r="P25" s="98"/>
+      <c r="S25" s="98"/>
+      <c r="T25" s="98"/>
+      <c r="U25" s="98"/>
+      <c r="V25" s="98"/>
+      <c r="W25" s="98"/>
+      <c r="X25" s="98"/>
+      <c r="Y25" s="98"/>
+      <c r="Z25" s="98"/>
+      <c r="AA25" s="98"/>
+      <c r="AB25" s="98"/>
+      <c r="AC25" s="98"/>
+      <c r="AD25" s="98"/>
+      <c r="AE25" s="98"/>
+      <c r="AF25" s="98"/>
+    </row>
+    <row r="26" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="100" t="s">
+      <c r="B26" s="151" t="s">
         <v>170</v>
       </c>
-      <c r="C26" s="100" t="s">
+      <c r="C26" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="100" t="s">
+      <c r="D26" s="151" t="s">
         <v>210</v>
       </c>
-      <c r="E26" s="100">
+      <c r="E26" s="151">
         <v>3</v>
       </c>
-      <c r="F26" s="100">
+      <c r="F26" s="151">
         <v>3</v>
       </c>
-      <c r="G26" s="100" t="s">
+      <c r="G26" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="H26" s="100" t="s">
+      <c r="H26" s="151" t="s">
         <v>94</v>
       </c>
-      <c r="I26" s="100" t="s">
+      <c r="I26" s="151" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="102" t="s">
+      <c r="K26" s="146"/>
+      <c r="L26" s="146"/>
+      <c r="N26" s="146"/>
+      <c r="O26" s="146"/>
+      <c r="Q26" s="146"/>
+      <c r="R26" s="146"/>
+    </row>
+    <row r="27" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="149" t="s">
         <v>173</v>
       </c>
-      <c r="B27" s="99" t="s">
+      <c r="B27" s="150" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="100" t="s">
+      <c r="C27" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="100" t="s">
+      <c r="D27" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E27" s="100">
+      <c r="E27" s="151">
         <v>8</v>
       </c>
-      <c r="F27" s="100">
+      <c r="F27" s="151">
         <v>3</v>
       </c>
-      <c r="G27" s="100" t="s">
+      <c r="G27" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H27" s="100" t="s">
+      <c r="H27" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="I27" s="100" t="s">
+      <c r="I27" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="102" t="s">
+      <c r="K27" s="146"/>
+      <c r="L27" s="146"/>
+      <c r="N27" s="146"/>
+      <c r="O27" s="146"/>
+      <c r="Q27" s="146"/>
+      <c r="R27" s="146"/>
+    </row>
+    <row r="28" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="149" t="s">
         <v>174</v>
       </c>
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="151" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="100" t="s">
+      <c r="C28" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="100" t="s">
+      <c r="D28" s="151" t="s">
         <v>211</v>
       </c>
-      <c r="E28" s="100">
+      <c r="E28" s="151">
         <v>13</v>
       </c>
-      <c r="F28" s="100">
+      <c r="F28" s="151">
         <v>3</v>
       </c>
-      <c r="G28" s="100" t="s">
+      <c r="G28" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H28" s="100" t="s">
+      <c r="H28" s="151" t="s">
         <v>95</v>
       </c>
-      <c r="I28" s="100" t="s">
+      <c r="I28" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="102" t="s">
+      <c r="K28" s="146"/>
+      <c r="L28" s="146"/>
+      <c r="N28" s="146"/>
+      <c r="O28" s="146"/>
+      <c r="Q28" s="146"/>
+      <c r="R28" s="146"/>
+    </row>
+    <row r="29" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="149" t="s">
         <v>175</v>
       </c>
-      <c r="B29" s="99" t="s">
+      <c r="B29" s="150" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="100" t="s">
+      <c r="C29" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="100" t="s">
+      <c r="D29" s="151" t="s">
         <v>210</v>
       </c>
-      <c r="E29" s="100">
+      <c r="E29" s="151">
         <v>5</v>
       </c>
-      <c r="F29" s="100">
+      <c r="F29" s="151">
         <v>3</v>
       </c>
-      <c r="G29" s="100" t="s">
+      <c r="G29" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H29" s="100" t="s">
+      <c r="H29" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="I29" s="100" t="s">
+      <c r="I29" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="102" t="s">
+      <c r="K29" s="146"/>
+      <c r="L29" s="146"/>
+      <c r="N29" s="146"/>
+      <c r="O29" s="146"/>
+      <c r="Q29" s="146"/>
+      <c r="R29" s="146"/>
+    </row>
+    <row r="30" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="149" t="s">
         <v>196</v>
       </c>
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="151" t="s">
         <v>203</v>
       </c>
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="100" t="s">
+      <c r="D30" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E30" s="100">
+      <c r="E30" s="151">
         <v>8</v>
       </c>
-      <c r="F30" s="100">
+      <c r="F30" s="151">
         <v>3</v>
       </c>
-      <c r="G30" s="100" t="s">
+      <c r="G30" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H30" s="100" t="s">
+      <c r="H30" s="151" t="s">
         <v>94</v>
       </c>
-      <c r="I30" s="100" t="s">
+      <c r="I30" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="102" t="s">
+      <c r="K30" s="146"/>
+      <c r="L30" s="146"/>
+      <c r="N30" s="146"/>
+      <c r="O30" s="146"/>
+      <c r="Q30" s="146"/>
+      <c r="R30" s="146"/>
+    </row>
+    <row r="31" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="149" t="s">
         <v>197</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="151" t="s">
         <v>204</v>
       </c>
-      <c r="C31" s="100" t="s">
+      <c r="C31" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="100" t="s">
+      <c r="D31" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E31" s="100">
+      <c r="E31" s="151">
         <v>8</v>
       </c>
-      <c r="F31" s="100">
+      <c r="F31" s="151">
         <v>3</v>
       </c>
-      <c r="G31" s="100" t="s">
+      <c r="G31" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H31" s="100" t="s">
+      <c r="H31" s="151" t="s">
         <v>125</v>
       </c>
-      <c r="I31" s="100" t="s">
+      <c r="I31" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="102" t="s">
+      <c r="K31" s="146"/>
+      <c r="L31" s="146"/>
+      <c r="N31" s="146"/>
+      <c r="O31" s="146"/>
+      <c r="Q31" s="146"/>
+      <c r="R31" s="146"/>
+    </row>
+    <row r="32" spans="1:32" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="149" t="s">
         <v>198</v>
       </c>
-      <c r="B32" s="100" t="s">
+      <c r="B32" s="151" t="s">
         <v>205</v>
       </c>
-      <c r="C32" s="100" t="s">
+      <c r="C32" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="100" t="s">
+      <c r="D32" s="151" t="s">
         <v>211</v>
       </c>
-      <c r="E32" s="100">
+      <c r="E32" s="151">
         <v>13</v>
       </c>
-      <c r="F32" s="100">
+      <c r="F32" s="151">
         <v>3</v>
       </c>
-      <c r="G32" s="100" t="s">
+      <c r="G32" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H32" s="100" t="s">
+      <c r="H32" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="I32" s="100" t="s">
+      <c r="I32" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="102" t="s">
+      <c r="K32" s="146"/>
+      <c r="L32" s="146"/>
+      <c r="N32" s="146"/>
+      <c r="O32" s="146"/>
+      <c r="Q32" s="146"/>
+      <c r="R32" s="146"/>
+    </row>
+    <row r="33" spans="1:20" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="149" t="s">
         <v>199</v>
       </c>
-      <c r="B33" s="100" t="s">
+      <c r="B33" s="151" t="s">
         <v>206</v>
       </c>
-      <c r="C33" s="100" t="s">
+      <c r="C33" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="100" t="s">
+      <c r="D33" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="E33" s="100">
+      <c r="E33" s="151">
         <v>8</v>
       </c>
-      <c r="F33" s="100">
+      <c r="F33" s="151">
         <v>3</v>
       </c>
-      <c r="G33" s="100" t="s">
+      <c r="G33" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H33" s="100" t="s">
+      <c r="H33" s="151" t="s">
         <v>115</v>
       </c>
-      <c r="I33" s="100" t="s">
+      <c r="I33" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="102" t="s">
+      <c r="K33" s="146"/>
+      <c r="L33" s="146"/>
+      <c r="N33" s="146"/>
+      <c r="O33" s="146"/>
+      <c r="Q33" s="146"/>
+      <c r="R33" s="146"/>
+    </row>
+    <row r="34" spans="1:20" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="149" t="s">
         <v>200</v>
       </c>
-      <c r="B34" s="100" t="s">
+      <c r="B34" s="151" t="s">
         <v>207</v>
       </c>
-      <c r="C34" s="100" t="s">
+      <c r="C34" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="151" t="s">
         <v>211</v>
       </c>
-      <c r="E34" s="100">
+      <c r="E34" s="151">
         <v>13</v>
       </c>
-      <c r="F34" s="100">
+      <c r="F34" s="151">
         <v>3</v>
       </c>
-      <c r="G34" s="100" t="s">
+      <c r="G34" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H34" s="100" t="s">
+      <c r="H34" s="151" t="s">
         <v>94</v>
       </c>
-      <c r="I34" s="100" t="s">
+      <c r="I34" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="102" t="s">
+      <c r="K34" s="146"/>
+      <c r="L34" s="146"/>
+      <c r="N34" s="146"/>
+      <c r="O34" s="146"/>
+      <c r="Q34" s="146"/>
+      <c r="R34" s="146"/>
+    </row>
+    <row r="35" spans="1:20" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="149" t="s">
         <v>213</v>
       </c>
-      <c r="B35" s="100" t="s">
+      <c r="B35" s="151" t="s">
         <v>208</v>
       </c>
-      <c r="C35" s="100" t="s">
+      <c r="C35" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="100" t="s">
+      <c r="D35" s="151" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="100">
+      <c r="E35" s="151">
         <v>21</v>
       </c>
-      <c r="F35" s="100">
+      <c r="F35" s="151">
         <v>3</v>
       </c>
-      <c r="G35" s="100" t="s">
+      <c r="G35" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H35" s="100" t="s">
+      <c r="H35" s="151" t="s">
         <v>115</v>
       </c>
-      <c r="I35" s="100" t="s">
+      <c r="I35" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="102" t="s">
+      <c r="K35" s="146"/>
+      <c r="L35" s="146"/>
+      <c r="N35" s="146"/>
+      <c r="O35" s="146"/>
+      <c r="Q35" s="146"/>
+      <c r="R35" s="146"/>
+    </row>
+    <row r="36" spans="1:20" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="149" t="s">
         <v>201</v>
       </c>
-      <c r="B36" s="100" t="s">
+      <c r="B36" s="151" t="s">
         <v>209</v>
       </c>
-      <c r="C36" s="100" t="s">
+      <c r="C36" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D36" s="100" t="s">
+      <c r="D36" s="151" t="s">
         <v>211</v>
       </c>
-      <c r="E36" s="100">
+      <c r="E36" s="151">
         <v>21</v>
       </c>
-      <c r="F36" s="100">
+      <c r="F36" s="151">
         <v>3</v>
       </c>
-      <c r="G36" s="100" t="s">
+      <c r="G36" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H36" s="100" t="s">
+      <c r="H36" s="151" t="s">
         <v>125</v>
       </c>
-      <c r="I36" s="100" t="s">
+      <c r="I36" s="151" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="102" t="s">
+      <c r="K36" s="146"/>
+      <c r="L36" s="146"/>
+      <c r="N36" s="146"/>
+      <c r="O36" s="146"/>
+      <c r="Q36" s="146"/>
+      <c r="R36" s="146"/>
+    </row>
+    <row r="37" spans="1:20" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="149" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="100" t="s">
+      <c r="B37" s="151" t="s">
         <v>214</v>
       </c>
-      <c r="C37" s="100" t="s">
+      <c r="C37" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="123" t="s">
+      <c r="D37" s="152" t="s">
         <v>211</v>
       </c>
-      <c r="E37" s="123">
+      <c r="E37" s="152">
         <v>21</v>
       </c>
-      <c r="F37" s="123">
+      <c r="F37" s="152">
         <v>3</v>
       </c>
-      <c r="G37" s="100" t="s">
+      <c r="G37" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="H37" s="123" t="s">
+      <c r="H37" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="I37" s="100" t="s">
+      <c r="I37" s="151" t="s">
         <v>241</v>
       </c>
+      <c r="K37" s="146"/>
+      <c r="L37" s="146"/>
+      <c r="N37" s="146"/>
+      <c r="O37" s="146"/>
+      <c r="Q37" s="146"/>
+      <c r="R37" s="146"/>
+    </row>
+    <row r="38" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="144"/>
+      <c r="B38" s="145"/>
+      <c r="C38" s="145"/>
+      <c r="G38" s="145"/>
+      <c r="T38" s="153"/>
+    </row>
+    <row r="39" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="144"/>
+      <c r="B39" s="145"/>
+      <c r="C39" s="145"/>
+      <c r="G39" s="145"/>
+      <c r="T39" s="153"/>
+    </row>
+    <row r="40" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="144"/>
+      <c r="B40" s="145"/>
+      <c r="C40" s="145"/>
+      <c r="G40" s="145"/>
+      <c r="T40" s="153"/>
+    </row>
+    <row r="41" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="144"/>
+      <c r="B41" s="145"/>
+      <c r="C41" s="145"/>
+      <c r="G41" s="145"/>
+      <c r="T41" s="153"/>
+    </row>
+    <row r="42" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="144"/>
+      <c r="B42" s="145"/>
+      <c r="C42" s="145"/>
+      <c r="G42" s="145"/>
+      <c r="T42" s="153"/>
+    </row>
+    <row r="43" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="144"/>
+      <c r="B43" s="145"/>
+      <c r="C43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="T43" s="153"/>
+    </row>
+    <row r="44" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="144"/>
+      <c r="B44" s="145"/>
+      <c r="C44" s="145"/>
+      <c r="G44" s="145"/>
+      <c r="T44" s="153"/>
+    </row>
+    <row r="45" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="144"/>
+      <c r="B45" s="145"/>
+      <c r="C45" s="145"/>
+      <c r="G45" s="145"/>
+      <c r="T45" s="153"/>
+    </row>
+    <row r="46" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="144"/>
+      <c r="B46" s="145"/>
+      <c r="C46" s="145"/>
+      <c r="G46" s="145"/>
+      <c r="T46" s="153"/>
+    </row>
+    <row r="47" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="144"/>
+      <c r="B47" s="145"/>
+      <c r="C47" s="145"/>
+      <c r="G47" s="145"/>
+      <c r="T47" s="153"/>
+    </row>
+    <row r="48" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="144"/>
+      <c r="B48" s="145"/>
+      <c r="C48" s="145"/>
+      <c r="G48" s="145"/>
+      <c r="T48" s="153"/>
+    </row>
+    <row r="49" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="144"/>
+      <c r="B49" s="145"/>
+      <c r="C49" s="145"/>
+      <c r="G49" s="145"/>
+      <c r="T49" s="153"/>
+    </row>
+    <row r="50" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="144"/>
+      <c r="B50" s="145"/>
+      <c r="C50" s="145"/>
+      <c r="G50" s="145"/>
+      <c r="T50" s="153"/>
+    </row>
+    <row r="51" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="144"/>
+      <c r="B51" s="145"/>
+      <c r="C51" s="145"/>
+      <c r="G51" s="145"/>
+      <c r="T51" s="153"/>
+    </row>
+    <row r="52" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="144"/>
+      <c r="B52" s="145"/>
+      <c r="C52" s="145"/>
+      <c r="G52" s="145"/>
+      <c r="T52" s="153"/>
+    </row>
+    <row r="53" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="144"/>
+      <c r="B53" s="145"/>
+      <c r="C53" s="145"/>
+      <c r="G53" s="145"/>
+      <c r="T53" s="153"/>
+    </row>
+    <row r="54" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="144"/>
+      <c r="B54" s="145"/>
+      <c r="C54" s="145"/>
+      <c r="G54" s="145"/>
+      <c r="T54" s="153"/>
+    </row>
+    <row r="55" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="144"/>
+      <c r="B55" s="145"/>
+      <c r="C55" s="145"/>
+      <c r="G55" s="145"/>
+      <c r="T55" s="153"/>
+    </row>
+    <row r="56" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="144"/>
+      <c r="B56" s="145"/>
+      <c r="C56" s="145"/>
+      <c r="G56" s="145"/>
+      <c r="T56" s="153"/>
+    </row>
+    <row r="57" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="144"/>
+      <c r="B57" s="145"/>
+      <c r="C57" s="145"/>
+      <c r="G57" s="145"/>
+      <c r="T57" s="153"/>
+    </row>
+    <row r="58" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="144"/>
+      <c r="B58" s="145"/>
+      <c r="C58" s="145"/>
+      <c r="G58" s="145"/>
+      <c r="T58" s="153"/>
+    </row>
+    <row r="59" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="144"/>
+      <c r="B59" s="145"/>
+      <c r="C59" s="145"/>
+      <c r="G59" s="145"/>
+      <c r="T59" s="153"/>
+    </row>
+    <row r="60" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="144"/>
+      <c r="B60" s="145"/>
+      <c r="C60" s="145"/>
+      <c r="G60" s="145"/>
+      <c r="T60" s="153"/>
+    </row>
+    <row r="61" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="144"/>
+      <c r="B61" s="145"/>
+      <c r="C61" s="145"/>
+      <c r="G61" s="145"/>
+      <c r="T61" s="153"/>
+    </row>
+    <row r="62" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="144"/>
+      <c r="B62" s="145"/>
+      <c r="C62" s="145"/>
+      <c r="G62" s="145"/>
+      <c r="T62" s="153"/>
+    </row>
+    <row r="63" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="144"/>
+      <c r="B63" s="145"/>
+      <c r="C63" s="145"/>
+      <c r="G63" s="145"/>
+      <c r="T63" s="153"/>
+    </row>
+    <row r="64" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="144"/>
+      <c r="B64" s="145"/>
+      <c r="C64" s="145"/>
+      <c r="G64" s="145"/>
+      <c r="T64" s="153"/>
+    </row>
+    <row r="65" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="144"/>
+      <c r="B65" s="145"/>
+      <c r="C65" s="145"/>
+      <c r="G65" s="145"/>
+      <c r="T65" s="153"/>
+    </row>
+    <row r="66" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="144"/>
+      <c r="B66" s="145"/>
+      <c r="C66" s="145"/>
+      <c r="G66" s="145"/>
+      <c r="T66" s="153"/>
+    </row>
+    <row r="67" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="144"/>
+      <c r="B67" s="145"/>
+      <c r="C67" s="145"/>
+      <c r="G67" s="145"/>
+      <c r="T67" s="153"/>
+    </row>
+    <row r="68" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="144"/>
+      <c r="B68" s="145"/>
+      <c r="C68" s="145"/>
+      <c r="G68" s="145"/>
+      <c r="T68" s="153"/>
+    </row>
+    <row r="69" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="144"/>
+      <c r="B69" s="145"/>
+      <c r="C69" s="145"/>
+      <c r="G69" s="145"/>
+      <c r="T69" s="153"/>
+    </row>
+    <row r="70" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="144"/>
+      <c r="B70" s="145"/>
+      <c r="C70" s="145"/>
+      <c r="G70" s="145"/>
+      <c r="T70" s="153"/>
+    </row>
+    <row r="71" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="144"/>
+      <c r="B71" s="145"/>
+      <c r="C71" s="145"/>
+      <c r="G71" s="145"/>
+      <c r="T71" s="153"/>
+    </row>
+    <row r="72" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="144"/>
+      <c r="B72" s="145"/>
+      <c r="C72" s="145"/>
+      <c r="G72" s="145"/>
+      <c r="T72" s="153"/>
+    </row>
+    <row r="73" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="144"/>
+      <c r="B73" s="145"/>
+      <c r="C73" s="145"/>
+      <c r="G73" s="145"/>
+      <c r="T73" s="153"/>
+    </row>
+    <row r="74" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="144"/>
+      <c r="B74" s="145"/>
+      <c r="C74" s="145"/>
+      <c r="G74" s="145"/>
+      <c r="T74" s="153"/>
+    </row>
+    <row r="75" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="144"/>
+      <c r="B75" s="145"/>
+      <c r="C75" s="145"/>
+      <c r="G75" s="145"/>
+      <c r="T75" s="153"/>
+    </row>
+    <row r="76" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="144"/>
+      <c r="B76" s="145"/>
+      <c r="C76" s="145"/>
+      <c r="G76" s="145"/>
+      <c r="T76" s="153"/>
+    </row>
+    <row r="77" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="144"/>
+      <c r="B77" s="145"/>
+      <c r="C77" s="145"/>
+      <c r="G77" s="145"/>
+      <c r="T77" s="153"/>
+    </row>
+    <row r="78" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="144"/>
+      <c r="B78" s="145"/>
+      <c r="C78" s="145"/>
+      <c r="G78" s="145"/>
+      <c r="T78" s="153"/>
+    </row>
+    <row r="79" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="144"/>
+      <c r="B79" s="145"/>
+      <c r="C79" s="145"/>
+      <c r="G79" s="145"/>
+      <c r="T79" s="153"/>
+    </row>
+    <row r="80" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="144"/>
+      <c r="B80" s="145"/>
+      <c r="C80" s="145"/>
+      <c r="G80" s="145"/>
+      <c r="T80" s="153"/>
+    </row>
+    <row r="81" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="144"/>
+      <c r="B81" s="145"/>
+      <c r="C81" s="145"/>
+      <c r="G81" s="145"/>
+      <c r="T81" s="153"/>
+    </row>
+    <row r="82" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="144"/>
+      <c r="B82" s="145"/>
+      <c r="C82" s="145"/>
+      <c r="G82" s="145"/>
+      <c r="T82" s="153"/>
+    </row>
+    <row r="83" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="144"/>
+      <c r="B83" s="145"/>
+      <c r="C83" s="145"/>
+      <c r="G83" s="145"/>
+      <c r="T83" s="153"/>
+    </row>
+    <row r="84" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="144"/>
+      <c r="B84" s="145"/>
+      <c r="C84" s="145"/>
+      <c r="G84" s="145"/>
+      <c r="T84" s="153"/>
+    </row>
+    <row r="85" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="144"/>
+      <c r="B85" s="145"/>
+      <c r="C85" s="145"/>
+      <c r="G85" s="145"/>
+      <c r="T85" s="153"/>
+    </row>
+    <row r="86" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="144"/>
+      <c r="B86" s="145"/>
+      <c r="C86" s="145"/>
+      <c r="G86" s="145"/>
+      <c r="T86" s="153"/>
+    </row>
+    <row r="87" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="144"/>
+      <c r="B87" s="145"/>
+      <c r="C87" s="145"/>
+      <c r="G87" s="145"/>
+      <c r="T87" s="153"/>
+    </row>
+    <row r="88" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="144"/>
+      <c r="B88" s="145"/>
+      <c r="C88" s="145"/>
+      <c r="G88" s="145"/>
+      <c r="T88" s="153"/>
+    </row>
+    <row r="89" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="144"/>
+      <c r="B89" s="145"/>
+      <c r="C89" s="145"/>
+      <c r="G89" s="145"/>
+      <c r="T89" s="153"/>
+    </row>
+    <row r="90" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="144"/>
+      <c r="B90" s="145"/>
+      <c r="C90" s="145"/>
+      <c r="G90" s="145"/>
+      <c r="T90" s="153"/>
+    </row>
+    <row r="91" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="144"/>
+      <c r="B91" s="145"/>
+      <c r="C91" s="145"/>
+      <c r="G91" s="145"/>
+      <c r="T91" s="153"/>
+    </row>
+    <row r="92" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="144"/>
+      <c r="B92" s="145"/>
+      <c r="C92" s="145"/>
+      <c r="G92" s="145"/>
+      <c r="T92" s="153"/>
+    </row>
+    <row r="93" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="144"/>
+      <c r="B93" s="145"/>
+      <c r="C93" s="145"/>
+      <c r="G93" s="145"/>
+      <c r="T93" s="153"/>
+    </row>
+    <row r="94" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="144"/>
+      <c r="B94" s="145"/>
+      <c r="C94" s="145"/>
+      <c r="G94" s="145"/>
+      <c r="T94" s="153"/>
+    </row>
+    <row r="95" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="144"/>
+      <c r="B95" s="145"/>
+      <c r="C95" s="145"/>
+      <c r="G95" s="145"/>
+      <c r="T95" s="153"/>
+    </row>
+    <row r="96" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="144"/>
+      <c r="B96" s="145"/>
+      <c r="C96" s="145"/>
+      <c r="G96" s="145"/>
+      <c r="T96" s="153"/>
+    </row>
+    <row r="97" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="144"/>
+      <c r="B97" s="145"/>
+      <c r="C97" s="145"/>
+      <c r="G97" s="145"/>
+      <c r="T97" s="153"/>
+    </row>
+    <row r="98" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="144"/>
+      <c r="B98" s="145"/>
+      <c r="C98" s="145"/>
+      <c r="G98" s="145"/>
+      <c r="T98" s="153"/>
+    </row>
+    <row r="99" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="144"/>
+      <c r="B99" s="145"/>
+      <c r="C99" s="145"/>
+      <c r="G99" s="145"/>
+      <c r="T99" s="153"/>
+    </row>
+    <row r="100" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="144"/>
+      <c r="B100" s="145"/>
+      <c r="C100" s="145"/>
+      <c r="G100" s="145"/>
+      <c r="T100" s="153"/>
+    </row>
+    <row r="101" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="144"/>
+      <c r="B101" s="145"/>
+      <c r="C101" s="145"/>
+      <c r="G101" s="145"/>
+      <c r="T101" s="153"/>
+    </row>
+    <row r="102" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="144"/>
+      <c r="B102" s="145"/>
+      <c r="C102" s="145"/>
+      <c r="G102" s="145"/>
+      <c r="T102" s="153"/>
+    </row>
+    <row r="103" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="144"/>
+      <c r="B103" s="145"/>
+      <c r="C103" s="145"/>
+      <c r="G103" s="145"/>
+      <c r="T103" s="153"/>
+    </row>
+    <row r="104" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="144"/>
+      <c r="B104" s="145"/>
+      <c r="C104" s="145"/>
+      <c r="G104" s="145"/>
+      <c r="T104" s="153"/>
+    </row>
+    <row r="105" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="144"/>
+      <c r="B105" s="145"/>
+      <c r="C105" s="145"/>
+      <c r="G105" s="145"/>
+      <c r="T105" s="153"/>
+    </row>
+    <row r="106" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="144"/>
+      <c r="B106" s="145"/>
+      <c r="C106" s="145"/>
+      <c r="G106" s="145"/>
+      <c r="T106" s="153"/>
+    </row>
+    <row r="107" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="144"/>
+      <c r="B107" s="145"/>
+      <c r="C107" s="145"/>
+      <c r="G107" s="145"/>
+      <c r="T107" s="153"/>
+    </row>
+    <row r="108" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="144"/>
+      <c r="B108" s="145"/>
+      <c r="C108" s="145"/>
+      <c r="G108" s="145"/>
+      <c r="T108" s="153"/>
+    </row>
+    <row r="109" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="144"/>
+      <c r="B109" s="145"/>
+      <c r="C109" s="145"/>
+      <c r="G109" s="145"/>
+      <c r="T109" s="153"/>
+    </row>
+    <row r="110" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="144"/>
+      <c r="B110" s="145"/>
+      <c r="C110" s="145"/>
+      <c r="G110" s="145"/>
+      <c r="T110" s="153"/>
+    </row>
+    <row r="111" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="144"/>
+      <c r="B111" s="145"/>
+      <c r="C111" s="145"/>
+      <c r="G111" s="145"/>
+      <c r="T111" s="153"/>
+    </row>
+    <row r="112" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="144"/>
+      <c r="B112" s="145"/>
+      <c r="C112" s="145"/>
+      <c r="G112" s="145"/>
+      <c r="T112" s="153"/>
+    </row>
+    <row r="113" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="144"/>
+      <c r="B113" s="145"/>
+      <c r="C113" s="145"/>
+      <c r="G113" s="145"/>
+      <c r="T113" s="153"/>
+    </row>
+    <row r="114" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="144"/>
+      <c r="B114" s="145"/>
+      <c r="C114" s="145"/>
+      <c r="G114" s="145"/>
+      <c r="T114" s="153"/>
+    </row>
+    <row r="115" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="144"/>
+      <c r="B115" s="145"/>
+      <c r="C115" s="145"/>
+      <c r="G115" s="145"/>
+      <c r="T115" s="153"/>
+    </row>
+    <row r="116" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="144"/>
+      <c r="B116" s="145"/>
+      <c r="C116" s="145"/>
+      <c r="G116" s="145"/>
+      <c r="T116" s="153"/>
+    </row>
+    <row r="117" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="144"/>
+      <c r="B117" s="145"/>
+      <c r="C117" s="145"/>
+      <c r="G117" s="145"/>
+      <c r="T117" s="153"/>
+    </row>
+    <row r="118" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="144"/>
+      <c r="B118" s="145"/>
+      <c r="C118" s="145"/>
+      <c r="G118" s="145"/>
+      <c r="T118" s="153"/>
+    </row>
+    <row r="119" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="144"/>
+      <c r="B119" s="145"/>
+      <c r="C119" s="145"/>
+      <c r="G119" s="145"/>
+      <c r="T119" s="153"/>
+    </row>
+    <row r="120" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="144"/>
+      <c r="B120" s="145"/>
+      <c r="C120" s="145"/>
+      <c r="G120" s="145"/>
+      <c r="T120" s="153"/>
+    </row>
+    <row r="121" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="144"/>
+      <c r="B121" s="145"/>
+      <c r="C121" s="145"/>
+      <c r="G121" s="145"/>
+      <c r="T121" s="153"/>
+    </row>
+    <row r="122" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="144"/>
+      <c r="B122" s="145"/>
+      <c r="C122" s="145"/>
+      <c r="G122" s="145"/>
+      <c r="T122" s="153"/>
+    </row>
+    <row r="123" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="144"/>
+      <c r="B123" s="145"/>
+      <c r="C123" s="145"/>
+      <c r="G123" s="145"/>
+      <c r="T123" s="153"/>
+    </row>
+    <row r="124" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="144"/>
+      <c r="B124" s="145"/>
+      <c r="C124" s="145"/>
+      <c r="G124" s="145"/>
+      <c r="T124" s="153"/>
+    </row>
+    <row r="125" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="144"/>
+      <c r="B125" s="145"/>
+      <c r="C125" s="145"/>
+      <c r="G125" s="145"/>
+      <c r="T125" s="153"/>
+    </row>
+    <row r="126" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="144"/>
+      <c r="B126" s="145"/>
+      <c r="C126" s="145"/>
+      <c r="G126" s="145"/>
+      <c r="T126" s="153"/>
+    </row>
+    <row r="127" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="144"/>
+      <c r="B127" s="145"/>
+      <c r="C127" s="145"/>
+      <c r="G127" s="145"/>
+      <c r="T127" s="153"/>
+    </row>
+    <row r="128" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="144"/>
+      <c r="B128" s="145"/>
+      <c r="C128" s="145"/>
+      <c r="G128" s="145"/>
+      <c r="T128" s="153"/>
+    </row>
+    <row r="129" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="144"/>
+      <c r="B129" s="145"/>
+      <c r="C129" s="145"/>
+      <c r="G129" s="145"/>
+      <c r="T129" s="153"/>
+    </row>
+    <row r="130" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="144"/>
+      <c r="B130" s="145"/>
+      <c r="C130" s="145"/>
+      <c r="G130" s="145"/>
+      <c r="T130" s="153"/>
+    </row>
+    <row r="131" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="144"/>
+      <c r="B131" s="145"/>
+      <c r="C131" s="145"/>
+      <c r="G131" s="145"/>
+      <c r="T131" s="153"/>
+    </row>
+    <row r="132" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="144"/>
+      <c r="B132" s="145"/>
+      <c r="C132" s="145"/>
+      <c r="G132" s="145"/>
+      <c r="T132" s="153"/>
+    </row>
+    <row r="133" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="144"/>
+      <c r="B133" s="145"/>
+      <c r="C133" s="145"/>
+      <c r="G133" s="145"/>
+      <c r="T133" s="153"/>
+    </row>
+    <row r="134" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="144"/>
+      <c r="B134" s="145"/>
+      <c r="C134" s="145"/>
+      <c r="G134" s="145"/>
+      <c r="T134" s="153"/>
+    </row>
+    <row r="135" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="144"/>
+      <c r="B135" s="145"/>
+      <c r="C135" s="145"/>
+      <c r="G135" s="145"/>
+      <c r="T135" s="153"/>
+    </row>
+    <row r="136" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="144"/>
+      <c r="B136" s="145"/>
+      <c r="C136" s="145"/>
+      <c r="G136" s="145"/>
+      <c r="T136" s="153"/>
+    </row>
+    <row r="137" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="144"/>
+      <c r="B137" s="145"/>
+      <c r="C137" s="145"/>
+      <c r="G137" s="145"/>
+      <c r="T137" s="153"/>
+    </row>
+    <row r="138" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="144"/>
+      <c r="B138" s="145"/>
+      <c r="C138" s="145"/>
+      <c r="G138" s="145"/>
+      <c r="T138" s="153"/>
+    </row>
+    <row r="139" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="144"/>
+      <c r="B139" s="145"/>
+      <c r="C139" s="145"/>
+      <c r="G139" s="145"/>
+      <c r="T139" s="153"/>
+    </row>
+    <row r="140" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="144"/>
+      <c r="B140" s="145"/>
+      <c r="C140" s="145"/>
+      <c r="G140" s="145"/>
+      <c r="T140" s="153"/>
+    </row>
+    <row r="141" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="144"/>
+      <c r="B141" s="145"/>
+      <c r="C141" s="145"/>
+      <c r="G141" s="145"/>
+      <c r="T141" s="153"/>
+    </row>
+    <row r="142" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="144"/>
+      <c r="B142" s="145"/>
+      <c r="C142" s="145"/>
+      <c r="G142" s="145"/>
+      <c r="T142" s="153"/>
+    </row>
+    <row r="143" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="144"/>
+      <c r="B143" s="145"/>
+      <c r="C143" s="145"/>
+      <c r="G143" s="145"/>
+      <c r="T143" s="153"/>
+    </row>
+    <row r="144" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="144"/>
+      <c r="B144" s="145"/>
+      <c r="C144" s="145"/>
+      <c r="G144" s="145"/>
+      <c r="T144" s="153"/>
+    </row>
+    <row r="145" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="144"/>
+      <c r="B145" s="145"/>
+      <c r="C145" s="145"/>
+      <c r="G145" s="145"/>
+      <c r="T145" s="153"/>
+    </row>
+    <row r="146" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="144"/>
+      <c r="B146" s="145"/>
+      <c r="C146" s="145"/>
+      <c r="G146" s="145"/>
+      <c r="T146" s="153"/>
+    </row>
+    <row r="147" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="144"/>
+      <c r="B147" s="145"/>
+      <c r="C147" s="145"/>
+      <c r="G147" s="145"/>
+      <c r="T147" s="153"/>
+    </row>
+    <row r="148" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="144"/>
+      <c r="B148" s="145"/>
+      <c r="C148" s="145"/>
+      <c r="G148" s="145"/>
+      <c r="T148" s="153"/>
+    </row>
+    <row r="149" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="144"/>
+      <c r="B149" s="145"/>
+      <c r="C149" s="145"/>
+      <c r="G149" s="145"/>
+      <c r="T149" s="153"/>
+    </row>
+    <row r="150" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="144"/>
+      <c r="B150" s="145"/>
+      <c r="C150" s="145"/>
+      <c r="G150" s="145"/>
+      <c r="T150" s="153"/>
+    </row>
+    <row r="151" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="144"/>
+      <c r="B151" s="145"/>
+      <c r="C151" s="145"/>
+      <c r="G151" s="145"/>
+      <c r="T151" s="153"/>
+    </row>
+    <row r="152" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="144"/>
+      <c r="B152" s="145"/>
+      <c r="C152" s="145"/>
+      <c r="G152" s="145"/>
+      <c r="T152" s="153"/>
+    </row>
+    <row r="153" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="144"/>
+      <c r="B153" s="145"/>
+      <c r="C153" s="145"/>
+      <c r="G153" s="145"/>
+      <c r="T153" s="153"/>
+    </row>
+    <row r="154" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="144"/>
+      <c r="B154" s="145"/>
+      <c r="C154" s="145"/>
+      <c r="G154" s="145"/>
+      <c r="T154" s="153"/>
+    </row>
+    <row r="155" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="144"/>
+      <c r="B155" s="145"/>
+      <c r="C155" s="145"/>
+      <c r="G155" s="145"/>
+      <c r="T155" s="153"/>
+    </row>
+    <row r="156" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="144"/>
+      <c r="B156" s="145"/>
+      <c r="C156" s="145"/>
+      <c r="G156" s="145"/>
+      <c r="T156" s="153"/>
+    </row>
+    <row r="157" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="144"/>
+      <c r="B157" s="145"/>
+      <c r="C157" s="145"/>
+      <c r="G157" s="145"/>
+      <c r="T157" s="153"/>
+    </row>
+    <row r="158" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="144"/>
+      <c r="B158" s="145"/>
+      <c r="C158" s="145"/>
+      <c r="G158" s="145"/>
+      <c r="T158" s="153"/>
+    </row>
+    <row r="159" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="144"/>
+      <c r="B159" s="145"/>
+      <c r="C159" s="145"/>
+      <c r="G159" s="145"/>
+      <c r="T159" s="153"/>
+    </row>
+    <row r="160" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="144"/>
+      <c r="B160" s="145"/>
+      <c r="C160" s="145"/>
+      <c r="G160" s="145"/>
+      <c r="T160" s="153"/>
+    </row>
+    <row r="161" spans="1:20" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="144"/>
+      <c r="B161" s="145"/>
+      <c r="C161" s="145"/>
+      <c r="G161" s="145"/>
+      <c r="T161" s="153"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:I37" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
@@ -4547,13 +5981,13 @@
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="D2:I2 C2:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"ESSENCIAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"IMPORTANTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"DESEJÁVEL"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4604,7 +6038,7 @@
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="134" t="s">
+      <c r="G1" s="128" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4627,7 +6061,7 @@
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="134"/>
+      <c r="G2" s="128"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -4653,71 +6087,71 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="125" t="s">
+      <c r="E4" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="126" t="s">
+      <c r="G4" s="123" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="125" t="s">
+      <c r="D5" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="125" t="s">
+      <c r="E5" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="125" t="s">
+      <c r="F5" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="126" t="s">
+      <c r="G5" s="123" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="125" t="s">
+      <c r="E6" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="126" t="s">
+      <c r="G6" s="123" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4957,13 +6391,13 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G17">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Em execução">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="Em execução">
       <formula>NOT(ISERROR(SEARCH("Em execução",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Não iniciado">
+    <cfRule type="containsText" dxfId="36" priority="2" operator="containsText" text="Não iniciado">
       <formula>NOT(ISERROR(SEARCH("Não iniciado",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4980,7 +6414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="B1:R104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
@@ -5008,88 +6442,88 @@
   <sheetData>
     <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="137"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="135" t="s">
+      <c r="H2" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
-      <c r="N2" s="135" t="s">
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="133"/>
+      <c r="N2" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
-      <c r="R2" s="137"/>
+      <c r="O2" s="132"/>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="132"/>
+      <c r="R2" s="133"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="141">
+      <c r="C3" s="134">
         <v>45554</v>
       </c>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="142"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="135"/>
       <c r="G3" s="5"/>
       <c r="H3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="134">
         <v>45555</v>
       </c>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="142"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="135"/>
       <c r="N3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="141">
+      <c r="O3" s="134">
         <v>45557</v>
       </c>
-      <c r="P3" s="141"/>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="142"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="135"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="149"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="141"/>
       <c r="G4" s="6"/>
       <c r="H4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="148" t="s">
+      <c r="I4" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="141"/>
       <c r="N4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="148" t="s">
+      <c r="O4" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="148"/>
-      <c r="R4" s="149"/>
+      <c r="P4" s="140"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="141"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
@@ -5220,22 +6654,22 @@
       <c r="R10" s="22"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="139"/>
-      <c r="D11" s="139" t="s">
+      <c r="C11" s="130"/>
+      <c r="D11" s="130" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="139"/>
+      <c r="E11" s="130"/>
       <c r="F11" s="24" t="s">
         <v>88</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="138" t="s">
+      <c r="H11" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="139"/>
+      <c r="I11" s="130"/>
       <c r="J11" s="26" t="s">
         <v>87</v>
       </c>
@@ -5243,10 +6677,10 @@
       <c r="L11" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="N11" s="138" t="s">
+      <c r="N11" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="O11" s="139"/>
+      <c r="O11" s="130"/>
       <c r="P11" s="42" t="s">
         <v>87</v>
       </c>
@@ -5258,22 +6692,22 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140" t="s">
+      <c r="C12" s="139"/>
+      <c r="D12" s="139" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="140"/>
+      <c r="E12" s="139"/>
       <c r="F12" s="16">
         <v>45560</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="147"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="140"/>
-      <c r="K12" s="140"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="139"/>
       <c r="L12" s="16"/>
       <c r="N12" s="49" t="s">
         <v>89</v>
@@ -5290,22 +6724,22 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="138" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140" t="s">
+      <c r="C13" s="139"/>
+      <c r="D13" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="140"/>
+      <c r="E13" s="139"/>
       <c r="F13" s="16">
         <v>45560</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="147"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="140"/>
-      <c r="K13" s="140"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="139"/>
       <c r="L13" s="16"/>
       <c r="N13" s="45" t="s">
         <v>90</v>
@@ -5322,22 +6756,22 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="147" t="s">
+      <c r="B14" s="138" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="140"/>
-      <c r="D14" s="140" t="s">
+      <c r="C14" s="139"/>
+      <c r="D14" s="139" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="140"/>
+      <c r="E14" s="139"/>
       <c r="F14" s="16">
         <v>45560</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="147"/>
-      <c r="I14" s="140"/>
-      <c r="J14" s="140"/>
-      <c r="K14" s="140"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="139"/>
       <c r="L14" s="16"/>
       <c r="N14" s="45" t="s">
         <v>91</v>
@@ -5354,7 +6788,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="142" t="s">
         <v>93</v>
       </c>
       <c r="C15" s="143"/>
@@ -5365,7 +6799,7 @@
       <c r="F15" s="19">
         <v>45560</v>
       </c>
-      <c r="H15" s="144"/>
+      <c r="H15" s="142"/>
       <c r="I15" s="143"/>
       <c r="J15" s="143"/>
       <c r="K15" s="143"/>
@@ -5397,85 +6831,85 @@
       <c r="R16" s="67"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="135" t="s">
+      <c r="B17" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="136"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="137"/>
-      <c r="H17" s="135" t="s">
+      <c r="C17" s="132"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="133"/>
+      <c r="H17" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="137"/>
-      <c r="N17" s="135" t="s">
+      <c r="I17" s="132"/>
+      <c r="J17" s="132"/>
+      <c r="K17" s="132"/>
+      <c r="L17" s="133"/>
+      <c r="N17" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="O17" s="136"/>
-      <c r="P17" s="136"/>
-      <c r="Q17" s="136"/>
-      <c r="R17" s="137"/>
+      <c r="O17" s="132"/>
+      <c r="P17" s="132"/>
+      <c r="Q17" s="132"/>
+      <c r="R17" s="133"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="141">
+      <c r="C18" s="134">
         <v>45558</v>
       </c>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="142"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="135"/>
       <c r="H18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="141">
+      <c r="I18" s="134">
         <v>45559</v>
       </c>
-      <c r="J18" s="141"/>
-      <c r="K18" s="141"/>
-      <c r="L18" s="142"/>
+      <c r="J18" s="134"/>
+      <c r="K18" s="134"/>
+      <c r="L18" s="135"/>
       <c r="N18" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="O18" s="141">
+      <c r="O18" s="134">
         <v>45560</v>
       </c>
-      <c r="P18" s="141"/>
-      <c r="Q18" s="141"/>
-      <c r="R18" s="142"/>
+      <c r="P18" s="134"/>
+      <c r="Q18" s="134"/>
+      <c r="R18" s="135"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="145" t="s">
+      <c r="C19" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="145"/>
-      <c r="E19" s="145"/>
-      <c r="F19" s="146"/>
+      <c r="D19" s="136"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="137"/>
       <c r="H19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="145" t="s">
+      <c r="I19" s="136" t="s">
         <v>117</v>
       </c>
-      <c r="J19" s="145"/>
-      <c r="K19" s="145"/>
-      <c r="L19" s="146"/>
+      <c r="J19" s="136"/>
+      <c r="K19" s="136"/>
+      <c r="L19" s="137"/>
       <c r="N19" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="O19" s="145" t="s">
+      <c r="O19" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="P19" s="145"/>
-      <c r="Q19" s="145"/>
-      <c r="R19" s="146"/>
+      <c r="P19" s="136"/>
+      <c r="Q19" s="136"/>
+      <c r="R19" s="137"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
@@ -5625,10 +7059,10 @@
       <c r="R26" s="22"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="138" t="s">
+      <c r="B27" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="139"/>
+      <c r="C27" s="130"/>
       <c r="D27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5638,10 +7072,10 @@
       <c r="F27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="138" t="s">
+      <c r="H27" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="139"/>
+      <c r="I27" s="130"/>
       <c r="J27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5651,10 +7085,10 @@
       <c r="L27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N27" s="138" t="s">
+      <c r="N27" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="O27" s="139"/>
+      <c r="O27" s="130"/>
       <c r="P27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5855,27 +7289,27 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="135" t="s">
+      <c r="B35" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="136"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="136"/>
-      <c r="F35" s="137"/>
-      <c r="H35" s="135" t="s">
+      <c r="C35" s="132"/>
+      <c r="D35" s="132"/>
+      <c r="E35" s="132"/>
+      <c r="F35" s="133"/>
+      <c r="H35" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="I35" s="136"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="136"/>
-      <c r="L35" s="137"/>
-      <c r="N35" s="135" t="s">
+      <c r="I35" s="132"/>
+      <c r="J35" s="132"/>
+      <c r="K35" s="132"/>
+      <c r="L35" s="133"/>
+      <c r="N35" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="O35" s="136"/>
-      <c r="P35" s="136"/>
-      <c r="Q35" s="136"/>
-      <c r="R35" s="137"/>
+      <c r="O35" s="132"/>
+      <c r="P35" s="132"/>
+      <c r="Q35" s="132"/>
+      <c r="R35" s="133"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
@@ -5890,12 +7324,12 @@
       <c r="H36" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="141">
+      <c r="I36" s="134">
         <v>45562</v>
       </c>
-      <c r="J36" s="141"/>
-      <c r="K36" s="141"/>
-      <c r="L36" s="142"/>
+      <c r="J36" s="134"/>
+      <c r="K36" s="134"/>
+      <c r="L36" s="135"/>
       <c r="N36" s="75" t="s">
         <v>78</v>
       </c>
@@ -5919,12 +7353,12 @@
       <c r="H37" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I37" s="145" t="s">
+      <c r="I37" s="136" t="s">
         <v>184</v>
       </c>
-      <c r="J37" s="145"/>
-      <c r="K37" s="145"/>
-      <c r="L37" s="146"/>
+      <c r="J37" s="136"/>
+      <c r="K37" s="136"/>
+      <c r="L37" s="137"/>
       <c r="N37" s="78" t="s">
         <v>79</v>
       </c>
@@ -6079,10 +7513,10 @@
       <c r="R44" s="22"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="138" t="s">
+      <c r="B45" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="139"/>
+      <c r="C45" s="130"/>
       <c r="D45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6092,10 +7526,10 @@
       <c r="F45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="138" t="s">
+      <c r="H45" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="139"/>
+      <c r="I45" s="130"/>
       <c r="J45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6105,10 +7539,10 @@
       <c r="L45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="138" t="s">
+      <c r="N45" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="O45" s="139"/>
+      <c r="O45" s="130"/>
       <c r="P45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6325,27 +7759,27 @@
       </c>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B53" s="135" t="s">
+      <c r="B53" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="136"/>
-      <c r="D53" s="136"/>
-      <c r="E53" s="136"/>
-      <c r="F53" s="137"/>
-      <c r="H53" s="135" t="s">
+      <c r="C53" s="132"/>
+      <c r="D53" s="132"/>
+      <c r="E53" s="132"/>
+      <c r="F53" s="133"/>
+      <c r="H53" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
-      <c r="K53" s="136"/>
-      <c r="L53" s="137"/>
-      <c r="N53" s="135" t="s">
+      <c r="I53" s="132"/>
+      <c r="J53" s="132"/>
+      <c r="K53" s="132"/>
+      <c r="L53" s="133"/>
+      <c r="N53" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="O53" s="136"/>
-      <c r="P53" s="136"/>
-      <c r="Q53" s="136"/>
-      <c r="R53" s="137"/>
+      <c r="O53" s="132"/>
+      <c r="P53" s="132"/>
+      <c r="Q53" s="132"/>
+      <c r="R53" s="133"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="s">
@@ -6453,20 +7887,20 @@
       <c r="D58" s="27"/>
       <c r="E58" s="27"/>
       <c r="F58" s="28"/>
-      <c r="H58" s="116" t="s">
+      <c r="H58" s="115" t="s">
         <v>219</v>
       </c>
-      <c r="I58" s="117"/>
-      <c r="J58" s="117"/>
-      <c r="K58" s="117"/>
-      <c r="L58" s="118"/>
-      <c r="N58" s="116" t="s">
+      <c r="I58" s="116"/>
+      <c r="J58" s="116"/>
+      <c r="K58" s="116"/>
+      <c r="L58" s="117"/>
+      <c r="N58" s="115" t="s">
         <v>226</v>
       </c>
-      <c r="O58" s="117"/>
-      <c r="P58" s="117"/>
-      <c r="Q58" s="117"/>
-      <c r="R58" s="118"/>
+      <c r="O58" s="116"/>
+      <c r="P58" s="116"/>
+      <c r="Q58" s="116"/>
+      <c r="R58" s="117"/>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B59" s="13" t="s">
@@ -6476,20 +7910,20 @@
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="15"/>
-      <c r="H59" s="115" t="s">
+      <c r="H59" s="114" t="s">
         <v>220</v>
       </c>
-      <c r="I59" s="119"/>
-      <c r="J59" s="119"/>
-      <c r="K59" s="119"/>
-      <c r="L59" s="120"/>
-      <c r="N59" s="115" t="s">
+      <c r="I59" s="118"/>
+      <c r="J59" s="118"/>
+      <c r="K59" s="118"/>
+      <c r="L59" s="119"/>
+      <c r="N59" s="114" t="s">
         <v>225</v>
       </c>
-      <c r="O59" s="119"/>
-      <c r="P59" s="119"/>
-      <c r="Q59" s="119"/>
-      <c r="R59" s="120"/>
+      <c r="O59" s="118"/>
+      <c r="P59" s="118"/>
+      <c r="Q59" s="118"/>
+      <c r="R59" s="119"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B60" s="13" t="s">
@@ -6499,12 +7933,12 @@
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="15"/>
-      <c r="H60" s="121"/>
+      <c r="H60" s="120"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
       <c r="K60" s="14"/>
       <c r="L60" s="15"/>
-      <c r="N60" s="121" t="s">
+      <c r="N60" s="120" t="s">
         <v>223</v>
       </c>
       <c r="O60" s="14"/>
@@ -6557,10 +7991,10 @@
       <c r="R62" s="22"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="138" t="s">
+      <c r="B63" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="139"/>
+      <c r="C63" s="130"/>
       <c r="D63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6570,10 +8004,10 @@
       <c r="F63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H63" s="138" t="s">
+      <c r="H63" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="I63" s="139"/>
+      <c r="I63" s="130"/>
       <c r="J63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6583,10 +8017,10 @@
       <c r="L63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N63" s="138" t="s">
+      <c r="N63" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="O63" s="139"/>
+      <c r="O63" s="130"/>
       <c r="P63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6816,42 +8250,42 @@
       <c r="F69" s="74">
         <v>45571</v>
       </c>
-      <c r="H69" s="112" t="s">
+      <c r="H69" s="111" t="s">
         <v>195</v>
       </c>
-      <c r="I69" s="113"/>
-      <c r="J69" s="113" t="s">
+      <c r="I69" s="112"/>
+      <c r="J69" s="112" t="s">
         <v>126</v>
       </c>
-      <c r="K69" s="113" t="s">
+      <c r="K69" s="112" t="s">
         <v>238</v>
       </c>
-      <c r="L69" s="114">
+      <c r="L69" s="113">
         <v>45572</v>
       </c>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B71" s="135" t="s">
+      <c r="B71" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="136"/>
-      <c r="D71" s="136"/>
-      <c r="E71" s="136"/>
-      <c r="F71" s="137"/>
-      <c r="H71" s="135" t="s">
+      <c r="C71" s="132"/>
+      <c r="D71" s="132"/>
+      <c r="E71" s="132"/>
+      <c r="F71" s="133"/>
+      <c r="H71" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="I71" s="136"/>
-      <c r="J71" s="136"/>
-      <c r="K71" s="136"/>
-      <c r="L71" s="137"/>
-      <c r="N71" s="135" t="s">
+      <c r="I71" s="132"/>
+      <c r="J71" s="132"/>
+      <c r="K71" s="132"/>
+      <c r="L71" s="133"/>
+      <c r="N71" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="O71" s="136"/>
-      <c r="P71" s="136"/>
-      <c r="Q71" s="136"/>
-      <c r="R71" s="137"/>
+      <c r="O71" s="132"/>
+      <c r="P71" s="132"/>
+      <c r="Q71" s="132"/>
+      <c r="R71" s="133"/>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B72" s="8" t="s">
@@ -6952,67 +8386,67 @@
       <c r="R75" s="22"/>
     </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B76" s="116" t="s">
+      <c r="B76" s="115" t="s">
         <v>228</v>
       </c>
-      <c r="C76" s="117"/>
-      <c r="D76" s="117"/>
-      <c r="E76" s="117"/>
-      <c r="F76" s="118"/>
-      <c r="H76" s="116" t="s">
+      <c r="C76" s="116"/>
+      <c r="D76" s="116"/>
+      <c r="E76" s="116"/>
+      <c r="F76" s="117"/>
+      <c r="H76" s="115" t="s">
         <v>243</v>
       </c>
-      <c r="I76" s="117"/>
-      <c r="J76" s="117"/>
-      <c r="K76" s="117"/>
-      <c r="L76" s="118"/>
-      <c r="N76" s="116" t="s">
+      <c r="I76" s="116"/>
+      <c r="J76" s="116"/>
+      <c r="K76" s="116"/>
+      <c r="L76" s="117"/>
+      <c r="N76" s="115" t="s">
         <v>250</v>
       </c>
-      <c r="O76" s="117"/>
-      <c r="P76" s="117"/>
-      <c r="Q76" s="117"/>
-      <c r="R76" s="118"/>
+      <c r="O76" s="116"/>
+      <c r="P76" s="116"/>
+      <c r="Q76" s="116"/>
+      <c r="R76" s="117"/>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B77" s="115" t="s">
+      <c r="B77" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="C77" s="119"/>
-      <c r="D77" s="119"/>
-      <c r="E77" s="119"/>
-      <c r="F77" s="120"/>
-      <c r="H77" s="115" t="s">
+      <c r="C77" s="118"/>
+      <c r="D77" s="118"/>
+      <c r="E77" s="118"/>
+      <c r="F77" s="119"/>
+      <c r="H77" s="114" t="s">
         <v>244</v>
       </c>
-      <c r="I77" s="119"/>
-      <c r="J77" s="119"/>
-      <c r="K77" s="119"/>
-      <c r="L77" s="120"/>
-      <c r="N77" s="115" t="s">
+      <c r="I77" s="118"/>
+      <c r="J77" s="118"/>
+      <c r="K77" s="118"/>
+      <c r="L77" s="119"/>
+      <c r="N77" s="114" t="s">
         <v>251</v>
       </c>
-      <c r="O77" s="119"/>
-      <c r="P77" s="119"/>
-      <c r="Q77" s="119"/>
-      <c r="R77" s="120"/>
+      <c r="O77" s="118"/>
+      <c r="P77" s="118"/>
+      <c r="Q77" s="118"/>
+      <c r="R77" s="119"/>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B78" s="121" t="s">
+      <c r="B78" s="120" t="s">
         <v>230</v>
       </c>
       <c r="C78" s="14"/>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="15"/>
-      <c r="H78" s="121" t="s">
+      <c r="H78" s="120" t="s">
         <v>245</v>
       </c>
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
       <c r="K78" s="14"/>
       <c r="L78" s="15"/>
-      <c r="N78" s="121"/>
+      <c r="N78" s="120"/>
       <c r="O78" s="14"/>
       <c r="P78" s="14"/>
       <c r="Q78" s="14"/>
@@ -7059,10 +8493,10 @@
       <c r="R80" s="22"/>
     </row>
     <row r="81" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B81" s="138" t="s">
+      <c r="B81" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="C81" s="139"/>
+      <c r="C81" s="130"/>
       <c r="D81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7072,10 +8506,10 @@
       <c r="F81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H81" s="138" t="s">
+      <c r="H81" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="I81" s="139"/>
+      <c r="I81" s="130"/>
       <c r="J81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7085,10 +8519,10 @@
       <c r="L81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N81" s="138" t="s">
+      <c r="N81" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="O81" s="139"/>
+      <c r="O81" s="130"/>
       <c r="P81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7292,13 +8726,13 @@
       </c>
     </row>
     <row r="87" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B87" s="135" t="s">
+      <c r="B87" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="C87" s="136"/>
-      <c r="D87" s="136"/>
-      <c r="E87" s="136"/>
-      <c r="F87" s="137"/>
+      <c r="C87" s="132"/>
+      <c r="D87" s="132"/>
+      <c r="E87" s="132"/>
+      <c r="F87" s="133"/>
     </row>
     <row r="88" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B88" s="8" t="s">
@@ -7339,25 +8773,25 @@
       <c r="F91" s="22"/>
     </row>
     <row r="92" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B92" s="116" t="s">
+      <c r="B92" s="115" t="s">
         <v>256</v>
       </c>
-      <c r="C92" s="117"/>
-      <c r="D92" s="117"/>
-      <c r="E92" s="117"/>
-      <c r="F92" s="118"/>
+      <c r="C92" s="116"/>
+      <c r="D92" s="116"/>
+      <c r="E92" s="116"/>
+      <c r="F92" s="117"/>
     </row>
     <row r="93" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B93" s="115" t="s">
+      <c r="B93" s="114" t="s">
         <v>257</v>
       </c>
-      <c r="C93" s="119"/>
-      <c r="D93" s="119"/>
-      <c r="E93" s="119"/>
-      <c r="F93" s="120"/>
+      <c r="C93" s="118"/>
+      <c r="D93" s="118"/>
+      <c r="E93" s="118"/>
+      <c r="F93" s="119"/>
     </row>
     <row r="94" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B94" s="121"/>
+      <c r="B94" s="120"/>
       <c r="C94" s="14"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
@@ -7380,10 +8814,10 @@
       <c r="F96" s="22"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="138" t="s">
+      <c r="B97" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="C97" s="139"/>
+      <c r="C97" s="130"/>
       <c r="D97" s="42" t="s">
         <v>87</v>
       </c>
@@ -7395,7 +8829,7 @@
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B98" s="127" t="s">
+      <c r="B98" s="124" t="s">
         <v>121</v>
       </c>
       <c r="C98" s="63"/>
@@ -7425,7 +8859,7 @@
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B100" s="127" t="s">
+      <c r="B100" s="124" t="s">
         <v>194</v>
       </c>
       <c r="C100" s="63"/>
@@ -7440,7 +8874,7 @@
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B101" s="127" t="s">
+      <c r="B101" s="124" t="s">
         <v>193</v>
       </c>
       <c r="C101" s="63"/>
@@ -7455,7 +8889,7 @@
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B102" s="127" t="s">
+      <c r="B102" s="124" t="s">
         <v>246</v>
       </c>
       <c r="C102" s="63"/>
@@ -7501,15 +8935,44 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="H53:L53"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="N71:R71"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="N53:R53"/>
+    <mergeCell ref="N63:O63"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="N35:R35"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
@@ -7526,44 +8989,15 @@
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="H71:L71"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="N53:R53"/>
-    <mergeCell ref="N63:O63"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="N35:R35"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="N71:R71"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="H53:L53"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="I37:L37"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Docs novas e atualização da ata
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3539E-7497-49D0-8751-3239EC06FC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E768B258-1E11-4E84-92F6-7E5E6FFDC642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="260">
   <si>
     <t>Requisito</t>
   </si>
@@ -963,6 +963,12 @@
   </si>
   <si>
     <t>ponderamos ideias sobre o projeto em geral e revisamos dificuldades do grupo em geral.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Finalizamos a maioria das atividades propostas pela equipe e deixamos </t>
+  </si>
+  <si>
+    <t>a resolução final da dahsboard para a semana do dia 13</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1654,6 +1660,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1690,27 +1699,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1719,6 +1728,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3346,17 +3361,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="132"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="133"/>
     </row>
     <row r="2" spans="1:18" s="122" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="124" t="s">
@@ -3416,18 +3431,18 @@
       <c r="I3" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="133" t="s">
+      <c r="K3" s="134" t="s">
         <v>217</v>
       </c>
-      <c r="L3" s="133"/>
-      <c r="N3" s="133" t="s">
+      <c r="L3" s="134"/>
+      <c r="N3" s="134" t="s">
         <v>218</v>
       </c>
-      <c r="O3" s="133"/>
-      <c r="Q3" s="133" t="s">
+      <c r="O3" s="134"/>
+      <c r="Q3" s="134" t="s">
         <v>232</v>
       </c>
-      <c r="R3" s="133"/>
+      <c r="R3" s="134"/>
     </row>
     <row r="4" spans="1:18" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="102" t="s">
@@ -3471,10 +3486,10 @@
         <f>SUM(O5:O7)</f>
         <v>154</v>
       </c>
-      <c r="Q4" s="128" t="s">
+      <c r="Q4" s="129" t="s">
         <v>233</v>
       </c>
-      <c r="R4" s="129"/>
+      <c r="R4" s="130"/>
     </row>
     <row r="5" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="102" t="s">
@@ -3518,10 +3533,10 @@
         <f>SUM(E15:E26)</f>
         <v>88</v>
       </c>
-      <c r="Q5" s="128" t="s">
+      <c r="Q5" s="129" t="s">
         <v>234</v>
       </c>
-      <c r="R5" s="129"/>
+      <c r="R5" s="130"/>
     </row>
     <row r="6" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="102" t="s">
@@ -3565,10 +3580,10 @@
         <f>SUM(E3,E6,E8,E12,E13)</f>
         <v>66</v>
       </c>
-      <c r="Q6" s="128" t="s">
+      <c r="Q6" s="129" t="s">
         <v>235</v>
       </c>
-      <c r="R6" s="129"/>
+      <c r="R6" s="130"/>
     </row>
     <row r="7" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="102" t="s">
@@ -3611,10 +3626,10 @@
       <c r="O7" s="108">
         <v>0</v>
       </c>
-      <c r="Q7" s="128" t="s">
+      <c r="Q7" s="129" t="s">
         <v>236</v>
       </c>
-      <c r="R7" s="129"/>
+      <c r="R7" s="130"/>
     </row>
     <row r="8" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="102" t="s">
@@ -3656,10 +3671,10 @@
       <c r="O8" s="108">
         <v>0</v>
       </c>
-      <c r="Q8" s="128" t="s">
+      <c r="Q8" s="129" t="s">
         <v>237</v>
       </c>
-      <c r="R8" s="129"/>
+      <c r="R8" s="130"/>
     </row>
     <row r="9" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="102" t="s">
@@ -4604,7 +4619,7 @@
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="134" t="s">
+      <c r="G1" s="135" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4627,7 +4642,7 @@
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="134"/>
+      <c r="G2" s="135"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -4978,10 +4993,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
-  <dimension ref="B1:R104"/>
+  <dimension ref="B1:R105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4991,10 +5006,10 @@
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
     <col min="7" max="7" width="3.5546875" customWidth="1"/>
     <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" customWidth="1"/>
     <col min="11" max="11" width="17.5546875" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" customWidth="1"/>
@@ -5008,28 +5023,28 @@
   <sheetData>
     <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="138"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="135" t="s">
+      <c r="H2" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
-      <c r="N2" s="135" t="s">
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
+      <c r="L2" s="138"/>
+      <c r="N2" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
-      <c r="R2" s="137"/>
+      <c r="O2" s="137"/>
+      <c r="P2" s="137"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="138"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -5065,31 +5080,31 @@
       <c r="B4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="149" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="149"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="150"/>
       <c r="G4" s="6"/>
       <c r="H4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="148" t="s">
+      <c r="I4" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="149"/>
+      <c r="K4" s="149"/>
+      <c r="L4" s="150"/>
       <c r="N4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="148" t="s">
+      <c r="O4" s="149" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="148"/>
-      <c r="R4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
+      <c r="R4" s="150"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
@@ -5220,22 +5235,22 @@
       <c r="R10" s="22"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="139"/>
-      <c r="D11" s="139" t="s">
+      <c r="C11" s="140"/>
+      <c r="D11" s="140" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="139"/>
+      <c r="E11" s="140"/>
       <c r="F11" s="24" t="s">
         <v>88</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="138" t="s">
+      <c r="H11" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="139"/>
+      <c r="I11" s="140"/>
       <c r="J11" s="26" t="s">
         <v>87</v>
       </c>
@@ -5243,10 +5258,10 @@
       <c r="L11" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="N11" s="138" t="s">
+      <c r="N11" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="O11" s="139"/>
+      <c r="O11" s="140"/>
       <c r="P11" s="42" t="s">
         <v>87</v>
       </c>
@@ -5258,22 +5273,22 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="148" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140" t="s">
+      <c r="C12" s="147"/>
+      <c r="D12" s="147" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="140"/>
+      <c r="E12" s="147"/>
       <c r="F12" s="16">
         <v>45560</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="147"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="140"/>
-      <c r="K12" s="140"/>
+      <c r="H12" s="148"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="147"/>
+      <c r="K12" s="147"/>
       <c r="L12" s="16"/>
       <c r="N12" s="49" t="s">
         <v>89</v>
@@ -5290,22 +5305,22 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140" t="s">
+      <c r="C13" s="147"/>
+      <c r="D13" s="147" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="140"/>
+      <c r="E13" s="147"/>
       <c r="F13" s="16">
         <v>45560</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="147"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="140"/>
-      <c r="K13" s="140"/>
+      <c r="H13" s="148"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="147"/>
+      <c r="K13" s="147"/>
       <c r="L13" s="16"/>
       <c r="N13" s="45" t="s">
         <v>90</v>
@@ -5322,22 +5337,22 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="147" t="s">
+      <c r="B14" s="148" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="140"/>
-      <c r="D14" s="140" t="s">
+      <c r="C14" s="147"/>
+      <c r="D14" s="147" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="140"/>
+      <c r="E14" s="147"/>
       <c r="F14" s="16">
         <v>45560</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="147"/>
-      <c r="I14" s="140"/>
-      <c r="J14" s="140"/>
-      <c r="K14" s="140"/>
+      <c r="H14" s="148"/>
+      <c r="I14" s="147"/>
+      <c r="J14" s="147"/>
+      <c r="K14" s="147"/>
       <c r="L14" s="16"/>
       <c r="N14" s="45" t="s">
         <v>91</v>
@@ -5397,27 +5412,27 @@
       <c r="R16" s="67"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="135" t="s">
+      <c r="B17" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="136"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="137"/>
-      <c r="H17" s="135" t="s">
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="138"/>
+      <c r="H17" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="137"/>
-      <c r="N17" s="135" t="s">
+      <c r="I17" s="137"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="137"/>
+      <c r="L17" s="138"/>
+      <c r="N17" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="O17" s="136"/>
-      <c r="P17" s="136"/>
-      <c r="Q17" s="136"/>
-      <c r="R17" s="137"/>
+      <c r="O17" s="137"/>
+      <c r="P17" s="137"/>
+      <c r="Q17" s="137"/>
+      <c r="R17" s="138"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
@@ -5625,10 +5640,10 @@
       <c r="R26" s="22"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="138" t="s">
+      <c r="B27" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="139"/>
+      <c r="C27" s="140"/>
       <c r="D27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5638,10 +5653,10 @@
       <c r="F27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="138" t="s">
+      <c r="H27" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="139"/>
+      <c r="I27" s="140"/>
       <c r="J27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5651,10 +5666,10 @@
       <c r="L27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N27" s="138" t="s">
+      <c r="N27" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="O27" s="139"/>
+      <c r="O27" s="140"/>
       <c r="P27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5855,27 +5870,27 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="135" t="s">
+      <c r="B35" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="136"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="136"/>
-      <c r="F35" s="137"/>
-      <c r="H35" s="135" t="s">
+      <c r="C35" s="137"/>
+      <c r="D35" s="137"/>
+      <c r="E35" s="137"/>
+      <c r="F35" s="138"/>
+      <c r="H35" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="I35" s="136"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="136"/>
-      <c r="L35" s="137"/>
-      <c r="N35" s="135" t="s">
+      <c r="I35" s="137"/>
+      <c r="J35" s="137"/>
+      <c r="K35" s="137"/>
+      <c r="L35" s="138"/>
+      <c r="N35" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="O35" s="136"/>
-      <c r="P35" s="136"/>
-      <c r="Q35" s="136"/>
-      <c r="R35" s="137"/>
+      <c r="O35" s="137"/>
+      <c r="P35" s="137"/>
+      <c r="Q35" s="137"/>
+      <c r="R35" s="138"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
@@ -6079,10 +6094,10 @@
       <c r="R44" s="22"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="138" t="s">
+      <c r="B45" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="139"/>
+      <c r="C45" s="140"/>
       <c r="D45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6092,10 +6107,10 @@
       <c r="F45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="138" t="s">
+      <c r="H45" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="139"/>
+      <c r="I45" s="140"/>
       <c r="J45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6105,10 +6120,10 @@
       <c r="L45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="138" t="s">
+      <c r="N45" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="O45" s="139"/>
+      <c r="O45" s="140"/>
       <c r="P45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6325,27 +6340,27 @@
       </c>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B53" s="135" t="s">
+      <c r="B53" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="136"/>
-      <c r="D53" s="136"/>
-      <c r="E53" s="136"/>
-      <c r="F53" s="137"/>
-      <c r="H53" s="135" t="s">
+      <c r="C53" s="137"/>
+      <c r="D53" s="137"/>
+      <c r="E53" s="137"/>
+      <c r="F53" s="138"/>
+      <c r="H53" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
-      <c r="K53" s="136"/>
-      <c r="L53" s="137"/>
-      <c r="N53" s="135" t="s">
+      <c r="I53" s="137"/>
+      <c r="J53" s="137"/>
+      <c r="K53" s="137"/>
+      <c r="L53" s="138"/>
+      <c r="N53" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="O53" s="136"/>
-      <c r="P53" s="136"/>
-      <c r="Q53" s="136"/>
-      <c r="R53" s="137"/>
+      <c r="O53" s="137"/>
+      <c r="P53" s="137"/>
+      <c r="Q53" s="137"/>
+      <c r="R53" s="138"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="s">
@@ -6557,10 +6572,10 @@
       <c r="R62" s="22"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="138" t="s">
+      <c r="B63" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="139"/>
+      <c r="C63" s="140"/>
       <c r="D63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6570,10 +6585,10 @@
       <c r="F63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H63" s="138" t="s">
+      <c r="H63" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="I63" s="139"/>
+      <c r="I63" s="140"/>
       <c r="J63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6583,10 +6598,10 @@
       <c r="L63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N63" s="138" t="s">
+      <c r="N63" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="O63" s="139"/>
+      <c r="O63" s="140"/>
       <c r="P63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6831,27 +6846,27 @@
       </c>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B71" s="135" t="s">
+      <c r="B71" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="136"/>
-      <c r="D71" s="136"/>
-      <c r="E71" s="136"/>
-      <c r="F71" s="137"/>
-      <c r="H71" s="135" t="s">
+      <c r="C71" s="137"/>
+      <c r="D71" s="137"/>
+      <c r="E71" s="137"/>
+      <c r="F71" s="138"/>
+      <c r="H71" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="I71" s="136"/>
-      <c r="J71" s="136"/>
-      <c r="K71" s="136"/>
-      <c r="L71" s="137"/>
-      <c r="N71" s="135" t="s">
+      <c r="I71" s="137"/>
+      <c r="J71" s="137"/>
+      <c r="K71" s="137"/>
+      <c r="L71" s="138"/>
+      <c r="N71" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="O71" s="136"/>
-      <c r="P71" s="136"/>
-      <c r="Q71" s="136"/>
-      <c r="R71" s="137"/>
+      <c r="O71" s="137"/>
+      <c r="P71" s="137"/>
+      <c r="Q71" s="137"/>
+      <c r="R71" s="138"/>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B72" s="8" t="s">
@@ -7059,10 +7074,10 @@
       <c r="R80" s="22"/>
     </row>
     <row r="81" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B81" s="138" t="s">
+      <c r="B81" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="C81" s="139"/>
+      <c r="C81" s="140"/>
       <c r="D81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7072,10 +7087,10 @@
       <c r="F81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H81" s="138" t="s">
+      <c r="H81" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="I81" s="139"/>
+      <c r="I81" s="140"/>
       <c r="J81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7085,10 +7100,10 @@
       <c r="L81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N81" s="138" t="s">
+      <c r="N81" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="O81" s="139"/>
+      <c r="O81" s="140"/>
       <c r="P81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7291,161 +7306,253 @@
         <v>45577</v>
       </c>
     </row>
-    <row r="87" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B87" s="135" t="s">
+    <row r="88" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B88" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C87" s="136"/>
-      <c r="D87" s="136"/>
-      <c r="E87" s="136"/>
-      <c r="F87" s="137"/>
-    </row>
-    <row r="88" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B88" s="8" t="s">
+      <c r="C88" s="137"/>
+      <c r="D88" s="137"/>
+      <c r="E88" s="137"/>
+      <c r="F88" s="138"/>
+      <c r="H88" s="136" t="s">
+        <v>77</v>
+      </c>
+      <c r="I88" s="137"/>
+      <c r="J88" s="137"/>
+      <c r="K88" s="137"/>
+      <c r="L88" s="138"/>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B89" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C89" s="9">
         <v>45576</v>
       </c>
-      <c r="D88" s="68"/>
-      <c r="E88" s="68"/>
-      <c r="F88" s="69"/>
-    </row>
-    <row r="89" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B89" s="13" t="s">
+      <c r="D89" s="68"/>
+      <c r="E89" s="68"/>
+      <c r="F89" s="69"/>
+      <c r="H89" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I89" s="9">
+        <v>45578</v>
+      </c>
+      <c r="J89" s="68"/>
+      <c r="K89" s="68"/>
+      <c r="L89" s="69"/>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B90" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C89" s="14" t="s">
+      <c r="C90" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="15"/>
-    </row>
-    <row r="90" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B90" s="10"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="70"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="15"/>
+      <c r="H90" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I90" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="15"/>
     </row>
     <row r="91" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B91" s="20" t="s">
+      <c r="B91" s="10"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="70"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="70"/>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B92" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="22"/>
-    </row>
-    <row r="92" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B92" s="116" t="s">
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="22"/>
+      <c r="H92" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="22"/>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B93" s="116" t="s">
         <v>256</v>
       </c>
-      <c r="C92" s="117"/>
-      <c r="D92" s="117"/>
-      <c r="E92" s="117"/>
-      <c r="F92" s="118"/>
-    </row>
-    <row r="93" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B93" s="115" t="s">
+      <c r="C93" s="117"/>
+      <c r="D93" s="117"/>
+      <c r="E93" s="117"/>
+      <c r="F93" s="118"/>
+      <c r="H93" s="116" t="s">
+        <v>258</v>
+      </c>
+      <c r="I93" s="117"/>
+      <c r="J93" s="117"/>
+      <c r="K93" s="117"/>
+      <c r="L93" s="118"/>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B94" s="115" t="s">
         <v>257</v>
       </c>
-      <c r="C93" s="119"/>
-      <c r="D93" s="119"/>
-      <c r="E93" s="119"/>
-      <c r="F93" s="120"/>
-    </row>
-    <row r="94" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B94" s="121"/>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="15"/>
+      <c r="C94" s="119"/>
+      <c r="D94" s="119"/>
+      <c r="E94" s="119"/>
+      <c r="F94" s="120"/>
+      <c r="H94" s="151" t="s">
+        <v>259</v>
+      </c>
+      <c r="I94" s="152"/>
+      <c r="J94" s="152"/>
+      <c r="K94" s="152"/>
+      <c r="L94" s="120"/>
     </row>
     <row r="95" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B95" s="10"/>
-      <c r="C95" s="29"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="30"/>
+      <c r="B95" s="121"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="15"/>
+      <c r="H95" s="121"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
+      <c r="L95" s="15"/>
     </row>
     <row r="96" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="10"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="30"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
+      <c r="K96" s="29"/>
+      <c r="L96" s="30"/>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B97" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="C96" s="21"/>
-      <c r="D96" s="21"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="22"/>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="138" t="s">
+      <c r="C97" s="21"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="22"/>
+      <c r="H97" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="I97" s="21"/>
+      <c r="J97" s="21"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="22"/>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B98" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="C97" s="139"/>
-      <c r="D97" s="42" t="s">
+      <c r="C98" s="140"/>
+      <c r="D98" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="E97" s="23" t="s">
+      <c r="E98" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="F97" s="24" t="s">
+      <c r="F98" s="24" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B98" s="127" t="s">
+      <c r="H98" s="128" t="s">
+        <v>86</v>
+      </c>
+      <c r="I98" s="23"/>
+      <c r="J98" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="K98" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="L98" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B99" s="127" t="s">
         <v>121</v>
       </c>
-      <c r="C98" s="63"/>
-      <c r="D98" s="63" t="s">
+      <c r="C99" s="63"/>
+      <c r="D99" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="E98" s="63" t="s">
+      <c r="E99" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F98" s="64">
+      <c r="F99" s="64">
         <v>45576</v>
       </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B99" s="87" t="s">
+      <c r="H99" s="127" t="s">
+        <v>121</v>
+      </c>
+      <c r="I99" s="63"/>
+      <c r="J99" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="K99" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="L99" s="64">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B100" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="C99" s="47"/>
-      <c r="D99" s="47" t="s">
+      <c r="C100" s="47"/>
+      <c r="D100" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E99" s="47" t="s">
+      <c r="E100" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="F99" s="48">
+      <c r="F100" s="48">
         <v>45608</v>
       </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B100" s="127" t="s">
+      <c r="H100" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="I100" s="47"/>
+      <c r="J100" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="K100" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="L100" s="48">
+        <v>45610</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B101" s="127" t="s">
         <v>194</v>
-      </c>
-      <c r="C100" s="63"/>
-      <c r="D100" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="E100" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="F100" s="64">
-        <v>45576</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B101" s="127" t="s">
-        <v>193</v>
       </c>
       <c r="C101" s="63"/>
       <c r="D101" s="63" t="s">
-        <v>248</v>
+        <v>95</v>
       </c>
       <c r="E101" s="63" t="s">
         <v>47</v>
@@ -7453,54 +7560,134 @@
       <c r="F101" s="64">
         <v>45576</v>
       </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H101" s="127" t="s">
+        <v>194</v>
+      </c>
+      <c r="I101" s="63"/>
+      <c r="J101" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="K101" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="L101" s="64">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B102" s="127" t="s">
-        <v>246</v>
+        <v>193</v>
       </c>
       <c r="C102" s="63"/>
       <c r="D102" s="63" t="s">
-        <v>116</v>
+        <v>248</v>
       </c>
       <c r="E102" s="63" t="s">
         <v>47</v>
       </c>
       <c r="F102" s="64">
+        <v>45576</v>
+      </c>
+      <c r="H102" s="127" t="s">
+        <v>193</v>
+      </c>
+      <c r="I102" s="63"/>
+      <c r="J102" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="K102" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="L102" s="64">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B103" s="127" t="s">
+        <v>246</v>
+      </c>
+      <c r="C103" s="63"/>
+      <c r="D103" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="E103" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="F103" s="64">
         <v>45577</v>
       </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B103" s="87" t="s">
+      <c r="H103" s="127" t="s">
+        <v>246</v>
+      </c>
+      <c r="I103" s="63"/>
+      <c r="J103" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="K103" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="L103" s="64">
+        <v>45577</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B104" s="87" t="s">
         <v>253</v>
       </c>
-      <c r="C103" s="47"/>
-      <c r="D103" s="47" t="s">
+      <c r="C104" s="47"/>
+      <c r="D104" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="E103" s="47" t="s">
+      <c r="E104" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="F103" s="48">
+      <c r="F104" s="48">
         <v>45577</v>
       </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B104" s="97" t="s">
+      <c r="H104" s="127" t="s">
+        <v>253</v>
+      </c>
+      <c r="I104" s="63"/>
+      <c r="J104" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="K104" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="L104" s="64">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B105" s="97" t="s">
         <v>254</v>
       </c>
-      <c r="C104" s="73"/>
-      <c r="D104" s="73" t="s">
+      <c r="C105" s="73"/>
+      <c r="D105" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="E104" s="73" t="s">
+      <c r="E105" s="73" t="s">
         <v>255</v>
       </c>
-      <c r="F104" s="74">
+      <c r="F105" s="74">
         <v>45578</v>
       </c>
+      <c r="H105" s="81" t="s">
+        <v>254</v>
+      </c>
+      <c r="I105" s="82"/>
+      <c r="J105" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="K105" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="L105" s="83">
+        <v>45578</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="64">
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B35:F35"/>
@@ -7534,6 +7721,7 @@
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H12:I12"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="C18:F18"/>
@@ -7547,9 +7735,6 @@
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="O19:R19"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="H71:L71"/>
-    <mergeCell ref="H81:I81"/>
     <mergeCell ref="N17:R17"/>
     <mergeCell ref="O18:R18"/>
     <mergeCell ref="D15:E15"/>
@@ -7558,12 +7743,15 @@
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="N35:R35"/>
     <mergeCell ref="N45:O45"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="H88:L88"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B98:C98"/>
     <mergeCell ref="N71:R71"/>
     <mergeCell ref="N81:O81"/>
     <mergeCell ref="B71:F71"/>
     <mergeCell ref="B81:C81"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="H81:I81"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da ata de reunião do dia 14/-10-2024
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-diesel-2\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ariel\Downloads\SPTECH 1 SEMETRE ADS\PI\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E768B258-1E11-4E84-92F6-7E5E6FFDC642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A62A63-A041-4459-B81D-5A32AEE60EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="265">
   <si>
     <t>Requisito</t>
   </si>
@@ -969,6 +969,21 @@
   </si>
   <si>
     <t>a resolução final da dahsboard para a semana do dia 13</t>
+  </si>
+  <si>
+    <t>Gustavo ausente</t>
+  </si>
+  <si>
+    <t>* Decidimos iniciar a criação dos sldies para a apresentaçõ do projeto</t>
+  </si>
+  <si>
+    <t>*Ficou decidido também que será feito novas páginas para a dashboard, com os tanques do cliente e alertas</t>
+  </si>
+  <si>
+    <t>Slides</t>
+  </si>
+  <si>
+    <t>* Decidimos datas para encontros durante a semana do fôlego para ensaios</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1663,6 +1678,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1684,6 +1717,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1693,47 +1732,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3338,42 +3365,42 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="75.6640625" style="104" customWidth="1"/>
-    <col min="2" max="2" width="79.5546875" style="103" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" style="103" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" style="98" customWidth="1"/>
+    <col min="1" max="1" width="75.7109375" style="104" customWidth="1"/>
+    <col min="2" max="2" width="79.5703125" style="103" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="103" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="98" customWidth="1"/>
     <col min="5" max="5" width="17" style="98" customWidth="1"/>
     <col min="6" max="6" width="18" style="98" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" style="103" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="98" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="98"/>
-    <col min="11" max="11" width="15.44140625" style="98" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="103" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="98" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="98" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="98"/>
+    <col min="11" max="11" width="15.42578125" style="98" customWidth="1"/>
     <col min="12" max="12" width="13" style="98" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="98"/>
-    <col min="14" max="14" width="15.5546875" style="98" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="98" customWidth="1"/>
-    <col min="16" max="17" width="9.109375" style="98"/>
-    <col min="18" max="18" width="15.6640625" style="98" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="98"/>
+    <col min="13" max="13" width="9.140625" style="98"/>
+    <col min="14" max="14" width="15.5703125" style="98" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="98" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="98"/>
+    <col min="18" max="18" width="15.7109375" style="98" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+    <row r="1" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="137" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="133"/>
-    </row>
-    <row r="2" spans="1:18" s="122" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="139"/>
+    </row>
+    <row r="2" spans="1:18" s="122" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="124" t="s">
         <v>0</v>
       </c>
@@ -3403,7 +3430,7 @@
       </c>
       <c r="M2" s="100"/>
     </row>
-    <row r="3" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>138</v>
       </c>
@@ -3431,20 +3458,20 @@
       <c r="I3" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="134" t="s">
+      <c r="K3" s="140" t="s">
         <v>217</v>
       </c>
-      <c r="L3" s="134"/>
-      <c r="N3" s="134" t="s">
+      <c r="L3" s="140"/>
+      <c r="N3" s="140" t="s">
         <v>218</v>
       </c>
-      <c r="O3" s="134"/>
-      <c r="Q3" s="134" t="s">
+      <c r="O3" s="140"/>
+      <c r="Q3" s="140" t="s">
         <v>232</v>
       </c>
-      <c r="R3" s="134"/>
-    </row>
-    <row r="4" spans="1:18" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="140"/>
+    </row>
+    <row r="4" spans="1:18" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>97</v>
       </c>
@@ -3486,12 +3513,12 @@
         <f>SUM(O5:O7)</f>
         <v>154</v>
       </c>
-      <c r="Q4" s="129" t="s">
+      <c r="Q4" s="135" t="s">
         <v>233</v>
       </c>
-      <c r="R4" s="130"/>
-    </row>
-    <row r="5" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="136"/>
+    </row>
+    <row r="5" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="102" t="s">
         <v>142</v>
       </c>
@@ -3533,12 +3560,12 @@
         <f>SUM(E15:E26)</f>
         <v>88</v>
       </c>
-      <c r="Q5" s="129" t="s">
+      <c r="Q5" s="135" t="s">
         <v>234</v>
       </c>
-      <c r="R5" s="130"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="136"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="102" t="s">
         <v>98</v>
       </c>
@@ -3580,12 +3607,12 @@
         <f>SUM(E3,E6,E8,E12,E13)</f>
         <v>66</v>
       </c>
-      <c r="Q6" s="129" t="s">
+      <c r="Q6" s="135" t="s">
         <v>235</v>
       </c>
-      <c r="R6" s="130"/>
-    </row>
-    <row r="7" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="136"/>
+    </row>
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="102" t="s">
         <v>144</v>
       </c>
@@ -3626,12 +3653,12 @@
       <c r="O7" s="108">
         <v>0</v>
       </c>
-      <c r="Q7" s="129" t="s">
+      <c r="Q7" s="135" t="s">
         <v>236</v>
       </c>
-      <c r="R7" s="130"/>
-    </row>
-    <row r="8" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="136"/>
+    </row>
+    <row r="8" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="102" t="s">
         <v>146</v>
       </c>
@@ -3671,12 +3698,12 @@
       <c r="O8" s="108">
         <v>0</v>
       </c>
-      <c r="Q8" s="129" t="s">
+      <c r="Q8" s="135" t="s">
         <v>237</v>
       </c>
-      <c r="R8" s="130"/>
-    </row>
-    <row r="9" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R8" s="136"/>
+    </row>
+    <row r="9" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="102" t="s">
         <v>148</v>
       </c>
@@ -3720,7 +3747,7 @@
       </c>
       <c r="Q9" s="101"/>
     </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="102" t="s">
         <v>150</v>
       </c>
@@ -3750,7 +3777,7 @@
       </c>
       <c r="Q10" s="101"/>
     </row>
-    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="102" t="s">
         <v>161</v>
       </c>
@@ -3780,7 +3807,7 @@
       </c>
       <c r="Q11" s="101"/>
     </row>
-    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="102" t="s">
         <v>153</v>
       </c>
@@ -3811,7 +3838,7 @@
       <c r="K12" s="111"/>
       <c r="Q12" s="101"/>
     </row>
-    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="102" t="s">
         <v>155</v>
       </c>
@@ -3841,7 +3868,7 @@
       </c>
       <c r="Q13" s="101"/>
     </row>
-    <row r="14" spans="1:18" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="102" t="s">
         <v>157</v>
       </c>
@@ -3871,7 +3898,7 @@
       </c>
       <c r="Q14" s="101"/>
     </row>
-    <row r="15" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="102" t="s">
         <v>134</v>
       </c>
@@ -3901,7 +3928,7 @@
       </c>
       <c r="Q15" s="101"/>
     </row>
-    <row r="16" spans="1:18" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="102" t="s">
         <v>5</v>
       </c>
@@ -3931,7 +3958,7 @@
       </c>
       <c r="Q16" s="101"/>
     </row>
-    <row r="17" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="102" t="s">
         <v>159</v>
       </c>
@@ -3960,7 +3987,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="102" t="s">
         <v>162</v>
       </c>
@@ -3989,7 +4016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="102" t="s">
         <v>10</v>
       </c>
@@ -4018,7 +4045,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="102" t="s">
         <v>11</v>
       </c>
@@ -4047,7 +4074,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="102" t="s">
         <v>3</v>
       </c>
@@ -4076,7 +4103,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="102" t="s">
         <v>7</v>
       </c>
@@ -4105,7 +4132,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="102" t="s">
         <v>12</v>
       </c>
@@ -4134,7 +4161,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="102" t="s">
         <v>6</v>
       </c>
@@ -4163,7 +4190,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="102" t="s">
         <v>8</v>
       </c>
@@ -4192,7 +4219,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="102" t="s">
         <v>9</v>
       </c>
@@ -4221,7 +4248,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="102" t="s">
         <v>173</v>
       </c>
@@ -4250,7 +4277,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="102" t="s">
         <v>174</v>
       </c>
@@ -4279,7 +4306,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="102" t="s">
         <v>175</v>
       </c>
@@ -4308,7 +4335,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="102" t="s">
         <v>196</v>
       </c>
@@ -4337,7 +4364,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="102" t="s">
         <v>197</v>
       </c>
@@ -4366,7 +4393,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="102" t="s">
         <v>198</v>
       </c>
@@ -4395,7 +4422,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="102" t="s">
         <v>199</v>
       </c>
@@ -4424,7 +4451,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="102" t="s">
         <v>200</v>
       </c>
@@ -4453,7 +4480,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="102" t="s">
         <v>213</v>
       </c>
@@ -4482,7 +4509,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="102" t="s">
         <v>201</v>
       </c>
@@ -4511,7 +4538,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="102" t="s">
         <v>202</v>
       </c>
@@ -4594,13 +4621,13 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4619,11 +4646,11 @@
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="135" t="s">
+      <c r="G1" s="141" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -4642,9 +4669,9 @@
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="135"/>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G2" s="141"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -4667,7 +4694,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="125" t="s">
         <v>31</v>
       </c>
@@ -4690,7 +4717,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="125" t="s">
         <v>32</v>
       </c>
@@ -4713,7 +4740,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="125" t="s">
         <v>33</v>
       </c>
@@ -4736,7 +4763,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -4757,7 +4784,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -4778,7 +4805,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -4799,7 +4826,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -4820,7 +4847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -4841,7 +4868,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
@@ -4862,7 +4889,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -4883,7 +4910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
@@ -4904,7 +4931,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -4925,7 +4952,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -4946,7 +4973,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
@@ -4995,118 +5022,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="B1:R105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O92" sqref="O92"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R101" sqref="R101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
-    <col min="7" max="7" width="3.5546875" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="3.33203125" customWidth="1"/>
-    <col min="14" max="14" width="23.6640625" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.28515625" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" customWidth="1"/>
-    <col min="18" max="18" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="136" t="s">
+    <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="138"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="146"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="136" t="s">
+      <c r="H2" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="138"/>
-      <c r="N2" s="136" t="s">
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="146"/>
+      <c r="N2" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="137"/>
-      <c r="P2" s="137"/>
-      <c r="Q2" s="137"/>
-      <c r="R2" s="138"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O2" s="145"/>
+      <c r="P2" s="145"/>
+      <c r="Q2" s="145"/>
+      <c r="R2" s="146"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="141">
+      <c r="C3" s="147">
         <v>45554</v>
       </c>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="142"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="148"/>
       <c r="G3" s="5"/>
       <c r="H3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="147">
         <v>45555</v>
       </c>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="142"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="148"/>
       <c r="N3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="141">
+      <c r="O3" s="147">
         <v>45557</v>
       </c>
-      <c r="P3" s="141"/>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="142"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P3" s="147"/>
+      <c r="Q3" s="147"/>
+      <c r="R3" s="148"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="149" t="s">
+      <c r="C4" s="153" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="149"/>
-      <c r="E4" s="149"/>
-      <c r="F4" s="150"/>
+      <c r="D4" s="153"/>
+      <c r="E4" s="153"/>
+      <c r="F4" s="154"/>
       <c r="G4" s="6"/>
       <c r="H4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="153" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="150"/>
+      <c r="J4" s="153"/>
+      <c r="K4" s="153"/>
+      <c r="L4" s="154"/>
       <c r="N4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="149" t="s">
+      <c r="O4" s="153" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="149"/>
-      <c r="Q4" s="149"/>
-      <c r="R4" s="150"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P4" s="153"/>
+      <c r="Q4" s="153"/>
+      <c r="R4" s="154"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>80</v>
       </c>
@@ -5129,7 +5156,7 @@
       <c r="Q5" s="21"/>
       <c r="R5" s="22"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>83</v>
       </c>
@@ -5152,7 +5179,7 @@
       <c r="Q6" s="27"/>
       <c r="R6" s="28"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>82</v>
       </c>
@@ -5173,7 +5200,7 @@
       <c r="Q7" s="14"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>84</v>
       </c>
@@ -5192,7 +5219,7 @@
       <c r="Q8" s="14"/>
       <c r="R8" s="15"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>85</v>
       </c>
@@ -5211,7 +5238,7 @@
       <c r="Q9" s="29"/>
       <c r="R9" s="30"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>181</v>
       </c>
@@ -5234,23 +5261,23 @@
       <c r="Q10" s="21"/>
       <c r="R10" s="22"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="139" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140" t="s">
+      <c r="C11" s="143"/>
+      <c r="D11" s="143" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="140"/>
+      <c r="E11" s="143"/>
       <c r="F11" s="24" t="s">
         <v>88</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="139" t="s">
+      <c r="H11" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="140"/>
+      <c r="I11" s="143"/>
       <c r="J11" s="26" t="s">
         <v>87</v>
       </c>
@@ -5258,10 +5285,10 @@
       <c r="L11" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="N11" s="139" t="s">
+      <c r="N11" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="O11" s="140"/>
+      <c r="O11" s="143"/>
       <c r="P11" s="42" t="s">
         <v>87</v>
       </c>
@@ -5272,23 +5299,23 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="148" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="147"/>
-      <c r="D12" s="147" t="s">
+      <c r="C12" s="152"/>
+      <c r="D12" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="147"/>
+      <c r="E12" s="152"/>
       <c r="F12" s="16">
         <v>45560</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="147"/>
-      <c r="J12" s="147"/>
-      <c r="K12" s="147"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="152"/>
+      <c r="J12" s="152"/>
+      <c r="K12" s="152"/>
       <c r="L12" s="16"/>
       <c r="N12" s="49" t="s">
         <v>89</v>
@@ -5304,23 +5331,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="148" t="s">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="147"/>
-      <c r="D13" s="147" t="s">
+      <c r="C13" s="152"/>
+      <c r="D13" s="152" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="147"/>
+      <c r="E13" s="152"/>
       <c r="F13" s="16">
         <v>45560</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="148"/>
-      <c r="I13" s="147"/>
-      <c r="J13" s="147"/>
-      <c r="K13" s="147"/>
+      <c r="H13" s="151"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="152"/>
+      <c r="K13" s="152"/>
       <c r="L13" s="16"/>
       <c r="N13" s="45" t="s">
         <v>90</v>
@@ -5336,23 +5363,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="148" t="s">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="147"/>
-      <c r="D14" s="147" t="s">
+      <c r="C14" s="152"/>
+      <c r="D14" s="152" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="147"/>
+      <c r="E14" s="152"/>
       <c r="F14" s="16">
         <v>45560</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="148"/>
-      <c r="I14" s="147"/>
-      <c r="J14" s="147"/>
-      <c r="K14" s="147"/>
+      <c r="H14" s="151"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
       <c r="L14" s="16"/>
       <c r="N14" s="45" t="s">
         <v>91</v>
@@ -5368,22 +5395,22 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="144" t="s">
+    <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="155" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="143"/>
-      <c r="D15" s="143" t="s">
+      <c r="C15" s="156"/>
+      <c r="D15" s="156" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="143"/>
+      <c r="E15" s="156"/>
       <c r="F15" s="19">
         <v>45560</v>
       </c>
-      <c r="H15" s="144"/>
-      <c r="I15" s="143"/>
-      <c r="J15" s="143"/>
-      <c r="K15" s="143"/>
+      <c r="H15" s="155"/>
+      <c r="I15" s="156"/>
+      <c r="J15" s="156"/>
+      <c r="K15" s="156"/>
       <c r="L15" s="19"/>
       <c r="N15" s="84" t="s">
         <v>93</v>
@@ -5399,7 +5426,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -5411,88 +5438,88 @@
       <c r="Q16" s="66"/>
       <c r="R16" s="67"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="136" t="s">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="137"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="138"/>
-      <c r="H17" s="136" t="s">
+      <c r="C17" s="145"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="146"/>
+      <c r="H17" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="137"/>
-      <c r="J17" s="137"/>
-      <c r="K17" s="137"/>
-      <c r="L17" s="138"/>
-      <c r="N17" s="136" t="s">
+      <c r="I17" s="145"/>
+      <c r="J17" s="145"/>
+      <c r="K17" s="145"/>
+      <c r="L17" s="146"/>
+      <c r="N17" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="O17" s="137"/>
-      <c r="P17" s="137"/>
-      <c r="Q17" s="137"/>
-      <c r="R17" s="138"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O17" s="145"/>
+      <c r="P17" s="145"/>
+      <c r="Q17" s="145"/>
+      <c r="R17" s="146"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="141">
+      <c r="C18" s="147">
         <v>45558</v>
       </c>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="142"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="148"/>
       <c r="H18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="141">
+      <c r="I18" s="147">
         <v>45559</v>
       </c>
-      <c r="J18" s="141"/>
-      <c r="K18" s="141"/>
-      <c r="L18" s="142"/>
+      <c r="J18" s="147"/>
+      <c r="K18" s="147"/>
+      <c r="L18" s="148"/>
       <c r="N18" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="O18" s="141">
+      <c r="O18" s="147">
         <v>45560</v>
       </c>
-      <c r="P18" s="141"/>
-      <c r="Q18" s="141"/>
-      <c r="R18" s="142"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P18" s="147"/>
+      <c r="Q18" s="147"/>
+      <c r="R18" s="148"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="145" t="s">
+      <c r="C19" s="149" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="145"/>
-      <c r="E19" s="145"/>
-      <c r="F19" s="146"/>
+      <c r="D19" s="149"/>
+      <c r="E19" s="149"/>
+      <c r="F19" s="150"/>
       <c r="H19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="145" t="s">
+      <c r="I19" s="149" t="s">
         <v>117</v>
       </c>
-      <c r="J19" s="145"/>
-      <c r="K19" s="145"/>
-      <c r="L19" s="146"/>
+      <c r="J19" s="149"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="150"/>
       <c r="N19" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="O19" s="145" t="s">
+      <c r="O19" s="149" t="s">
         <v>81</v>
       </c>
-      <c r="P19" s="145"/>
-      <c r="Q19" s="145"/>
-      <c r="R19" s="146"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P19" s="149"/>
+      <c r="Q19" s="149"/>
+      <c r="R19" s="150"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -5509,7 +5536,7 @@
       <c r="Q20" s="11"/>
       <c r="R20" s="12"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>80</v>
       </c>
@@ -5532,7 +5559,7 @@
       <c r="Q21" s="21"/>
       <c r="R21" s="22"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="33" t="s">
         <v>107</v>
       </c>
@@ -5555,7 +5582,7 @@
       <c r="Q22" s="34"/>
       <c r="R22" s="35"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="36" t="s">
         <v>106</v>
       </c>
@@ -5578,7 +5605,7 @@
       <c r="Q23" s="37"/>
       <c r="R23" s="38"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="36" t="s">
         <v>108</v>
       </c>
@@ -5599,7 +5626,7 @@
       <c r="Q24" s="37"/>
       <c r="R24" s="38"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
@@ -5616,7 +5643,7 @@
       <c r="Q25" s="40"/>
       <c r="R25" s="41"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
         <v>181</v>
       </c>
@@ -5639,11 +5666,11 @@
       <c r="Q26" s="21"/>
       <c r="R26" s="22"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="139" t="s">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="140"/>
+      <c r="C27" s="143"/>
       <c r="D27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5653,10 +5680,10 @@
       <c r="F27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="139" t="s">
+      <c r="H27" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="140"/>
+      <c r="I27" s="143"/>
       <c r="J27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5666,10 +5693,10 @@
       <c r="L27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N27" s="139" t="s">
+      <c r="N27" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="O27" s="140"/>
+      <c r="O27" s="143"/>
       <c r="P27" s="42" t="s">
         <v>87</v>
       </c>
@@ -5680,7 +5707,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="88" t="s">
         <v>109</v>
       </c>
@@ -5721,7 +5748,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="45" t="s">
         <v>90</v>
       </c>
@@ -5762,7 +5789,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="49" t="s">
         <v>111</v>
       </c>
@@ -5803,7 +5830,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="49" t="s">
         <v>114</v>
       </c>
@@ -5844,7 +5871,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="53"/>
       <c r="C32" s="54"/>
       <c r="D32" s="54"/>
@@ -5869,30 +5896,30 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="136" t="s">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="137"/>
-      <c r="D35" s="137"/>
-      <c r="E35" s="137"/>
-      <c r="F35" s="138"/>
-      <c r="H35" s="136" t="s">
+      <c r="C35" s="145"/>
+      <c r="D35" s="145"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="146"/>
+      <c r="H35" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="I35" s="137"/>
-      <c r="J35" s="137"/>
-      <c r="K35" s="137"/>
-      <c r="L35" s="138"/>
-      <c r="N35" s="136" t="s">
+      <c r="I35" s="145"/>
+      <c r="J35" s="145"/>
+      <c r="K35" s="145"/>
+      <c r="L35" s="146"/>
+      <c r="N35" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="O35" s="137"/>
-      <c r="P35" s="137"/>
-      <c r="Q35" s="137"/>
-      <c r="R35" s="138"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O35" s="145"/>
+      <c r="P35" s="145"/>
+      <c r="Q35" s="145"/>
+      <c r="R35" s="146"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>78</v>
       </c>
@@ -5905,12 +5932,12 @@
       <c r="H36" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="141">
+      <c r="I36" s="147">
         <v>45562</v>
       </c>
-      <c r="J36" s="141"/>
-      <c r="K36" s="141"/>
-      <c r="L36" s="142"/>
+      <c r="J36" s="147"/>
+      <c r="K36" s="147"/>
+      <c r="L36" s="148"/>
       <c r="N36" s="75" t="s">
         <v>78</v>
       </c>
@@ -5921,7 +5948,7 @@
       <c r="Q36" s="76"/>
       <c r="R36" s="77"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="13" t="s">
         <v>79</v>
       </c>
@@ -5934,12 +5961,12 @@
       <c r="H37" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I37" s="145" t="s">
+      <c r="I37" s="149" t="s">
         <v>184</v>
       </c>
-      <c r="J37" s="145"/>
-      <c r="K37" s="145"/>
-      <c r="L37" s="146"/>
+      <c r="J37" s="149"/>
+      <c r="K37" s="149"/>
+      <c r="L37" s="150"/>
       <c r="N37" s="78" t="s">
         <v>79</v>
       </c>
@@ -5950,7 +5977,7 @@
       <c r="Q37" s="31"/>
       <c r="R37" s="32"/>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -5967,7 +5994,7 @@
       <c r="Q38" s="29"/>
       <c r="R38" s="30"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="20" t="s">
         <v>80</v>
       </c>
@@ -5990,7 +6017,7 @@
       <c r="Q39" s="21"/>
       <c r="R39" s="22"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>182</v>
       </c>
@@ -6013,7 +6040,7 @@
       <c r="Q40" s="27"/>
       <c r="R40" s="28"/>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
         <v>183</v>
       </c>
@@ -6036,7 +6063,7 @@
       <c r="Q41" s="14"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -6053,7 +6080,7 @@
       <c r="Q42" s="14"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
       <c r="C43" s="29"/>
       <c r="D43" s="29"/>
@@ -6070,7 +6097,7 @@
       <c r="Q43" s="29"/>
       <c r="R43" s="30"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="20" t="s">
         <v>181</v>
       </c>
@@ -6093,11 +6120,11 @@
       <c r="Q44" s="21"/>
       <c r="R44" s="22"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="139" t="s">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="140"/>
+      <c r="C45" s="143"/>
       <c r="D45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6107,10 +6134,10 @@
       <c r="F45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="139" t="s">
+      <c r="H45" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="140"/>
+      <c r="I45" s="143"/>
       <c r="J45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6120,10 +6147,10 @@
       <c r="L45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="139" t="s">
+      <c r="N45" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="O45" s="140"/>
+      <c r="O45" s="143"/>
       <c r="P45" s="42" t="s">
         <v>87</v>
       </c>
@@ -6134,7 +6161,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="86" t="s">
         <v>120</v>
       </c>
@@ -6175,7 +6202,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="87" t="s">
         <v>121</v>
       </c>
@@ -6216,7 +6243,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="80" t="s">
         <v>122</v>
       </c>
@@ -6257,7 +6284,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="80" t="s">
         <v>123</v>
       </c>
@@ -6298,7 +6325,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="90" t="s">
         <v>188</v>
       </c>
@@ -6339,30 +6366,30 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B53" s="136" t="s">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B53" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="137"/>
-      <c r="D53" s="137"/>
-      <c r="E53" s="137"/>
-      <c r="F53" s="138"/>
-      <c r="H53" s="136" t="s">
+      <c r="C53" s="145"/>
+      <c r="D53" s="145"/>
+      <c r="E53" s="145"/>
+      <c r="F53" s="146"/>
+      <c r="H53" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="I53" s="137"/>
-      <c r="J53" s="137"/>
-      <c r="K53" s="137"/>
-      <c r="L53" s="138"/>
-      <c r="N53" s="136" t="s">
+      <c r="I53" s="145"/>
+      <c r="J53" s="145"/>
+      <c r="K53" s="145"/>
+      <c r="L53" s="146"/>
+      <c r="N53" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="O53" s="137"/>
-      <c r="P53" s="137"/>
-      <c r="Q53" s="137"/>
-      <c r="R53" s="138"/>
-    </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O53" s="145"/>
+      <c r="P53" s="145"/>
+      <c r="Q53" s="145"/>
+      <c r="R53" s="146"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>78</v>
       </c>
@@ -6391,7 +6418,7 @@
       <c r="Q54" s="68"/>
       <c r="R54" s="69"/>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" s="13" t="s">
         <v>79</v>
       </c>
@@ -6420,7 +6447,7 @@
       <c r="Q55" s="14"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B56" s="10"/>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -6437,7 +6464,7 @@
       <c r="Q56" s="18"/>
       <c r="R56" s="70"/>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" s="20" t="s">
         <v>80</v>
       </c>
@@ -6460,7 +6487,7 @@
       <c r="Q57" s="21"/>
       <c r="R57" s="22"/>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" s="8" t="s">
         <v>191</v>
       </c>
@@ -6483,7 +6510,7 @@
       <c r="Q58" s="117"/>
       <c r="R58" s="118"/>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" s="13" t="s">
         <v>189</v>
       </c>
@@ -6506,7 +6533,7 @@
       <c r="Q59" s="119"/>
       <c r="R59" s="120"/>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="13" t="s">
         <v>190</v>
       </c>
@@ -6527,7 +6554,7 @@
       <c r="Q60" s="14"/>
       <c r="R60" s="15"/>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="s">
         <v>192</v>
       </c>
@@ -6548,7 +6575,7 @@
       <c r="Q61" s="29"/>
       <c r="R61" s="30"/>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B62" s="20" t="s">
         <v>181</v>
       </c>
@@ -6571,11 +6598,11 @@
       <c r="Q62" s="21"/>
       <c r="R62" s="22"/>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="139" t="s">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B63" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="140"/>
+      <c r="C63" s="143"/>
       <c r="D63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6585,10 +6612,10 @@
       <c r="F63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H63" s="139" t="s">
+      <c r="H63" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="I63" s="140"/>
+      <c r="I63" s="143"/>
       <c r="J63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6598,10 +6625,10 @@
       <c r="L63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N63" s="139" t="s">
+      <c r="N63" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="O63" s="140"/>
+      <c r="O63" s="143"/>
       <c r="P63" s="42" t="s">
         <v>87</v>
       </c>
@@ -6612,7 +6639,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B64" s="93" t="s">
         <v>120</v>
       </c>
@@ -6653,7 +6680,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="87" t="s">
         <v>121</v>
       </c>
@@ -6694,7 +6721,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66" s="87" t="s">
         <v>122</v>
       </c>
@@ -6735,7 +6762,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" s="87" t="s">
         <v>194</v>
       </c>
@@ -6776,7 +6803,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="68" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" s="87" t="s">
         <v>193</v>
       </c>
@@ -6817,7 +6844,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="97" t="s">
         <v>195</v>
       </c>
@@ -6845,30 +6872,30 @@
         <v>45572</v>
       </c>
     </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B71" s="136" t="s">
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B71" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="137"/>
-      <c r="D71" s="137"/>
-      <c r="E71" s="137"/>
-      <c r="F71" s="138"/>
-      <c r="H71" s="136" t="s">
+      <c r="C71" s="145"/>
+      <c r="D71" s="145"/>
+      <c r="E71" s="145"/>
+      <c r="F71" s="146"/>
+      <c r="H71" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="I71" s="137"/>
-      <c r="J71" s="137"/>
-      <c r="K71" s="137"/>
-      <c r="L71" s="138"/>
-      <c r="N71" s="136" t="s">
+      <c r="I71" s="145"/>
+      <c r="J71" s="145"/>
+      <c r="K71" s="145"/>
+      <c r="L71" s="146"/>
+      <c r="N71" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="O71" s="137"/>
-      <c r="P71" s="137"/>
-      <c r="Q71" s="137"/>
-      <c r="R71" s="138"/>
-    </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O71" s="145"/>
+      <c r="P71" s="145"/>
+      <c r="Q71" s="145"/>
+      <c r="R71" s="146"/>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="s">
         <v>78</v>
       </c>
@@ -6897,7 +6924,7 @@
       <c r="Q72" s="68"/>
       <c r="R72" s="69"/>
     </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" s="13" t="s">
         <v>79</v>
       </c>
@@ -6926,7 +6953,7 @@
       <c r="Q73" s="14"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B74" s="10"/>
       <c r="C74" s="18"/>
       <c r="D74" s="18"/>
@@ -6943,7 +6970,7 @@
       <c r="Q74" s="18"/>
       <c r="R74" s="70"/>
     </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" s="20" t="s">
         <v>80</v>
       </c>
@@ -6966,7 +6993,7 @@
       <c r="Q75" s="21"/>
       <c r="R75" s="22"/>
     </row>
-    <row r="76" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B76" s="116" t="s">
         <v>228</v>
       </c>
@@ -6989,7 +7016,7 @@
       <c r="Q76" s="117"/>
       <c r="R76" s="118"/>
     </row>
-    <row r="77" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B77" s="115" t="s">
         <v>229</v>
       </c>
@@ -7012,7 +7039,7 @@
       <c r="Q77" s="119"/>
       <c r="R77" s="120"/>
     </row>
-    <row r="78" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B78" s="121" t="s">
         <v>230</v>
       </c>
@@ -7033,7 +7060,7 @@
       <c r="Q78" s="14"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B79" s="10"/>
       <c r="C79" s="29"/>
       <c r="D79" s="29"/>
@@ -7050,7 +7077,7 @@
       <c r="Q79" s="29"/>
       <c r="R79" s="30"/>
     </row>
-    <row r="80" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B80" s="20" t="s">
         <v>181</v>
       </c>
@@ -7073,11 +7100,11 @@
       <c r="Q80" s="21"/>
       <c r="R80" s="22"/>
     </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B81" s="139" t="s">
+    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B81" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="C81" s="140"/>
+      <c r="C81" s="143"/>
       <c r="D81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7087,10 +7114,10 @@
       <c r="F81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H81" s="139" t="s">
+      <c r="H81" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="I81" s="140"/>
+      <c r="I81" s="143"/>
       <c r="J81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7100,10 +7127,10 @@
       <c r="L81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N81" s="139" t="s">
+      <c r="N81" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="O81" s="140"/>
+      <c r="O81" s="143"/>
       <c r="P81" s="42" t="s">
         <v>87</v>
       </c>
@@ -7114,7 +7141,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B82" s="87" t="s">
         <v>121</v>
       </c>
@@ -7155,7 +7182,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B83" s="87" t="s">
         <v>122</v>
       </c>
@@ -7196,7 +7223,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B84" s="87" t="s">
         <v>194</v>
       </c>
@@ -7237,7 +7264,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B85" s="90" t="s">
         <v>193</v>
       </c>
@@ -7278,7 +7305,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H86" s="90" t="s">
         <v>246</v>
       </c>
@@ -7306,23 +7333,30 @@
         <v>45577</v>
       </c>
     </row>
-    <row r="88" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B88" s="136" t="s">
+    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B88" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="C88" s="137"/>
-      <c r="D88" s="137"/>
-      <c r="E88" s="137"/>
-      <c r="F88" s="138"/>
-      <c r="H88" s="136" t="s">
+      <c r="C88" s="145"/>
+      <c r="D88" s="145"/>
+      <c r="E88" s="145"/>
+      <c r="F88" s="146"/>
+      <c r="H88" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="I88" s="137"/>
-      <c r="J88" s="137"/>
-      <c r="K88" s="137"/>
-      <c r="L88" s="138"/>
-    </row>
-    <row r="89" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="I88" s="145"/>
+      <c r="J88" s="145"/>
+      <c r="K88" s="145"/>
+      <c r="L88" s="146"/>
+      <c r="N88" s="144" t="s">
+        <v>77</v>
+      </c>
+      <c r="O88" s="145"/>
+      <c r="P88" s="145"/>
+      <c r="Q88" s="145"/>
+      <c r="R88" s="146"/>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="s">
         <v>78</v>
       </c>
@@ -7341,8 +7375,17 @@
       <c r="J89" s="68"/>
       <c r="K89" s="68"/>
       <c r="L89" s="69"/>
-    </row>
-    <row r="90" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N89" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="O89" s="131">
+        <v>45579</v>
+      </c>
+      <c r="P89" s="68"/>
+      <c r="Q89" s="68"/>
+      <c r="R89" s="69"/>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B90" s="13" t="s">
         <v>79</v>
       </c>
@@ -7361,8 +7404,17 @@
       <c r="J90" s="14"/>
       <c r="K90" s="14"/>
       <c r="L90" s="15"/>
-    </row>
-    <row r="91" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N90" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="O90" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="P90" s="14"/>
+      <c r="Q90" s="14"/>
+      <c r="R90" s="15"/>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B91" s="10"/>
       <c r="C91" s="18"/>
       <c r="D91" s="18"/>
@@ -7373,8 +7425,13 @@
       <c r="J91" s="18"/>
       <c r="K91" s="18"/>
       <c r="L91" s="70"/>
-    </row>
-    <row r="92" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N91" s="10"/>
+      <c r="O91" s="132"/>
+      <c r="P91" s="132"/>
+      <c r="Q91" s="132"/>
+      <c r="R91" s="70"/>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B92" s="20" t="s">
         <v>80</v>
       </c>
@@ -7389,8 +7446,15 @@
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
       <c r="L92" s="22"/>
-    </row>
-    <row r="93" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N92" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O92" s="21"/>
+      <c r="P92" s="21"/>
+      <c r="Q92" s="21"/>
+      <c r="R92" s="22"/>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B93" s="116" t="s">
         <v>256</v>
       </c>
@@ -7405,8 +7469,15 @@
       <c r="J93" s="117"/>
       <c r="K93" s="117"/>
       <c r="L93" s="118"/>
-    </row>
-    <row r="94" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N93" s="116" t="s">
+        <v>261</v>
+      </c>
+      <c r="O93" s="117"/>
+      <c r="P93" s="117"/>
+      <c r="Q93" s="117"/>
+      <c r="R93" s="118"/>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B94" s="115" t="s">
         <v>257</v>
       </c>
@@ -7414,15 +7485,22 @@
       <c r="D94" s="119"/>
       <c r="E94" s="119"/>
       <c r="F94" s="120"/>
-      <c r="H94" s="151" t="s">
+      <c r="H94" s="133" t="s">
         <v>259</v>
       </c>
-      <c r="I94" s="152"/>
-      <c r="J94" s="152"/>
-      <c r="K94" s="152"/>
+      <c r="I94" s="134"/>
+      <c r="J94" s="134"/>
+      <c r="K94" s="134"/>
       <c r="L94" s="120"/>
-    </row>
-    <row r="95" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N94" s="133" t="s">
+        <v>262</v>
+      </c>
+      <c r="O94" s="134"/>
+      <c r="P94" s="134"/>
+      <c r="Q94" s="134"/>
+      <c r="R94" s="120"/>
+    </row>
+    <row r="95" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B95" s="121"/>
       <c r="C95" s="14"/>
       <c r="D95" s="14"/>
@@ -7433,8 +7511,15 @@
       <c r="J95" s="14"/>
       <c r="K95" s="14"/>
       <c r="L95" s="15"/>
-    </row>
-    <row r="96" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N95" s="121" t="s">
+        <v>264</v>
+      </c>
+      <c r="O95" s="14"/>
+      <c r="P95" s="14"/>
+      <c r="Q95" s="14"/>
+      <c r="R95" s="15"/>
+    </row>
+    <row r="96" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B96" s="10"/>
       <c r="C96" s="29"/>
       <c r="D96" s="29"/>
@@ -7445,8 +7530,13 @@
       <c r="J96" s="29"/>
       <c r="K96" s="29"/>
       <c r="L96" s="30"/>
-    </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N96" s="10"/>
+      <c r="O96" s="29"/>
+      <c r="P96" s="29"/>
+      <c r="Q96" s="29"/>
+      <c r="R96" s="30"/>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B97" s="20" t="s">
         <v>181</v>
       </c>
@@ -7461,12 +7551,19 @@
       <c r="J97" s="21"/>
       <c r="K97" s="21"/>
       <c r="L97" s="22"/>
-    </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B98" s="139" t="s">
+      <c r="N97" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="O97" s="21"/>
+      <c r="P97" s="21"/>
+      <c r="Q97" s="21"/>
+      <c r="R97" s="22"/>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B98" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="C98" s="140"/>
+      <c r="C98" s="143"/>
       <c r="D98" s="42" t="s">
         <v>87</v>
       </c>
@@ -7489,8 +7586,21 @@
       <c r="L98" s="24" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N98" s="129" t="s">
+        <v>86</v>
+      </c>
+      <c r="O98" s="130"/>
+      <c r="P98" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q98" s="130" t="s">
+        <v>113</v>
+      </c>
+      <c r="R98" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B99" s="127" t="s">
         <v>121</v>
       </c>
@@ -7517,8 +7627,21 @@
       <c r="L99" s="64">
         <v>45576</v>
       </c>
-    </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N99" s="87" t="s">
+        <v>263</v>
+      </c>
+      <c r="O99" s="47"/>
+      <c r="P99" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q99" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="R99" s="48">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B100" s="87" t="s">
         <v>122</v>
       </c>
@@ -7545,8 +7668,21 @@
       <c r="L100" s="48">
         <v>45610</v>
       </c>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N100" s="127" t="s">
+        <v>122</v>
+      </c>
+      <c r="O100" s="63"/>
+      <c r="P100" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q100" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="R100" s="64">
+        <v>45610</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B101" s="127" t="s">
         <v>194</v>
       </c>
@@ -7573,8 +7709,21 @@
       <c r="L101" s="64">
         <v>45576</v>
       </c>
-    </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N101" s="127" t="s">
+        <v>194</v>
+      </c>
+      <c r="O101" s="63"/>
+      <c r="P101" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q101" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="R101" s="64">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B102" s="127" t="s">
         <v>193</v>
       </c>
@@ -7601,8 +7750,21 @@
       <c r="L102" s="64">
         <v>45576</v>
       </c>
-    </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N102" s="127" t="s">
+        <v>193</v>
+      </c>
+      <c r="O102" s="63"/>
+      <c r="P102" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q102" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="R102" s="64">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B103" s="127" t="s">
         <v>246</v>
       </c>
@@ -7629,8 +7791,21 @@
       <c r="L103" s="64">
         <v>45577</v>
       </c>
-    </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N103" s="127" t="s">
+        <v>246</v>
+      </c>
+      <c r="O103" s="63"/>
+      <c r="P103" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q103" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="R103" s="64">
+        <v>45577</v>
+      </c>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B104" s="87" t="s">
         <v>253</v>
       </c>
@@ -7657,8 +7832,21 @@
       <c r="L104" s="64">
         <v>45578</v>
       </c>
-    </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N104" s="127" t="s">
+        <v>253</v>
+      </c>
+      <c r="O104" s="63"/>
+      <c r="P104" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q104" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="R104" s="64">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B105" s="97" t="s">
         <v>254</v>
       </c>
@@ -7685,18 +7873,62 @@
       <c r="L105" s="83">
         <v>45578</v>
       </c>
+      <c r="N105" s="81" t="s">
+        <v>254</v>
+      </c>
+      <c r="O105" s="82"/>
+      <c r="P105" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q105" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="R105" s="83">
+        <v>45578</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="H53:L53"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="I37:L37"/>
+  <mergeCells count="65">
+    <mergeCell ref="H88:L88"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="N71:R71"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="N88:R88"/>
+    <mergeCell ref="N53:R53"/>
+    <mergeCell ref="N63:O63"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="N35:R35"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
@@ -7713,45 +7945,15 @@
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="N53:R53"/>
-    <mergeCell ref="N63:O63"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="N35:R35"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="H88:L88"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="N71:R71"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="H71:L71"/>
-    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="H53:L53"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="I37:L37"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização das atas de reunião
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI_GraficoBurndown.xlsx
+++ b/Documentação/RequisitosPI_GraficoBurndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Gotardo\Desktop\Projeto Grupo\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E51446-12A1-463E-BD31-4C4782FDBEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3C7906-EF04-4023-B7E7-6FFCA925E99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="296">
   <si>
     <t>Requisito</t>
   </si>
@@ -1044,6 +1044,39 @@
   </si>
   <si>
     <t>Concluído</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Suporte e atendimento ao cliente</t>
+  </si>
+  <si>
+    <t>Integração da API com BD</t>
+  </si>
+  <si>
+    <t>Integração da API com DASH</t>
+  </si>
+  <si>
+    <t>Realizar modificações propostas pelo Cliente. Vamos definir uma página inicial das dashboards, para</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ter uma seleção dos tanques monitorados. Página de suporte e atendimento ao cliente, modificações </t>
+  </si>
+  <si>
+    <t xml:space="preserve">da modelagem, com novas tabelas. </t>
+  </si>
+  <si>
+    <t>Iniciar</t>
+  </si>
+  <si>
+    <t>Ajustes modelagem, de acordo com orientações da sprint 2</t>
+  </si>
+  <si>
+    <t>Ajustes diagrama e documentação</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1766,6 +1799,15 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1787,6 +1829,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1802,6 +1862,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1832,37 +1898,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3334,7 +3373,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3360,17 +3399,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="142" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="141"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
     </row>
     <row r="2" spans="1:20" s="126" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="120" t="s">
@@ -3430,20 +3469,20 @@
       <c r="I3" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="142" t="s">
+      <c r="K3" s="145" t="s">
         <v>216</v>
       </c>
-      <c r="L3" s="142"/>
+      <c r="L3" s="145"/>
       <c r="M3" s="118"/>
-      <c r="N3" s="142" t="s">
+      <c r="N3" s="145" t="s">
         <v>217</v>
       </c>
-      <c r="O3" s="142"/>
+      <c r="O3" s="145"/>
       <c r="P3" s="118"/>
-      <c r="Q3" s="142" t="s">
+      <c r="Q3" s="145" t="s">
         <v>231</v>
       </c>
-      <c r="R3" s="142"/>
+      <c r="R3" s="145"/>
       <c r="T3" s="118">
         <v>88</v>
       </c>
@@ -3492,10 +3531,10 @@
         <v>207</v>
       </c>
       <c r="P4" s="118"/>
-      <c r="Q4" s="137" t="s">
+      <c r="Q4" s="140" t="s">
         <v>232</v>
       </c>
-      <c r="R4" s="138"/>
+      <c r="R4" s="141"/>
       <c r="T4" s="118">
         <v>119</v>
       </c>
@@ -3543,10 +3582,10 @@
         <v>88</v>
       </c>
       <c r="P5" s="118"/>
-      <c r="Q5" s="137" t="s">
+      <c r="Q5" s="140" t="s">
         <v>233</v>
       </c>
-      <c r="R5" s="138"/>
+      <c r="R5" s="141"/>
       <c r="T5" s="118">
         <v>139</v>
       </c>
@@ -3594,10 +3633,10 @@
         <v>119</v>
       </c>
       <c r="P6" s="118"/>
-      <c r="Q6" s="137" t="s">
+      <c r="Q6" s="140" t="s">
         <v>234</v>
       </c>
-      <c r="R6" s="138"/>
+      <c r="R6" s="141"/>
       <c r="T6" s="118">
         <v>0</v>
       </c>
@@ -3645,10 +3684,10 @@
         <v>0</v>
       </c>
       <c r="P7" s="118"/>
-      <c r="Q7" s="137" t="s">
+      <c r="Q7" s="140" t="s">
         <v>235</v>
       </c>
-      <c r="R7" s="138"/>
+      <c r="R7" s="141"/>
     </row>
     <row r="8" spans="1:20" s="128" customFormat="1" ht="34.950000000000003" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="134" t="s">
@@ -3692,10 +3731,10 @@
         <v>0</v>
       </c>
       <c r="P8" s="118"/>
-      <c r="Q8" s="137" t="s">
+      <c r="Q8" s="140" t="s">
         <v>236</v>
       </c>
-      <c r="R8" s="138"/>
+      <c r="R8" s="141"/>
     </row>
     <row r="9" spans="1:20" s="128" customFormat="1" ht="34.950000000000003" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="134" t="s">
@@ -6752,7 +6791,7 @@
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="143" t="s">
+      <c r="G1" s="146" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6775,7 +6814,7 @@
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="143"/>
+      <c r="G2" s="146"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -7126,10 +7165,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
-  <dimension ref="B1:R142"/>
+  <dimension ref="B1:R160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I141" sqref="I141"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7156,88 +7195,88 @@
   <sheetData>
     <row r="1" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="146"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="155"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="144" t="s">
+      <c r="H2" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="145"/>
-      <c r="J2" s="145"/>
-      <c r="K2" s="145"/>
-      <c r="L2" s="146"/>
-      <c r="N2" s="144" t="s">
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="155"/>
+      <c r="N2" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="145"/>
-      <c r="P2" s="145"/>
-      <c r="Q2" s="145"/>
-      <c r="R2" s="146"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="155"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="151">
+      <c r="C3" s="162">
         <v>45554</v>
       </c>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="152"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="163"/>
       <c r="G3" s="5"/>
       <c r="H3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="151">
+      <c r="I3" s="162">
         <v>45555</v>
       </c>
-      <c r="J3" s="151"/>
-      <c r="K3" s="151"/>
-      <c r="L3" s="152"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="163"/>
       <c r="N3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="151">
+      <c r="O3" s="162">
         <v>45557</v>
       </c>
-      <c r="P3" s="151"/>
-      <c r="Q3" s="151"/>
-      <c r="R3" s="152"/>
+      <c r="P3" s="162"/>
+      <c r="Q3" s="162"/>
+      <c r="R3" s="163"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="168" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
-      <c r="F4" s="158"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="169"/>
       <c r="G4" s="6"/>
       <c r="H4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="157" t="s">
+      <c r="I4" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="157"/>
-      <c r="K4" s="157"/>
-      <c r="L4" s="158"/>
+      <c r="J4" s="168"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="169"/>
       <c r="N4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="157" t="s">
+      <c r="O4" s="168" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="157"/>
-      <c r="Q4" s="157"/>
-      <c r="R4" s="158"/>
+      <c r="P4" s="168"/>
+      <c r="Q4" s="168"/>
+      <c r="R4" s="169"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
@@ -7368,22 +7407,22 @@
       <c r="R10" s="22"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="147" t="s">
+      <c r="B11" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="148"/>
-      <c r="D11" s="148" t="s">
+      <c r="C11" s="157"/>
+      <c r="D11" s="157" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="148"/>
+      <c r="E11" s="157"/>
       <c r="F11" s="24" t="s">
         <v>88</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="147" t="s">
+      <c r="H11" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="148"/>
+      <c r="I11" s="157"/>
       <c r="J11" s="26" t="s">
         <v>87</v>
       </c>
@@ -7391,10 +7430,10 @@
       <c r="L11" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="N11" s="147" t="s">
+      <c r="N11" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="O11" s="148"/>
+      <c r="O11" s="157"/>
       <c r="P11" s="42" t="s">
         <v>87</v>
       </c>
@@ -7406,22 +7445,22 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="156" t="s">
+      <c r="B12" s="167" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="155"/>
-      <c r="D12" s="155" t="s">
+      <c r="C12" s="166"/>
+      <c r="D12" s="166" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="155"/>
+      <c r="E12" s="166"/>
       <c r="F12" s="16">
         <v>45560</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="156"/>
-      <c r="I12" s="155"/>
-      <c r="J12" s="155"/>
-      <c r="K12" s="155"/>
+      <c r="H12" s="167"/>
+      <c r="I12" s="166"/>
+      <c r="J12" s="166"/>
+      <c r="K12" s="166"/>
       <c r="L12" s="16"/>
       <c r="N12" s="49" t="s">
         <v>89</v>
@@ -7438,22 +7477,22 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="167" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="155" t="s">
+      <c r="C13" s="166"/>
+      <c r="D13" s="166" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="155"/>
+      <c r="E13" s="166"/>
       <c r="F13" s="16">
         <v>45560</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="156"/>
-      <c r="I13" s="155"/>
-      <c r="J13" s="155"/>
-      <c r="K13" s="155"/>
+      <c r="H13" s="167"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="16"/>
       <c r="N13" s="45" t="s">
         <v>90</v>
@@ -7470,22 +7509,22 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="167" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="155" t="s">
+      <c r="C14" s="166"/>
+      <c r="D14" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="155"/>
+      <c r="E14" s="166"/>
       <c r="F14" s="16">
         <v>45560</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="156"/>
-      <c r="I14" s="155"/>
-      <c r="J14" s="155"/>
-      <c r="K14" s="155"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="16"/>
       <c r="N14" s="45" t="s">
         <v>91</v>
@@ -7502,21 +7541,21 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="149" t="s">
+      <c r="B15" s="160" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="150"/>
-      <c r="D15" s="150" t="s">
+      <c r="C15" s="161"/>
+      <c r="D15" s="161" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="150"/>
+      <c r="E15" s="161"/>
       <c r="F15" s="19">
         <v>45560</v>
       </c>
-      <c r="H15" s="149"/>
-      <c r="I15" s="150"/>
-      <c r="J15" s="150"/>
-      <c r="K15" s="150"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="161"/>
+      <c r="J15" s="161"/>
+      <c r="K15" s="161"/>
       <c r="L15" s="19"/>
       <c r="N15" s="84" t="s">
         <v>93</v>
@@ -7545,85 +7584,85 @@
       <c r="R16" s="67"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="144" t="s">
+      <c r="B17" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="145"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="146"/>
-      <c r="H17" s="144" t="s">
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
+      <c r="E17" s="154"/>
+      <c r="F17" s="155"/>
+      <c r="H17" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="145"/>
-      <c r="J17" s="145"/>
-      <c r="K17" s="145"/>
-      <c r="L17" s="146"/>
-      <c r="N17" s="144" t="s">
+      <c r="I17" s="154"/>
+      <c r="J17" s="154"/>
+      <c r="K17" s="154"/>
+      <c r="L17" s="155"/>
+      <c r="N17" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O17" s="145"/>
-      <c r="P17" s="145"/>
-      <c r="Q17" s="145"/>
-      <c r="R17" s="146"/>
+      <c r="O17" s="154"/>
+      <c r="P17" s="154"/>
+      <c r="Q17" s="154"/>
+      <c r="R17" s="155"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="151">
+      <c r="C18" s="162">
         <v>45558</v>
       </c>
-      <c r="D18" s="151"/>
-      <c r="E18" s="151"/>
-      <c r="F18" s="152"/>
+      <c r="D18" s="162"/>
+      <c r="E18" s="162"/>
+      <c r="F18" s="163"/>
       <c r="H18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="151">
+      <c r="I18" s="162">
         <v>45559</v>
       </c>
-      <c r="J18" s="151"/>
-      <c r="K18" s="151"/>
-      <c r="L18" s="152"/>
+      <c r="J18" s="162"/>
+      <c r="K18" s="162"/>
+      <c r="L18" s="163"/>
       <c r="N18" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="O18" s="151">
+      <c r="O18" s="162">
         <v>45560</v>
       </c>
-      <c r="P18" s="151"/>
-      <c r="Q18" s="151"/>
-      <c r="R18" s="152"/>
+      <c r="P18" s="162"/>
+      <c r="Q18" s="162"/>
+      <c r="R18" s="163"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="153" t="s">
+      <c r="C19" s="164" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="153"/>
-      <c r="E19" s="153"/>
-      <c r="F19" s="154"/>
+      <c r="D19" s="164"/>
+      <c r="E19" s="164"/>
+      <c r="F19" s="165"/>
       <c r="H19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="153" t="s">
+      <c r="I19" s="164" t="s">
         <v>116</v>
       </c>
-      <c r="J19" s="153"/>
-      <c r="K19" s="153"/>
-      <c r="L19" s="154"/>
+      <c r="J19" s="164"/>
+      <c r="K19" s="164"/>
+      <c r="L19" s="165"/>
       <c r="N19" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="O19" s="153" t="s">
+      <c r="O19" s="164" t="s">
         <v>81</v>
       </c>
-      <c r="P19" s="153"/>
-      <c r="Q19" s="153"/>
-      <c r="R19" s="154"/>
+      <c r="P19" s="164"/>
+      <c r="Q19" s="164"/>
+      <c r="R19" s="165"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
@@ -7773,10 +7812,10 @@
       <c r="R26" s="22"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="147" t="s">
+      <c r="B27" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="148"/>
+      <c r="C27" s="157"/>
       <c r="D27" s="42" t="s">
         <v>87</v>
       </c>
@@ -7786,10 +7825,10 @@
       <c r="F27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="147" t="s">
+      <c r="H27" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="148"/>
+      <c r="I27" s="157"/>
       <c r="J27" s="42" t="s">
         <v>87</v>
       </c>
@@ -7799,10 +7838,10 @@
       <c r="L27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N27" s="147" t="s">
+      <c r="N27" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="O27" s="148"/>
+      <c r="O27" s="157"/>
       <c r="P27" s="42" t="s">
         <v>87</v>
       </c>
@@ -8003,27 +8042,27 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="144" t="s">
+      <c r="B35" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="145"/>
-      <c r="D35" s="145"/>
-      <c r="E35" s="145"/>
-      <c r="F35" s="146"/>
-      <c r="H35" s="144" t="s">
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="155"/>
+      <c r="H35" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I35" s="145"/>
-      <c r="J35" s="145"/>
-      <c r="K35" s="145"/>
-      <c r="L35" s="146"/>
-      <c r="N35" s="144" t="s">
+      <c r="I35" s="154"/>
+      <c r="J35" s="154"/>
+      <c r="K35" s="154"/>
+      <c r="L35" s="155"/>
+      <c r="N35" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O35" s="145"/>
-      <c r="P35" s="145"/>
-      <c r="Q35" s="145"/>
-      <c r="R35" s="146"/>
+      <c r="O35" s="154"/>
+      <c r="P35" s="154"/>
+      <c r="Q35" s="154"/>
+      <c r="R35" s="155"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
@@ -8038,12 +8077,12 @@
       <c r="H36" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="151">
+      <c r="I36" s="162">
         <v>45562</v>
       </c>
-      <c r="J36" s="151"/>
-      <c r="K36" s="151"/>
-      <c r="L36" s="152"/>
+      <c r="J36" s="162"/>
+      <c r="K36" s="162"/>
+      <c r="L36" s="163"/>
       <c r="N36" s="75" t="s">
         <v>78</v>
       </c>
@@ -8067,12 +8106,12 @@
       <c r="H37" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I37" s="153" t="s">
+      <c r="I37" s="164" t="s">
         <v>183</v>
       </c>
-      <c r="J37" s="153"/>
-      <c r="K37" s="153"/>
-      <c r="L37" s="154"/>
+      <c r="J37" s="164"/>
+      <c r="K37" s="164"/>
+      <c r="L37" s="165"/>
       <c r="N37" s="78" t="s">
         <v>79</v>
       </c>
@@ -8227,10 +8266,10 @@
       <c r="R44" s="22"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="147" t="s">
+      <c r="B45" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="148"/>
+      <c r="C45" s="157"/>
       <c r="D45" s="42" t="s">
         <v>87</v>
       </c>
@@ -8240,10 +8279,10 @@
       <c r="F45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="147" t="s">
+      <c r="H45" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="148"/>
+      <c r="I45" s="157"/>
       <c r="J45" s="42" t="s">
         <v>87</v>
       </c>
@@ -8253,10 +8292,10 @@
       <c r="L45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="147" t="s">
+      <c r="N45" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="O45" s="148"/>
+      <c r="O45" s="157"/>
       <c r="P45" s="42" t="s">
         <v>87</v>
       </c>
@@ -8473,27 +8512,27 @@
       </c>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B53" s="144" t="s">
+      <c r="B53" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="145"/>
-      <c r="D53" s="145"/>
-      <c r="E53" s="145"/>
-      <c r="F53" s="146"/>
-      <c r="H53" s="144" t="s">
+      <c r="C53" s="154"/>
+      <c r="D53" s="154"/>
+      <c r="E53" s="154"/>
+      <c r="F53" s="155"/>
+      <c r="H53" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I53" s="145"/>
-      <c r="J53" s="145"/>
-      <c r="K53" s="145"/>
-      <c r="L53" s="146"/>
-      <c r="N53" s="144" t="s">
+      <c r="I53" s="154"/>
+      <c r="J53" s="154"/>
+      <c r="K53" s="154"/>
+      <c r="L53" s="155"/>
+      <c r="N53" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O53" s="145"/>
-      <c r="P53" s="145"/>
-      <c r="Q53" s="145"/>
-      <c r="R53" s="146"/>
+      <c r="O53" s="154"/>
+      <c r="P53" s="154"/>
+      <c r="Q53" s="154"/>
+      <c r="R53" s="155"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="s">
@@ -8705,10 +8744,10 @@
       <c r="R62" s="22"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="147" t="s">
+      <c r="B63" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="148"/>
+      <c r="C63" s="157"/>
       <c r="D63" s="42" t="s">
         <v>87</v>
       </c>
@@ -8718,10 +8757,10 @@
       <c r="F63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H63" s="147" t="s">
+      <c r="H63" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="I63" s="148"/>
+      <c r="I63" s="157"/>
       <c r="J63" s="42" t="s">
         <v>87</v>
       </c>
@@ -8731,10 +8770,10 @@
       <c r="L63" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N63" s="147" t="s">
+      <c r="N63" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="O63" s="148"/>
+      <c r="O63" s="157"/>
       <c r="P63" s="42" t="s">
         <v>87</v>
       </c>
@@ -8979,27 +9018,27 @@
       </c>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B71" s="144" t="s">
+      <c r="B71" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="145"/>
-      <c r="D71" s="145"/>
-      <c r="E71" s="145"/>
-      <c r="F71" s="146"/>
-      <c r="H71" s="144" t="s">
+      <c r="C71" s="154"/>
+      <c r="D71" s="154"/>
+      <c r="E71" s="154"/>
+      <c r="F71" s="155"/>
+      <c r="H71" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I71" s="145"/>
-      <c r="J71" s="145"/>
-      <c r="K71" s="145"/>
-      <c r="L71" s="146"/>
-      <c r="N71" s="144" t="s">
+      <c r="I71" s="154"/>
+      <c r="J71" s="154"/>
+      <c r="K71" s="154"/>
+      <c r="L71" s="155"/>
+      <c r="N71" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O71" s="145"/>
-      <c r="P71" s="145"/>
-      <c r="Q71" s="145"/>
-      <c r="R71" s="146"/>
+      <c r="O71" s="154"/>
+      <c r="P71" s="154"/>
+      <c r="Q71" s="154"/>
+      <c r="R71" s="155"/>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B72" s="8" t="s">
@@ -9207,10 +9246,10 @@
       <c r="R80" s="22"/>
     </row>
     <row r="81" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B81" s="147" t="s">
+      <c r="B81" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="C81" s="148"/>
+      <c r="C81" s="157"/>
       <c r="D81" s="42" t="s">
         <v>87</v>
       </c>
@@ -9220,10 +9259,10 @@
       <c r="F81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H81" s="147" t="s">
+      <c r="H81" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="I81" s="148"/>
+      <c r="I81" s="157"/>
       <c r="J81" s="42" t="s">
         <v>87</v>
       </c>
@@ -9233,10 +9272,10 @@
       <c r="L81" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N81" s="147" t="s">
+      <c r="N81" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="O81" s="148"/>
+      <c r="O81" s="157"/>
       <c r="P81" s="42" t="s">
         <v>87</v>
       </c>
@@ -9440,27 +9479,27 @@
       </c>
     </row>
     <row r="88" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B88" s="144" t="s">
+      <c r="B88" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C88" s="145"/>
-      <c r="D88" s="145"/>
-      <c r="E88" s="145"/>
-      <c r="F88" s="146"/>
-      <c r="H88" s="144" t="s">
+      <c r="C88" s="154"/>
+      <c r="D88" s="154"/>
+      <c r="E88" s="154"/>
+      <c r="F88" s="155"/>
+      <c r="H88" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I88" s="145"/>
-      <c r="J88" s="145"/>
-      <c r="K88" s="145"/>
-      <c r="L88" s="146"/>
-      <c r="N88" s="144" t="s">
+      <c r="I88" s="154"/>
+      <c r="J88" s="154"/>
+      <c r="K88" s="154"/>
+      <c r="L88" s="155"/>
+      <c r="N88" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O88" s="145"/>
-      <c r="P88" s="145"/>
-      <c r="Q88" s="145"/>
-      <c r="R88" s="146"/>
+      <c r="O88" s="154"/>
+      <c r="P88" s="154"/>
+      <c r="Q88" s="154"/>
+      <c r="R88" s="155"/>
     </row>
     <row r="89" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B89" s="8" t="s">
@@ -9666,10 +9705,10 @@
       <c r="R97" s="22"/>
     </row>
     <row r="98" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B98" s="147" t="s">
+      <c r="B98" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="C98" s="148"/>
+      <c r="C98" s="157"/>
       <c r="D98" s="42" t="s">
         <v>87</v>
       </c>
@@ -9994,27 +10033,27 @@
       </c>
     </row>
     <row r="107" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B107" s="144" t="s">
+      <c r="B107" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C107" s="145"/>
-      <c r="D107" s="145"/>
-      <c r="E107" s="145"/>
-      <c r="F107" s="146"/>
-      <c r="H107" s="144" t="s">
+      <c r="C107" s="154"/>
+      <c r="D107" s="154"/>
+      <c r="E107" s="154"/>
+      <c r="F107" s="155"/>
+      <c r="H107" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I107" s="145"/>
-      <c r="J107" s="145"/>
-      <c r="K107" s="145"/>
-      <c r="L107" s="146"/>
-      <c r="N107" s="144" t="s">
+      <c r="I107" s="154"/>
+      <c r="J107" s="154"/>
+      <c r="K107" s="154"/>
+      <c r="L107" s="155"/>
+      <c r="N107" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O107" s="145"/>
-      <c r="P107" s="145"/>
-      <c r="Q107" s="145"/>
-      <c r="R107" s="146"/>
+      <c r="O107" s="154"/>
+      <c r="P107" s="154"/>
+      <c r="Q107" s="154"/>
+      <c r="R107" s="155"/>
     </row>
     <row r="108" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B108" s="8" t="s">
@@ -10454,27 +10493,27 @@
       <c r="R124" s="83"/>
     </row>
     <row r="126" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B126" s="144" t="s">
+      <c r="B126" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="C126" s="145"/>
-      <c r="D126" s="145"/>
-      <c r="E126" s="145"/>
-      <c r="F126" s="146"/>
-      <c r="H126" s="144" t="s">
+      <c r="C126" s="154"/>
+      <c r="D126" s="154"/>
+      <c r="E126" s="154"/>
+      <c r="F126" s="155"/>
+      <c r="H126" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="I126" s="145"/>
-      <c r="J126" s="145"/>
-      <c r="K126" s="145"/>
-      <c r="L126" s="146"/>
-      <c r="N126" s="144" t="s">
+      <c r="I126" s="154"/>
+      <c r="J126" s="154"/>
+      <c r="K126" s="154"/>
+      <c r="L126" s="155"/>
+      <c r="N126" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="O126" s="145"/>
-      <c r="P126" s="145"/>
-      <c r="Q126" s="145"/>
-      <c r="R126" s="146"/>
+      <c r="O126" s="154"/>
+      <c r="P126" s="154"/>
+      <c r="Q126" s="154"/>
+      <c r="R126" s="155"/>
     </row>
     <row r="127" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B127" s="8" t="s">
@@ -10499,7 +10538,7 @@
         <v>78</v>
       </c>
       <c r="O127" s="9">
-        <v>45599</v>
+        <v>45600</v>
       </c>
       <c r="P127" s="68"/>
       <c r="Q127" s="68"/>
@@ -10572,7 +10611,9 @@
       <c r="J130" s="107"/>
       <c r="K130" s="107"/>
       <c r="L130" s="108"/>
-      <c r="N130" s="106"/>
+      <c r="N130" s="106" t="s">
+        <v>290</v>
+      </c>
       <c r="O130" s="107"/>
       <c r="P130" s="107"/>
       <c r="Q130" s="107"/>
@@ -10589,7 +10630,9 @@
       <c r="J131" s="109"/>
       <c r="K131" s="109"/>
       <c r="L131" s="110"/>
-      <c r="N131" s="116"/>
+      <c r="N131" s="116" t="s">
+        <v>291</v>
+      </c>
       <c r="O131" s="109"/>
       <c r="P131" s="109"/>
       <c r="Q131" s="109"/>
@@ -10606,7 +10649,9 @@
       <c r="J132" s="14"/>
       <c r="K132" s="14"/>
       <c r="L132" s="15"/>
-      <c r="N132" s="111"/>
+      <c r="N132" s="111" t="s">
+        <v>292</v>
+      </c>
       <c r="O132" s="14"/>
       <c r="P132" s="14"/>
       <c r="Q132" s="14"/>
@@ -10679,10 +10724,10 @@
       <c r="L135" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="N135" s="147" t="s">
+      <c r="N135" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="O135" s="148"/>
+      <c r="O135" s="157"/>
       <c r="P135" s="23" t="s">
         <v>87</v>
       </c>
@@ -10707,24 +10752,32 @@
       <c r="F136" s="48">
         <v>45585</v>
       </c>
-      <c r="H136" s="159" t="s">
+      <c r="H136" s="137" t="s">
         <v>279</v>
       </c>
-      <c r="I136" s="160"/>
-      <c r="J136" s="160" t="s">
+      <c r="I136" s="138"/>
+      <c r="J136" s="138" t="s">
         <v>94</v>
       </c>
-      <c r="K136" s="160" t="s">
+      <c r="K136" s="138" t="s">
         <v>284</v>
       </c>
-      <c r="L136" s="161">
+      <c r="L136" s="139">
         <v>45595</v>
       </c>
-      <c r="N136" s="168"/>
-      <c r="O136" s="169"/>
-      <c r="P136" s="160"/>
-      <c r="Q136" s="160"/>
-      <c r="R136" s="161"/>
+      <c r="N136" s="158" t="s">
+        <v>285</v>
+      </c>
+      <c r="O136" s="159"/>
+      <c r="P136" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q136" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="R136" s="52">
+        <v>45574</v>
+      </c>
     </row>
     <row r="137" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B137" s="87" t="s">
@@ -10740,24 +10793,32 @@
       <c r="F137" s="48">
         <v>45616</v>
       </c>
-      <c r="H137" s="159" t="s">
+      <c r="H137" s="137" t="s">
         <v>280</v>
       </c>
-      <c r="I137" s="160"/>
-      <c r="J137" s="160" t="s">
+      <c r="I137" s="138"/>
+      <c r="J137" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="K137" s="160" t="s">
+      <c r="K137" s="138" t="s">
         <v>284</v>
       </c>
-      <c r="L137" s="161">
+      <c r="L137" s="139">
         <v>45595</v>
       </c>
-      <c r="N137" s="166"/>
-      <c r="O137" s="167"/>
-      <c r="P137" s="160"/>
-      <c r="Q137" s="160"/>
-      <c r="R137" s="161"/>
+      <c r="N137" s="147" t="s">
+        <v>286</v>
+      </c>
+      <c r="O137" s="148"/>
+      <c r="P137" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q137" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="R137" s="52">
+        <v>45574</v>
+      </c>
     </row>
     <row r="138" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B138" s="114" t="s">
@@ -10773,24 +10834,32 @@
       <c r="F138" s="64">
         <v>45584</v>
       </c>
-      <c r="H138" s="159" t="s">
+      <c r="H138" s="137" t="s">
         <v>281</v>
       </c>
-      <c r="I138" s="160"/>
-      <c r="J138" s="160" t="s">
+      <c r="I138" s="138"/>
+      <c r="J138" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="K138" s="160" t="s">
+      <c r="K138" s="138" t="s">
         <v>284</v>
       </c>
-      <c r="L138" s="161">
+      <c r="L138" s="139">
         <v>45595</v>
       </c>
-      <c r="N138" s="166"/>
-      <c r="O138" s="167"/>
-      <c r="P138" s="160"/>
-      <c r="Q138" s="160"/>
-      <c r="R138" s="161"/>
+      <c r="N138" s="147" t="s">
+        <v>287</v>
+      </c>
+      <c r="O138" s="148"/>
+      <c r="P138" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q138" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="R138" s="52">
+        <v>45574</v>
+      </c>
     </row>
     <row r="139" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B139" s="87" t="s">
@@ -10806,24 +10875,32 @@
       <c r="F139" s="48">
         <v>45585</v>
       </c>
-      <c r="H139" s="159" t="s">
+      <c r="H139" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="I139" s="160"/>
-      <c r="J139" s="160" t="s">
+      <c r="I139" s="138"/>
+      <c r="J139" s="138" t="s">
         <v>124</v>
       </c>
-      <c r="K139" s="160" t="s">
+      <c r="K139" s="138" t="s">
         <v>284</v>
       </c>
-      <c r="L139" s="161">
+      <c r="L139" s="139">
         <v>45595</v>
       </c>
-      <c r="N139" s="166"/>
-      <c r="O139" s="167"/>
-      <c r="P139" s="160"/>
-      <c r="Q139" s="160"/>
-      <c r="R139" s="161"/>
+      <c r="N139" s="147" t="s">
+        <v>288</v>
+      </c>
+      <c r="O139" s="148"/>
+      <c r="P139" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q139" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="R139" s="52">
+        <v>45574</v>
+      </c>
     </row>
     <row r="140" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B140" s="87"/>
@@ -10831,24 +10908,32 @@
       <c r="D140" s="47"/>
       <c r="E140" s="47"/>
       <c r="F140" s="48"/>
-      <c r="H140" s="159" t="s">
+      <c r="H140" s="137" t="s">
         <v>283</v>
       </c>
-      <c r="I140" s="160"/>
-      <c r="J140" s="160" t="s">
+      <c r="I140" s="138"/>
+      <c r="J140" s="138" t="s">
         <v>115</v>
       </c>
-      <c r="K140" s="160" t="s">
+      <c r="K140" s="138" t="s">
         <v>284</v>
       </c>
-      <c r="L140" s="161">
+      <c r="L140" s="139">
         <v>45595</v>
       </c>
-      <c r="N140" s="166"/>
-      <c r="O140" s="167"/>
-      <c r="P140" s="160"/>
-      <c r="Q140" s="160"/>
-      <c r="R140" s="161"/>
+      <c r="N140" s="147" t="s">
+        <v>289</v>
+      </c>
+      <c r="O140" s="148"/>
+      <c r="P140" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q140" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="R140" s="52">
+        <v>45574</v>
+      </c>
     </row>
     <row r="141" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B141" s="114"/>
@@ -10861,8 +10946,8 @@
       <c r="J141" s="63"/>
       <c r="K141" s="63"/>
       <c r="L141" s="64"/>
-      <c r="N141" s="164"/>
-      <c r="O141" s="165"/>
+      <c r="N141" s="149"/>
+      <c r="O141" s="150"/>
       <c r="P141" s="63"/>
       <c r="Q141" s="63"/>
       <c r="R141" s="64"/>
@@ -10878,14 +10963,199 @@
       <c r="J142" s="82"/>
       <c r="K142" s="82"/>
       <c r="L142" s="83"/>
-      <c r="N142" s="162"/>
-      <c r="O142" s="163"/>
+      <c r="N142" s="151"/>
+      <c r="O142" s="152"/>
       <c r="P142" s="82"/>
       <c r="Q142" s="82"/>
       <c r="R142" s="83"/>
     </row>
+    <row r="144" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B144" s="153" t="s">
+        <v>77</v>
+      </c>
+      <c r="C144" s="154"/>
+      <c r="D144" s="154"/>
+      <c r="E144" s="154"/>
+      <c r="F144" s="155"/>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B145" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C145" s="9">
+        <v>45601</v>
+      </c>
+      <c r="D145" s="68"/>
+      <c r="E145" s="68"/>
+      <c r="F145" s="69"/>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B146" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C146" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D146" s="14"/>
+      <c r="E146" s="14"/>
+      <c r="F146" s="15"/>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B147" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C147" s="21"/>
+      <c r="D147" s="21"/>
+      <c r="E147" s="21"/>
+      <c r="F147" s="22"/>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B148" s="106" t="s">
+        <v>294</v>
+      </c>
+      <c r="C148" s="107"/>
+      <c r="D148" s="107"/>
+      <c r="E148" s="107"/>
+      <c r="F148" s="108"/>
+    </row>
+    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B149" s="116" t="s">
+        <v>295</v>
+      </c>
+      <c r="C149" s="109"/>
+      <c r="D149" s="109"/>
+      <c r="E149" s="109"/>
+      <c r="F149" s="110"/>
+    </row>
+    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B150" s="111"/>
+      <c r="C150" s="14"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="14"/>
+      <c r="F150" s="15"/>
+    </row>
+    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B151" s="10"/>
+      <c r="C151" s="29"/>
+      <c r="D151" s="29"/>
+      <c r="E151" s="29"/>
+      <c r="F151" s="30"/>
+    </row>
+    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B152" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C152" s="21"/>
+      <c r="D152" s="21"/>
+      <c r="E152" s="21"/>
+      <c r="F152" s="22"/>
+    </row>
+    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B153" s="156" t="s">
+        <v>86</v>
+      </c>
+      <c r="C153" s="157"/>
+      <c r="D153" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E153" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F153" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B154" s="158" t="s">
+        <v>285</v>
+      </c>
+      <c r="C154" s="159"/>
+      <c r="D154" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E154" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="F154" s="52">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B155" s="170" t="s">
+        <v>286</v>
+      </c>
+      <c r="C155" s="171"/>
+      <c r="D155" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="E155" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="F155" s="48">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B156" s="147" t="s">
+        <v>287</v>
+      </c>
+      <c r="C156" s="148"/>
+      <c r="D156" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="E156" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="F156" s="52">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B157" s="147" t="s">
+        <v>295</v>
+      </c>
+      <c r="C157" s="148"/>
+      <c r="D157" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="E157" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="F157" s="52">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="158" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B158" s="147" t="s">
+        <v>289</v>
+      </c>
+      <c r="C158" s="148"/>
+      <c r="D158" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E158" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="F158" s="52">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B159" s="149"/>
+      <c r="C159" s="150"/>
+      <c r="D159" s="63"/>
+      <c r="E159" s="63"/>
+      <c r="F159" s="64"/>
+    </row>
+    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B160" s="151"/>
+      <c r="C160" s="152"/>
+      <c r="D160" s="82"/>
+      <c r="E160" s="82"/>
+      <c r="F160" s="83"/>
+    </row>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="88">
     <mergeCell ref="N135:O135"/>
     <mergeCell ref="N142:O142"/>
     <mergeCell ref="N141:O141"/>
@@ -10965,6 +11235,15 @@
     <mergeCell ref="N88:R88"/>
     <mergeCell ref="H126:L126"/>
     <mergeCell ref="N126:R126"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>